<commit_message>
[Pipette] JTAG PCB 설계
</commit_message>
<xml_diff>
--- a/Femto Project schedule V1.0.xlsx
+++ b/Femto Project schedule V1.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="20180207" sheetId="18" r:id="rId1"/>
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="138">
   <si>
     <t>◇PCB설계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -772,10 +772,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>▶아르곤 게스 입고</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -805,10 +801,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>◇ Main PCB 2D,BOM,datasheet 전달</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>◇ Transformer PCB 2D,BOM,datasheet 전달</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -825,6 +817,29 @@
     <t>Pipette Proto-type test
  - Frequency 조정,
  - Gas 압력 조정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pipette JTAG PCB 설계</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pipette JTAG PCB 설계
+교수님 Transformer Test
+Femto에 Pipette proto type sample 준비 및 전달
+Femto에 Pipette proto type sample 준비</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>◇ Main PCB 2D,BOM,datasheet 전달</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>◇ BATT Con datasheet 전달</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>▶아르곤 가스 입고</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1617,7 +1632,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="207">
+  <cellXfs count="208">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1935,6 +1950,7 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -8505,14 +8521,14 @@
     <xdr:from>
       <xdr:col>113</xdr:col>
       <xdr:colOff>6723</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>170332</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>69474</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>133</xdr:col>
       <xdr:colOff>112058</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>78442</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>134467</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8521,8 +8537,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5475194" y="1862420"/>
-          <a:ext cx="4139452" cy="423581"/>
+          <a:off x="23628723" y="1402974"/>
+          <a:ext cx="4139453" cy="423581"/>
         </a:xfrm>
         <a:prstGeom prst="leftRightArrow">
           <a:avLst/>
@@ -35304,6 +35320,11 @@
     <row r="71" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="GA6:HE6"/>
+    <mergeCell ref="HF6:IJ6"/>
+    <mergeCell ref="IK6:JN6"/>
+    <mergeCell ref="JO6:KS6"/>
+    <mergeCell ref="KT6:LW6"/>
     <mergeCell ref="LX6:NB6"/>
     <mergeCell ref="A50:A54"/>
     <mergeCell ref="A15:A19"/>
@@ -35320,11 +35341,6 @@
     <mergeCell ref="BI6:CM6"/>
     <mergeCell ref="CN6:DQ6"/>
     <mergeCell ref="DR6:EV6"/>
-    <mergeCell ref="GA6:HE6"/>
-    <mergeCell ref="HF6:IJ6"/>
-    <mergeCell ref="IK6:JN6"/>
-    <mergeCell ref="JO6:KS6"/>
-    <mergeCell ref="KT6:LW6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35338,9 +35354,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:NB71"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="BS1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="EI35" sqref="EI35"/>
+      <selection pane="topRight" activeCell="DK26" sqref="DK26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -37768,7 +37784,7 @@
       <c r="DL10" s="30"/>
       <c r="DM10" s="30"/>
       <c r="DN10" s="30" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="DO10" s="31"/>
       <c r="DP10" s="31"/>
@@ -39631,7 +39647,9 @@
       <c r="DM15" s="76"/>
       <c r="DN15" s="76"/>
       <c r="DO15" s="77"/>
-      <c r="DP15" s="77"/>
+      <c r="DP15" s="80" t="s">
+        <v>135</v>
+      </c>
       <c r="DQ15" s="84"/>
       <c r="DR15" s="82"/>
       <c r="DS15" s="76"/>
@@ -40009,7 +40027,9 @@
       <c r="DO16" s="14"/>
       <c r="DP16" s="14"/>
       <c r="DQ16" s="25"/>
-      <c r="DR16" s="67"/>
+      <c r="DR16" s="207" t="s">
+        <v>136</v>
+      </c>
       <c r="DS16" s="16"/>
       <c r="DT16" s="16"/>
       <c r="DU16" s="16"/>
@@ -40377,9 +40397,7 @@
       <c r="DM17" s="16"/>
       <c r="DN17" s="16"/>
       <c r="DO17" s="14"/>
-      <c r="DP17" s="56" t="s">
-        <v>130</v>
-      </c>
+      <c r="DP17" s="14"/>
       <c r="DQ17" s="13"/>
       <c r="DR17" s="67"/>
       <c r="DS17" s="16"/>
@@ -40751,7 +40769,7 @@
       <c r="DQ18" s="25"/>
       <c r="DR18" s="67"/>
       <c r="DS18" s="16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="DT18" s="16"/>
       <c r="DU18" s="16"/>
@@ -42625,7 +42643,7 @@
       <c r="DN23" s="16"/>
       <c r="DO23" s="14"/>
       <c r="DP23" s="14"/>
-      <c r="DQ23" s="122" t="s">
+      <c r="DQ23" s="90" t="s">
         <v>53</v>
       </c>
       <c r="DR23" s="67"/>
@@ -54479,15 +54497,6 @@
     <row r="71" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="A45:A49"/>
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A30:A34"/>
-    <mergeCell ref="A35:A39"/>
     <mergeCell ref="LX6:NB6"/>
     <mergeCell ref="B6:AF6"/>
     <mergeCell ref="AG6:BH6"/>
@@ -54500,6 +54509,15 @@
     <mergeCell ref="IK6:JN6"/>
     <mergeCell ref="JO6:KS6"/>
     <mergeCell ref="KT6:LW6"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="A35:A39"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -54513,15 +54531,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="6.125" style="166" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.25" customWidth="1"/>
+    <col min="4" max="4" width="48.875" customWidth="1"/>
     <col min="5" max="5" width="6.125" style="166" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="50.5" customWidth="1"/>
   </cols>
@@ -54529,30 +54547,30 @@
     <row r="1" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="202" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C2" s="204" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D2" s="205"/>
       <c r="E2" s="206" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F2" s="205"/>
     </row>
     <row r="3" spans="2:6" s="167" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="203"/>
       <c r="C3" s="174" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D3" s="171" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E3" s="173" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F3" s="171" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="33" x14ac:dyDescent="0.3">
@@ -54563,13 +54581,13 @@
         <v>4</v>
       </c>
       <c r="D4" s="180" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E4" s="181">
         <v>1</v>
       </c>
       <c r="F4" s="182" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="33" x14ac:dyDescent="0.3">
@@ -54580,13 +54598,13 @@
         <v>2</v>
       </c>
       <c r="D5" s="184" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E5" s="185">
         <v>4</v>
       </c>
       <c r="F5" s="188" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
@@ -54597,17 +54615,27 @@
         <v>3.5</v>
       </c>
       <c r="D6" s="188" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E6" s="185"/>
       <c r="F6" s="184"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="187"/>
-      <c r="C7" s="183"/>
-      <c r="D7" s="184"/>
-      <c r="E7" s="185"/>
-      <c r="F7" s="184"/>
+    <row r="7" spans="2:6" ht="66" x14ac:dyDescent="0.3">
+      <c r="B7" s="187">
+        <v>43221</v>
+      </c>
+      <c r="C7" s="183">
+        <v>4</v>
+      </c>
+      <c r="D7" s="188" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" s="185">
+        <v>4</v>
+      </c>
+      <c r="F7" s="184" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="187"/>

</xml_diff>

<commit_message>
[Pipette] Transformer V2.0 완료
</commit_message>
<xml_diff>
--- a/Femto Project schedule V1.0.xlsx
+++ b/Femto Project schedule V1.0.xlsx
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="145">
   <si>
     <t>◇PCB설계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -815,10 +815,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Pipette JTAG PCB 설계</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>◇ Main PCB 2D,BOM,datasheet 전달</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -843,10 +839,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Transformer PCB 작업</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Pipette V1.0 - 2D data 작업, Gerber 작업</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -864,6 +856,14 @@
   </si>
   <si>
     <t>Pipette JTAG PCB Layout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pipette JTAG PCB Layout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transformer PCB Layout</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1921,6 +1921,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1974,9 +1977,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -8950,167 +8950,167 @@
     </row>
     <row r="6" spans="1:152" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="197">
+      <c r="B6" s="198">
         <v>1</v>
       </c>
-      <c r="C6" s="194"/>
-      <c r="D6" s="194"/>
-      <c r="E6" s="194"/>
-      <c r="F6" s="194"/>
-      <c r="G6" s="194"/>
-      <c r="H6" s="194"/>
-      <c r="I6" s="194"/>
-      <c r="J6" s="194"/>
-      <c r="K6" s="194"/>
-      <c r="L6" s="194"/>
-      <c r="M6" s="194"/>
-      <c r="N6" s="194"/>
-      <c r="O6" s="194"/>
-      <c r="P6" s="194"/>
-      <c r="Q6" s="194"/>
-      <c r="R6" s="194"/>
-      <c r="S6" s="194"/>
-      <c r="T6" s="194"/>
-      <c r="U6" s="194"/>
-      <c r="V6" s="194"/>
-      <c r="W6" s="194"/>
-      <c r="X6" s="194"/>
-      <c r="Y6" s="194"/>
-      <c r="Z6" s="194"/>
-      <c r="AA6" s="194"/>
-      <c r="AB6" s="194"/>
-      <c r="AC6" s="194"/>
-      <c r="AD6" s="194"/>
-      <c r="AE6" s="194"/>
-      <c r="AF6" s="194"/>
-      <c r="AG6" s="197">
+      <c r="C6" s="195"/>
+      <c r="D6" s="195"/>
+      <c r="E6" s="195"/>
+      <c r="F6" s="195"/>
+      <c r="G6" s="195"/>
+      <c r="H6" s="195"/>
+      <c r="I6" s="195"/>
+      <c r="J6" s="195"/>
+      <c r="K6" s="195"/>
+      <c r="L6" s="195"/>
+      <c r="M6" s="195"/>
+      <c r="N6" s="195"/>
+      <c r="O6" s="195"/>
+      <c r="P6" s="195"/>
+      <c r="Q6" s="195"/>
+      <c r="R6" s="195"/>
+      <c r="S6" s="195"/>
+      <c r="T6" s="195"/>
+      <c r="U6" s="195"/>
+      <c r="V6" s="195"/>
+      <c r="W6" s="195"/>
+      <c r="X6" s="195"/>
+      <c r="Y6" s="195"/>
+      <c r="Z6" s="195"/>
+      <c r="AA6" s="195"/>
+      <c r="AB6" s="195"/>
+      <c r="AC6" s="195"/>
+      <c r="AD6" s="195"/>
+      <c r="AE6" s="195"/>
+      <c r="AF6" s="195"/>
+      <c r="AG6" s="198">
         <v>2</v>
       </c>
-      <c r="AH6" s="194"/>
-      <c r="AI6" s="194"/>
-      <c r="AJ6" s="194"/>
-      <c r="AK6" s="194"/>
-      <c r="AL6" s="194"/>
-      <c r="AM6" s="194"/>
-      <c r="AN6" s="194"/>
-      <c r="AO6" s="194"/>
-      <c r="AP6" s="194"/>
-      <c r="AQ6" s="194"/>
-      <c r="AR6" s="194"/>
-      <c r="AS6" s="194"/>
-      <c r="AT6" s="194"/>
-      <c r="AU6" s="194"/>
-      <c r="AV6" s="194"/>
-      <c r="AW6" s="194"/>
-      <c r="AX6" s="194"/>
-      <c r="AY6" s="194"/>
-      <c r="AZ6" s="194"/>
-      <c r="BA6" s="194"/>
-      <c r="BB6" s="194"/>
-      <c r="BC6" s="194"/>
-      <c r="BD6" s="194"/>
-      <c r="BE6" s="194"/>
-      <c r="BF6" s="194"/>
-      <c r="BG6" s="194"/>
-      <c r="BH6" s="195"/>
-      <c r="BI6" s="194">
+      <c r="AH6" s="195"/>
+      <c r="AI6" s="195"/>
+      <c r="AJ6" s="195"/>
+      <c r="AK6" s="195"/>
+      <c r="AL6" s="195"/>
+      <c r="AM6" s="195"/>
+      <c r="AN6" s="195"/>
+      <c r="AO6" s="195"/>
+      <c r="AP6" s="195"/>
+      <c r="AQ6" s="195"/>
+      <c r="AR6" s="195"/>
+      <c r="AS6" s="195"/>
+      <c r="AT6" s="195"/>
+      <c r="AU6" s="195"/>
+      <c r="AV6" s="195"/>
+      <c r="AW6" s="195"/>
+      <c r="AX6" s="195"/>
+      <c r="AY6" s="195"/>
+      <c r="AZ6" s="195"/>
+      <c r="BA6" s="195"/>
+      <c r="BB6" s="195"/>
+      <c r="BC6" s="195"/>
+      <c r="BD6" s="195"/>
+      <c r="BE6" s="195"/>
+      <c r="BF6" s="195"/>
+      <c r="BG6" s="195"/>
+      <c r="BH6" s="196"/>
+      <c r="BI6" s="195">
         <v>3</v>
       </c>
-      <c r="BJ6" s="194"/>
-      <c r="BK6" s="194"/>
-      <c r="BL6" s="194"/>
-      <c r="BM6" s="194"/>
-      <c r="BN6" s="194"/>
-      <c r="BO6" s="194"/>
-      <c r="BP6" s="194"/>
-      <c r="BQ6" s="194"/>
-      <c r="BR6" s="194"/>
-      <c r="BS6" s="194"/>
-      <c r="BT6" s="194"/>
-      <c r="BU6" s="194"/>
-      <c r="BV6" s="194"/>
-      <c r="BW6" s="194"/>
-      <c r="BX6" s="194"/>
-      <c r="BY6" s="194"/>
-      <c r="BZ6" s="194"/>
-      <c r="CA6" s="194"/>
-      <c r="CB6" s="194"/>
-      <c r="CC6" s="194"/>
-      <c r="CD6" s="194"/>
-      <c r="CE6" s="194"/>
-      <c r="CF6" s="194"/>
-      <c r="CG6" s="194"/>
-      <c r="CH6" s="194"/>
-      <c r="CI6" s="194"/>
-      <c r="CJ6" s="194"/>
-      <c r="CK6" s="194"/>
-      <c r="CL6" s="194"/>
-      <c r="CM6" s="194"/>
-      <c r="CN6" s="198">
+      <c r="BJ6" s="195"/>
+      <c r="BK6" s="195"/>
+      <c r="BL6" s="195"/>
+      <c r="BM6" s="195"/>
+      <c r="BN6" s="195"/>
+      <c r="BO6" s="195"/>
+      <c r="BP6" s="195"/>
+      <c r="BQ6" s="195"/>
+      <c r="BR6" s="195"/>
+      <c r="BS6" s="195"/>
+      <c r="BT6" s="195"/>
+      <c r="BU6" s="195"/>
+      <c r="BV6" s="195"/>
+      <c r="BW6" s="195"/>
+      <c r="BX6" s="195"/>
+      <c r="BY6" s="195"/>
+      <c r="BZ6" s="195"/>
+      <c r="CA6" s="195"/>
+      <c r="CB6" s="195"/>
+      <c r="CC6" s="195"/>
+      <c r="CD6" s="195"/>
+      <c r="CE6" s="195"/>
+      <c r="CF6" s="195"/>
+      <c r="CG6" s="195"/>
+      <c r="CH6" s="195"/>
+      <c r="CI6" s="195"/>
+      <c r="CJ6" s="195"/>
+      <c r="CK6" s="195"/>
+      <c r="CL6" s="195"/>
+      <c r="CM6" s="195"/>
+      <c r="CN6" s="199">
         <v>4</v>
       </c>
-      <c r="CO6" s="199"/>
-      <c r="CP6" s="199"/>
-      <c r="CQ6" s="199"/>
-      <c r="CR6" s="199"/>
-      <c r="CS6" s="199"/>
-      <c r="CT6" s="199"/>
-      <c r="CU6" s="199"/>
-      <c r="CV6" s="199"/>
-      <c r="CW6" s="199"/>
-      <c r="CX6" s="199"/>
-      <c r="CY6" s="199"/>
-      <c r="CZ6" s="199"/>
-      <c r="DA6" s="199"/>
-      <c r="DB6" s="199"/>
-      <c r="DC6" s="199"/>
-      <c r="DD6" s="199"/>
-      <c r="DE6" s="199"/>
-      <c r="DF6" s="199"/>
-      <c r="DG6" s="199"/>
-      <c r="DH6" s="199"/>
-      <c r="DI6" s="199"/>
-      <c r="DJ6" s="199"/>
-      <c r="DK6" s="199"/>
-      <c r="DL6" s="199"/>
-      <c r="DM6" s="199"/>
-      <c r="DN6" s="199"/>
-      <c r="DO6" s="199"/>
-      <c r="DP6" s="199"/>
-      <c r="DQ6" s="200"/>
-      <c r="DR6" s="194">
+      <c r="CO6" s="200"/>
+      <c r="CP6" s="200"/>
+      <c r="CQ6" s="200"/>
+      <c r="CR6" s="200"/>
+      <c r="CS6" s="200"/>
+      <c r="CT6" s="200"/>
+      <c r="CU6" s="200"/>
+      <c r="CV6" s="200"/>
+      <c r="CW6" s="200"/>
+      <c r="CX6" s="200"/>
+      <c r="CY6" s="200"/>
+      <c r="CZ6" s="200"/>
+      <c r="DA6" s="200"/>
+      <c r="DB6" s="200"/>
+      <c r="DC6" s="200"/>
+      <c r="DD6" s="200"/>
+      <c r="DE6" s="200"/>
+      <c r="DF6" s="200"/>
+      <c r="DG6" s="200"/>
+      <c r="DH6" s="200"/>
+      <c r="DI6" s="200"/>
+      <c r="DJ6" s="200"/>
+      <c r="DK6" s="200"/>
+      <c r="DL6" s="200"/>
+      <c r="DM6" s="200"/>
+      <c r="DN6" s="200"/>
+      <c r="DO6" s="200"/>
+      <c r="DP6" s="200"/>
+      <c r="DQ6" s="201"/>
+      <c r="DR6" s="195">
         <v>5</v>
       </c>
-      <c r="DS6" s="194"/>
-      <c r="DT6" s="194"/>
-      <c r="DU6" s="194"/>
-      <c r="DV6" s="194"/>
-      <c r="DW6" s="194"/>
-      <c r="DX6" s="194"/>
-      <c r="DY6" s="194"/>
-      <c r="DZ6" s="194"/>
-      <c r="EA6" s="194"/>
-      <c r="EB6" s="194"/>
-      <c r="EC6" s="194"/>
-      <c r="ED6" s="194"/>
-      <c r="EE6" s="194"/>
-      <c r="EF6" s="194"/>
-      <c r="EG6" s="194"/>
-      <c r="EH6" s="194"/>
-      <c r="EI6" s="194"/>
-      <c r="EJ6" s="194"/>
-      <c r="EK6" s="194"/>
-      <c r="EL6" s="194"/>
-      <c r="EM6" s="194"/>
-      <c r="EN6" s="194"/>
-      <c r="EO6" s="194"/>
-      <c r="EP6" s="194"/>
-      <c r="EQ6" s="194"/>
-      <c r="ER6" s="194"/>
-      <c r="ES6" s="194"/>
-      <c r="ET6" s="194"/>
-      <c r="EU6" s="194"/>
-      <c r="EV6" s="195"/>
+      <c r="DS6" s="195"/>
+      <c r="DT6" s="195"/>
+      <c r="DU6" s="195"/>
+      <c r="DV6" s="195"/>
+      <c r="DW6" s="195"/>
+      <c r="DX6" s="195"/>
+      <c r="DY6" s="195"/>
+      <c r="DZ6" s="195"/>
+      <c r="EA6" s="195"/>
+      <c r="EB6" s="195"/>
+      <c r="EC6" s="195"/>
+      <c r="ED6" s="195"/>
+      <c r="EE6" s="195"/>
+      <c r="EF6" s="195"/>
+      <c r="EG6" s="195"/>
+      <c r="EH6" s="195"/>
+      <c r="EI6" s="195"/>
+      <c r="EJ6" s="195"/>
+      <c r="EK6" s="195"/>
+      <c r="EL6" s="195"/>
+      <c r="EM6" s="195"/>
+      <c r="EN6" s="195"/>
+      <c r="EO6" s="195"/>
+      <c r="EP6" s="195"/>
+      <c r="EQ6" s="195"/>
+      <c r="ER6" s="195"/>
+      <c r="ES6" s="195"/>
+      <c r="ET6" s="195"/>
+      <c r="EU6" s="195"/>
+      <c r="EV6" s="196"/>
     </row>
     <row r="7" spans="1:152" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -9569,7 +9569,7 @@
       </c>
     </row>
     <row r="8" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A8" s="191" t="s">
+      <c r="A8" s="192" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="34"/>
@@ -9733,7 +9733,7 @@
       <c r="EV8" s="99"/>
     </row>
     <row r="9" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A9" s="191"/>
+      <c r="A9" s="192"/>
       <c r="B9" s="29"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -9893,7 +9893,7 @@
       <c r="EV9" s="33"/>
     </row>
     <row r="10" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A10" s="191"/>
+      <c r="A10" s="192"/>
       <c r="B10" s="29"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
@@ -10053,7 +10053,7 @@
       <c r="EV10" s="33"/>
     </row>
     <row r="11" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A11" s="191"/>
+      <c r="A11" s="192"/>
       <c r="B11" s="29"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
@@ -10211,7 +10211,7 @@
       <c r="EV11" s="33"/>
     </row>
     <row r="12" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A12" s="191"/>
+      <c r="A12" s="192"/>
       <c r="B12" s="29"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
@@ -10369,7 +10369,7 @@
       <c r="EV12" s="33"/>
     </row>
     <row r="13" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A13" s="191"/>
+      <c r="A13" s="192"/>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -10525,7 +10525,7 @@
       <c r="EV13" s="33"/>
     </row>
     <row r="14" spans="1:152" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="196"/>
+      <c r="A14" s="197"/>
       <c r="B14" s="50"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51"/>
@@ -10679,7 +10679,7 @@
       <c r="EV14" s="100"/>
     </row>
     <row r="15" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A15" s="193" t="s">
+      <c r="A15" s="194" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="42"/>
@@ -10841,7 +10841,7 @@
       <c r="EV15" s="102"/>
     </row>
     <row r="16" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A16" s="191"/>
+      <c r="A16" s="192"/>
       <c r="B16" s="24"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -10999,7 +10999,7 @@
       <c r="EV16" s="17"/>
     </row>
     <row r="17" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A17" s="191"/>
+      <c r="A17" s="192"/>
       <c r="B17" s="24"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -11159,7 +11159,7 @@
       <c r="EV17" s="17"/>
     </row>
     <row r="18" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A18" s="191"/>
+      <c r="A18" s="192"/>
       <c r="B18" s="24"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -11315,7 +11315,7 @@
       <c r="EV18" s="17"/>
     </row>
     <row r="19" spans="1:152" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="191"/>
+      <c r="A19" s="192"/>
       <c r="B19" s="26"/>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
@@ -11471,7 +11471,7 @@
       <c r="EV19" s="98"/>
     </row>
     <row r="20" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="193" t="s">
+      <c r="A20" s="194" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="75"/>
@@ -11633,7 +11633,7 @@
       <c r="EV20" s="102"/>
     </row>
     <row r="21" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="191"/>
+      <c r="A21" s="192"/>
       <c r="B21" s="24"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -11791,7 +11791,7 @@
       <c r="EV21" s="17"/>
     </row>
     <row r="22" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="191"/>
+      <c r="A22" s="192"/>
       <c r="B22" s="24"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -11949,7 +11949,7 @@
       <c r="EV22" s="17"/>
     </row>
     <row r="23" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="191"/>
+      <c r="A23" s="192"/>
       <c r="B23" s="24"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -12107,7 +12107,7 @@
       <c r="EV23" s="17"/>
     </row>
     <row r="24" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="192"/>
+      <c r="A24" s="193"/>
       <c r="B24" s="91"/>
       <c r="C24" s="92"/>
       <c r="D24" s="92"/>
@@ -12261,7 +12261,7 @@
       <c r="EV24" s="98"/>
     </row>
     <row r="25" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="193" t="s">
+      <c r="A25" s="194" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="75"/>
@@ -12417,7 +12417,7 @@
       <c r="EV25" s="102"/>
     </row>
     <row r="26" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="191"/>
+      <c r="A26" s="192"/>
       <c r="B26" s="24"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -12571,7 +12571,7 @@
       <c r="EV26" s="17"/>
     </row>
     <row r="27" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="191"/>
+      <c r="A27" s="192"/>
       <c r="B27" s="24"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
@@ -12725,7 +12725,7 @@
       <c r="EV27" s="17"/>
     </row>
     <row r="28" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="191"/>
+      <c r="A28" s="192"/>
       <c r="B28" s="24"/>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
@@ -12879,7 +12879,7 @@
       <c r="EV28" s="17"/>
     </row>
     <row r="29" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="191"/>
+      <c r="A29" s="192"/>
       <c r="B29" s="85"/>
       <c r="C29" s="71"/>
       <c r="D29" s="71"/>
@@ -13033,7 +13033,7 @@
       <c r="EV29" s="98"/>
     </row>
     <row r="30" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="190" t="s">
+      <c r="A30" s="191" t="s">
         <v>20</v>
       </c>
       <c r="B30" s="75"/>
@@ -13199,7 +13199,7 @@
       <c r="EV30" s="102"/>
     </row>
     <row r="31" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="191"/>
+      <c r="A31" s="192"/>
       <c r="B31" s="24"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -13357,7 +13357,7 @@
       <c r="EV31" s="17"/>
     </row>
     <row r="32" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="191"/>
+      <c r="A32" s="192"/>
       <c r="B32" s="24"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
@@ -13515,7 +13515,7 @@
       <c r="EV32" s="17"/>
     </row>
     <row r="33" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="191"/>
+      <c r="A33" s="192"/>
       <c r="B33" s="24"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
@@ -13671,7 +13671,7 @@
       <c r="EV33" s="17"/>
     </row>
     <row r="34" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="192"/>
+      <c r="A34" s="193"/>
       <c r="B34" s="85"/>
       <c r="C34" s="71"/>
       <c r="D34" s="71"/>
@@ -13827,7 +13827,7 @@
       <c r="EV34" s="98"/>
     </row>
     <row r="35" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="191" t="s">
+      <c r="A35" s="192" t="s">
         <v>23</v>
       </c>
       <c r="B35" s="75"/>
@@ -13985,7 +13985,7 @@
       <c r="EV35" s="102"/>
     </row>
     <row r="36" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="191"/>
+      <c r="A36" s="192"/>
       <c r="B36" s="24"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
@@ -14141,7 +14141,7 @@
       <c r="EV36" s="17"/>
     </row>
     <row r="37" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="191"/>
+      <c r="A37" s="192"/>
       <c r="B37" s="24"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -14295,7 +14295,7 @@
       <c r="EV37" s="17"/>
     </row>
     <row r="38" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="191"/>
+      <c r="A38" s="192"/>
       <c r="B38" s="24"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
@@ -14449,7 +14449,7 @@
       <c r="EV38" s="17"/>
     </row>
     <row r="39" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="191"/>
+      <c r="A39" s="192"/>
       <c r="B39" s="85"/>
       <c r="C39" s="71"/>
       <c r="D39" s="71"/>
@@ -14603,7 +14603,7 @@
       <c r="EV39" s="98"/>
     </row>
     <row r="40" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="190" t="s">
+      <c r="A40" s="191" t="s">
         <v>22</v>
       </c>
       <c r="B40" s="75"/>
@@ -14765,7 +14765,7 @@
       <c r="EV40" s="102"/>
     </row>
     <row r="41" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="191"/>
+      <c r="A41" s="192"/>
       <c r="B41" s="24"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
@@ -14921,7 +14921,7 @@
       <c r="EV41" s="17"/>
     </row>
     <row r="42" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="191"/>
+      <c r="A42" s="192"/>
       <c r="B42" s="24"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -15079,7 +15079,7 @@
       <c r="EV42" s="17"/>
     </row>
     <row r="43" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="191"/>
+      <c r="A43" s="192"/>
       <c r="B43" s="24"/>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
@@ -15235,7 +15235,7 @@
       <c r="EV43" s="17"/>
     </row>
     <row r="44" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="192"/>
+      <c r="A44" s="193"/>
       <c r="B44" s="85"/>
       <c r="C44" s="71"/>
       <c r="D44" s="71"/>
@@ -15391,7 +15391,7 @@
       <c r="EV44" s="98"/>
     </row>
     <row r="45" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="191" t="s">
+      <c r="A45" s="192" t="s">
         <v>24</v>
       </c>
       <c r="B45" s="75"/>
@@ -15553,7 +15553,7 @@
       <c r="EV45" s="102"/>
     </row>
     <row r="46" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="191"/>
+      <c r="A46" s="192"/>
       <c r="B46" s="24"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
@@ -15709,7 +15709,7 @@
       <c r="EV46" s="17"/>
     </row>
     <row r="47" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="191"/>
+      <c r="A47" s="192"/>
       <c r="B47" s="24"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
@@ -15867,7 +15867,7 @@
       <c r="EV47" s="17"/>
     </row>
     <row r="48" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="191"/>
+      <c r="A48" s="192"/>
       <c r="B48" s="24"/>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -16023,7 +16023,7 @@
       <c r="EV48" s="17"/>
     </row>
     <row r="49" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="192"/>
+      <c r="A49" s="193"/>
       <c r="B49" s="85"/>
       <c r="C49" s="71"/>
       <c r="D49" s="71"/>
@@ -16259,395 +16259,395 @@
     </row>
     <row r="6" spans="1:366" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="197">
+      <c r="B6" s="198">
         <v>1</v>
       </c>
-      <c r="C6" s="194"/>
-      <c r="D6" s="194"/>
-      <c r="E6" s="194"/>
-      <c r="F6" s="194"/>
-      <c r="G6" s="194"/>
-      <c r="H6" s="194"/>
-      <c r="I6" s="194"/>
-      <c r="J6" s="194"/>
-      <c r="K6" s="194"/>
-      <c r="L6" s="194"/>
-      <c r="M6" s="194"/>
-      <c r="N6" s="194"/>
-      <c r="O6" s="194"/>
-      <c r="P6" s="194"/>
-      <c r="Q6" s="194"/>
-      <c r="R6" s="194"/>
-      <c r="S6" s="194"/>
-      <c r="T6" s="194"/>
-      <c r="U6" s="194"/>
-      <c r="V6" s="194"/>
-      <c r="W6" s="194"/>
-      <c r="X6" s="194"/>
-      <c r="Y6" s="194"/>
-      <c r="Z6" s="194"/>
-      <c r="AA6" s="194"/>
-      <c r="AB6" s="194"/>
-      <c r="AC6" s="194"/>
-      <c r="AD6" s="194"/>
-      <c r="AE6" s="194"/>
-      <c r="AF6" s="194"/>
-      <c r="AG6" s="197">
+      <c r="C6" s="195"/>
+      <c r="D6" s="195"/>
+      <c r="E6" s="195"/>
+      <c r="F6" s="195"/>
+      <c r="G6" s="195"/>
+      <c r="H6" s="195"/>
+      <c r="I6" s="195"/>
+      <c r="J6" s="195"/>
+      <c r="K6" s="195"/>
+      <c r="L6" s="195"/>
+      <c r="M6" s="195"/>
+      <c r="N6" s="195"/>
+      <c r="O6" s="195"/>
+      <c r="P6" s="195"/>
+      <c r="Q6" s="195"/>
+      <c r="R6" s="195"/>
+      <c r="S6" s="195"/>
+      <c r="T6" s="195"/>
+      <c r="U6" s="195"/>
+      <c r="V6" s="195"/>
+      <c r="W6" s="195"/>
+      <c r="X6" s="195"/>
+      <c r="Y6" s="195"/>
+      <c r="Z6" s="195"/>
+      <c r="AA6" s="195"/>
+      <c r="AB6" s="195"/>
+      <c r="AC6" s="195"/>
+      <c r="AD6" s="195"/>
+      <c r="AE6" s="195"/>
+      <c r="AF6" s="195"/>
+      <c r="AG6" s="198">
         <v>2</v>
       </c>
-      <c r="AH6" s="194"/>
-      <c r="AI6" s="194"/>
-      <c r="AJ6" s="194"/>
-      <c r="AK6" s="194"/>
-      <c r="AL6" s="194"/>
-      <c r="AM6" s="194"/>
-      <c r="AN6" s="194"/>
-      <c r="AO6" s="194"/>
-      <c r="AP6" s="194"/>
-      <c r="AQ6" s="194"/>
-      <c r="AR6" s="194"/>
-      <c r="AS6" s="194"/>
-      <c r="AT6" s="194"/>
-      <c r="AU6" s="194"/>
-      <c r="AV6" s="194"/>
-      <c r="AW6" s="194"/>
-      <c r="AX6" s="194"/>
-      <c r="AY6" s="194"/>
-      <c r="AZ6" s="194"/>
-      <c r="BA6" s="194"/>
-      <c r="BB6" s="194"/>
-      <c r="BC6" s="194"/>
-      <c r="BD6" s="194"/>
-      <c r="BE6" s="194"/>
-      <c r="BF6" s="194"/>
-      <c r="BG6" s="194"/>
-      <c r="BH6" s="195"/>
-      <c r="BI6" s="194">
+      <c r="AH6" s="195"/>
+      <c r="AI6" s="195"/>
+      <c r="AJ6" s="195"/>
+      <c r="AK6" s="195"/>
+      <c r="AL6" s="195"/>
+      <c r="AM6" s="195"/>
+      <c r="AN6" s="195"/>
+      <c r="AO6" s="195"/>
+      <c r="AP6" s="195"/>
+      <c r="AQ6" s="195"/>
+      <c r="AR6" s="195"/>
+      <c r="AS6" s="195"/>
+      <c r="AT6" s="195"/>
+      <c r="AU6" s="195"/>
+      <c r="AV6" s="195"/>
+      <c r="AW6" s="195"/>
+      <c r="AX6" s="195"/>
+      <c r="AY6" s="195"/>
+      <c r="AZ6" s="195"/>
+      <c r="BA6" s="195"/>
+      <c r="BB6" s="195"/>
+      <c r="BC6" s="195"/>
+      <c r="BD6" s="195"/>
+      <c r="BE6" s="195"/>
+      <c r="BF6" s="195"/>
+      <c r="BG6" s="195"/>
+      <c r="BH6" s="196"/>
+      <c r="BI6" s="195">
         <v>3</v>
       </c>
-      <c r="BJ6" s="194"/>
-      <c r="BK6" s="194"/>
-      <c r="BL6" s="194"/>
-      <c r="BM6" s="194"/>
-      <c r="BN6" s="194"/>
-      <c r="BO6" s="194"/>
-      <c r="BP6" s="194"/>
-      <c r="BQ6" s="194"/>
-      <c r="BR6" s="194"/>
-      <c r="BS6" s="194"/>
-      <c r="BT6" s="194"/>
-      <c r="BU6" s="194"/>
-      <c r="BV6" s="194"/>
-      <c r="BW6" s="194"/>
-      <c r="BX6" s="194"/>
-      <c r="BY6" s="194"/>
-      <c r="BZ6" s="194"/>
-      <c r="CA6" s="194"/>
-      <c r="CB6" s="194"/>
-      <c r="CC6" s="194"/>
-      <c r="CD6" s="194"/>
-      <c r="CE6" s="194"/>
-      <c r="CF6" s="194"/>
-      <c r="CG6" s="194"/>
-      <c r="CH6" s="194"/>
-      <c r="CI6" s="194"/>
-      <c r="CJ6" s="194"/>
-      <c r="CK6" s="194"/>
-      <c r="CL6" s="194"/>
-      <c r="CM6" s="194"/>
-      <c r="CN6" s="198">
+      <c r="BJ6" s="195"/>
+      <c r="BK6" s="195"/>
+      <c r="BL6" s="195"/>
+      <c r="BM6" s="195"/>
+      <c r="BN6" s="195"/>
+      <c r="BO6" s="195"/>
+      <c r="BP6" s="195"/>
+      <c r="BQ6" s="195"/>
+      <c r="BR6" s="195"/>
+      <c r="BS6" s="195"/>
+      <c r="BT6" s="195"/>
+      <c r="BU6" s="195"/>
+      <c r="BV6" s="195"/>
+      <c r="BW6" s="195"/>
+      <c r="BX6" s="195"/>
+      <c r="BY6" s="195"/>
+      <c r="BZ6" s="195"/>
+      <c r="CA6" s="195"/>
+      <c r="CB6" s="195"/>
+      <c r="CC6" s="195"/>
+      <c r="CD6" s="195"/>
+      <c r="CE6" s="195"/>
+      <c r="CF6" s="195"/>
+      <c r="CG6" s="195"/>
+      <c r="CH6" s="195"/>
+      <c r="CI6" s="195"/>
+      <c r="CJ6" s="195"/>
+      <c r="CK6" s="195"/>
+      <c r="CL6" s="195"/>
+      <c r="CM6" s="195"/>
+      <c r="CN6" s="199">
         <v>4</v>
       </c>
-      <c r="CO6" s="199"/>
-      <c r="CP6" s="199"/>
-      <c r="CQ6" s="199"/>
-      <c r="CR6" s="199"/>
-      <c r="CS6" s="199"/>
-      <c r="CT6" s="199"/>
-      <c r="CU6" s="199"/>
-      <c r="CV6" s="199"/>
-      <c r="CW6" s="199"/>
-      <c r="CX6" s="199"/>
-      <c r="CY6" s="199"/>
-      <c r="CZ6" s="199"/>
-      <c r="DA6" s="199"/>
-      <c r="DB6" s="199"/>
-      <c r="DC6" s="199"/>
-      <c r="DD6" s="199"/>
-      <c r="DE6" s="199"/>
-      <c r="DF6" s="199"/>
-      <c r="DG6" s="199"/>
-      <c r="DH6" s="199"/>
-      <c r="DI6" s="199"/>
-      <c r="DJ6" s="199"/>
-      <c r="DK6" s="199"/>
-      <c r="DL6" s="199"/>
-      <c r="DM6" s="199"/>
-      <c r="DN6" s="199"/>
-      <c r="DO6" s="199"/>
-      <c r="DP6" s="199"/>
-      <c r="DQ6" s="200"/>
-      <c r="DR6" s="194">
+      <c r="CO6" s="200"/>
+      <c r="CP6" s="200"/>
+      <c r="CQ6" s="200"/>
+      <c r="CR6" s="200"/>
+      <c r="CS6" s="200"/>
+      <c r="CT6" s="200"/>
+      <c r="CU6" s="200"/>
+      <c r="CV6" s="200"/>
+      <c r="CW6" s="200"/>
+      <c r="CX6" s="200"/>
+      <c r="CY6" s="200"/>
+      <c r="CZ6" s="200"/>
+      <c r="DA6" s="200"/>
+      <c r="DB6" s="200"/>
+      <c r="DC6" s="200"/>
+      <c r="DD6" s="200"/>
+      <c r="DE6" s="200"/>
+      <c r="DF6" s="200"/>
+      <c r="DG6" s="200"/>
+      <c r="DH6" s="200"/>
+      <c r="DI6" s="200"/>
+      <c r="DJ6" s="200"/>
+      <c r="DK6" s="200"/>
+      <c r="DL6" s="200"/>
+      <c r="DM6" s="200"/>
+      <c r="DN6" s="200"/>
+      <c r="DO6" s="200"/>
+      <c r="DP6" s="200"/>
+      <c r="DQ6" s="201"/>
+      <c r="DR6" s="195">
         <v>5</v>
       </c>
-      <c r="DS6" s="194"/>
-      <c r="DT6" s="194"/>
-      <c r="DU6" s="194"/>
-      <c r="DV6" s="194"/>
-      <c r="DW6" s="194"/>
-      <c r="DX6" s="194"/>
-      <c r="DY6" s="194"/>
-      <c r="DZ6" s="194"/>
-      <c r="EA6" s="194"/>
-      <c r="EB6" s="194"/>
-      <c r="EC6" s="194"/>
-      <c r="ED6" s="194"/>
-      <c r="EE6" s="194"/>
-      <c r="EF6" s="194"/>
-      <c r="EG6" s="194"/>
-      <c r="EH6" s="194"/>
-      <c r="EI6" s="194"/>
-      <c r="EJ6" s="194"/>
-      <c r="EK6" s="194"/>
-      <c r="EL6" s="194"/>
-      <c r="EM6" s="194"/>
-      <c r="EN6" s="194"/>
-      <c r="EO6" s="194"/>
-      <c r="EP6" s="194"/>
-      <c r="EQ6" s="194"/>
-      <c r="ER6" s="194"/>
-      <c r="ES6" s="194"/>
-      <c r="ET6" s="194"/>
-      <c r="EU6" s="194"/>
-      <c r="EV6" s="195"/>
-      <c r="EW6" s="198">
+      <c r="DS6" s="195"/>
+      <c r="DT6" s="195"/>
+      <c r="DU6" s="195"/>
+      <c r="DV6" s="195"/>
+      <c r="DW6" s="195"/>
+      <c r="DX6" s="195"/>
+      <c r="DY6" s="195"/>
+      <c r="DZ6" s="195"/>
+      <c r="EA6" s="195"/>
+      <c r="EB6" s="195"/>
+      <c r="EC6" s="195"/>
+      <c r="ED6" s="195"/>
+      <c r="EE6" s="195"/>
+      <c r="EF6" s="195"/>
+      <c r="EG6" s="195"/>
+      <c r="EH6" s="195"/>
+      <c r="EI6" s="195"/>
+      <c r="EJ6" s="195"/>
+      <c r="EK6" s="195"/>
+      <c r="EL6" s="195"/>
+      <c r="EM6" s="195"/>
+      <c r="EN6" s="195"/>
+      <c r="EO6" s="195"/>
+      <c r="EP6" s="195"/>
+      <c r="EQ6" s="195"/>
+      <c r="ER6" s="195"/>
+      <c r="ES6" s="195"/>
+      <c r="ET6" s="195"/>
+      <c r="EU6" s="195"/>
+      <c r="EV6" s="196"/>
+      <c r="EW6" s="199">
         <v>6</v>
       </c>
-      <c r="EX6" s="199"/>
-      <c r="EY6" s="199"/>
-      <c r="EZ6" s="199"/>
-      <c r="FA6" s="199"/>
-      <c r="FB6" s="199"/>
-      <c r="FC6" s="199"/>
-      <c r="FD6" s="199"/>
-      <c r="FE6" s="199"/>
-      <c r="FF6" s="199"/>
-      <c r="FG6" s="199"/>
-      <c r="FH6" s="199"/>
-      <c r="FI6" s="199"/>
-      <c r="FJ6" s="199"/>
-      <c r="FK6" s="199"/>
-      <c r="FL6" s="199"/>
-      <c r="FM6" s="199"/>
-      <c r="FN6" s="199"/>
-      <c r="FO6" s="199"/>
-      <c r="FP6" s="199"/>
-      <c r="FQ6" s="199"/>
-      <c r="FR6" s="199"/>
-      <c r="FS6" s="199"/>
-      <c r="FT6" s="199"/>
-      <c r="FU6" s="199"/>
-      <c r="FV6" s="199"/>
-      <c r="FW6" s="199"/>
-      <c r="FX6" s="199"/>
-      <c r="FY6" s="199"/>
-      <c r="FZ6" s="200"/>
-      <c r="GA6" s="194">
+      <c r="EX6" s="200"/>
+      <c r="EY6" s="200"/>
+      <c r="EZ6" s="200"/>
+      <c r="FA6" s="200"/>
+      <c r="FB6" s="200"/>
+      <c r="FC6" s="200"/>
+      <c r="FD6" s="200"/>
+      <c r="FE6" s="200"/>
+      <c r="FF6" s="200"/>
+      <c r="FG6" s="200"/>
+      <c r="FH6" s="200"/>
+      <c r="FI6" s="200"/>
+      <c r="FJ6" s="200"/>
+      <c r="FK6" s="200"/>
+      <c r="FL6" s="200"/>
+      <c r="FM6" s="200"/>
+      <c r="FN6" s="200"/>
+      <c r="FO6" s="200"/>
+      <c r="FP6" s="200"/>
+      <c r="FQ6" s="200"/>
+      <c r="FR6" s="200"/>
+      <c r="FS6" s="200"/>
+      <c r="FT6" s="200"/>
+      <c r="FU6" s="200"/>
+      <c r="FV6" s="200"/>
+      <c r="FW6" s="200"/>
+      <c r="FX6" s="200"/>
+      <c r="FY6" s="200"/>
+      <c r="FZ6" s="201"/>
+      <c r="GA6" s="195">
         <v>7</v>
       </c>
-      <c r="GB6" s="194"/>
-      <c r="GC6" s="194"/>
-      <c r="GD6" s="194"/>
-      <c r="GE6" s="194"/>
-      <c r="GF6" s="194"/>
-      <c r="GG6" s="194"/>
-      <c r="GH6" s="194"/>
-      <c r="GI6" s="194"/>
-      <c r="GJ6" s="194"/>
-      <c r="GK6" s="194"/>
-      <c r="GL6" s="194"/>
-      <c r="GM6" s="194"/>
-      <c r="GN6" s="194"/>
-      <c r="GO6" s="194"/>
-      <c r="GP6" s="194"/>
-      <c r="GQ6" s="194"/>
-      <c r="GR6" s="194"/>
-      <c r="GS6" s="194"/>
-      <c r="GT6" s="194"/>
-      <c r="GU6" s="194"/>
-      <c r="GV6" s="194"/>
-      <c r="GW6" s="194"/>
-      <c r="GX6" s="194"/>
-      <c r="GY6" s="194"/>
-      <c r="GZ6" s="194"/>
-      <c r="HA6" s="194"/>
-      <c r="HB6" s="194"/>
-      <c r="HC6" s="194"/>
-      <c r="HD6" s="194"/>
-      <c r="HE6" s="195"/>
-      <c r="HF6" s="194">
+      <c r="GB6" s="195"/>
+      <c r="GC6" s="195"/>
+      <c r="GD6" s="195"/>
+      <c r="GE6" s="195"/>
+      <c r="GF6" s="195"/>
+      <c r="GG6" s="195"/>
+      <c r="GH6" s="195"/>
+      <c r="GI6" s="195"/>
+      <c r="GJ6" s="195"/>
+      <c r="GK6" s="195"/>
+      <c r="GL6" s="195"/>
+      <c r="GM6" s="195"/>
+      <c r="GN6" s="195"/>
+      <c r="GO6" s="195"/>
+      <c r="GP6" s="195"/>
+      <c r="GQ6" s="195"/>
+      <c r="GR6" s="195"/>
+      <c r="GS6" s="195"/>
+      <c r="GT6" s="195"/>
+      <c r="GU6" s="195"/>
+      <c r="GV6" s="195"/>
+      <c r="GW6" s="195"/>
+      <c r="GX6" s="195"/>
+      <c r="GY6" s="195"/>
+      <c r="GZ6" s="195"/>
+      <c r="HA6" s="195"/>
+      <c r="HB6" s="195"/>
+      <c r="HC6" s="195"/>
+      <c r="HD6" s="195"/>
+      <c r="HE6" s="196"/>
+      <c r="HF6" s="195">
         <v>8</v>
       </c>
-      <c r="HG6" s="194"/>
-      <c r="HH6" s="194"/>
-      <c r="HI6" s="194"/>
-      <c r="HJ6" s="194"/>
-      <c r="HK6" s="194"/>
-      <c r="HL6" s="194"/>
-      <c r="HM6" s="194"/>
-      <c r="HN6" s="194"/>
-      <c r="HO6" s="194"/>
-      <c r="HP6" s="194"/>
-      <c r="HQ6" s="194"/>
-      <c r="HR6" s="194"/>
-      <c r="HS6" s="194"/>
-      <c r="HT6" s="194"/>
-      <c r="HU6" s="194"/>
-      <c r="HV6" s="194"/>
-      <c r="HW6" s="194"/>
-      <c r="HX6" s="194"/>
-      <c r="HY6" s="194"/>
-      <c r="HZ6" s="194"/>
-      <c r="IA6" s="194"/>
-      <c r="IB6" s="194"/>
-      <c r="IC6" s="194"/>
-      <c r="ID6" s="194"/>
-      <c r="IE6" s="194"/>
-      <c r="IF6" s="194"/>
-      <c r="IG6" s="194"/>
-      <c r="IH6" s="194"/>
-      <c r="II6" s="194"/>
-      <c r="IJ6" s="195"/>
-      <c r="IK6" s="198">
+      <c r="HG6" s="195"/>
+      <c r="HH6" s="195"/>
+      <c r="HI6" s="195"/>
+      <c r="HJ6" s="195"/>
+      <c r="HK6" s="195"/>
+      <c r="HL6" s="195"/>
+      <c r="HM6" s="195"/>
+      <c r="HN6" s="195"/>
+      <c r="HO6" s="195"/>
+      <c r="HP6" s="195"/>
+      <c r="HQ6" s="195"/>
+      <c r="HR6" s="195"/>
+      <c r="HS6" s="195"/>
+      <c r="HT6" s="195"/>
+      <c r="HU6" s="195"/>
+      <c r="HV6" s="195"/>
+      <c r="HW6" s="195"/>
+      <c r="HX6" s="195"/>
+      <c r="HY6" s="195"/>
+      <c r="HZ6" s="195"/>
+      <c r="IA6" s="195"/>
+      <c r="IB6" s="195"/>
+      <c r="IC6" s="195"/>
+      <c r="ID6" s="195"/>
+      <c r="IE6" s="195"/>
+      <c r="IF6" s="195"/>
+      <c r="IG6" s="195"/>
+      <c r="IH6" s="195"/>
+      <c r="II6" s="195"/>
+      <c r="IJ6" s="196"/>
+      <c r="IK6" s="199">
         <v>9</v>
       </c>
-      <c r="IL6" s="199"/>
-      <c r="IM6" s="199"/>
-      <c r="IN6" s="199"/>
-      <c r="IO6" s="199"/>
-      <c r="IP6" s="199"/>
-      <c r="IQ6" s="199"/>
-      <c r="IR6" s="199"/>
-      <c r="IS6" s="199"/>
-      <c r="IT6" s="199"/>
-      <c r="IU6" s="199"/>
-      <c r="IV6" s="199"/>
-      <c r="IW6" s="199"/>
-      <c r="IX6" s="199"/>
-      <c r="IY6" s="199"/>
-      <c r="IZ6" s="199"/>
-      <c r="JA6" s="199"/>
-      <c r="JB6" s="199"/>
-      <c r="JC6" s="199"/>
-      <c r="JD6" s="199"/>
-      <c r="JE6" s="199"/>
-      <c r="JF6" s="199"/>
-      <c r="JG6" s="199"/>
-      <c r="JH6" s="199"/>
-      <c r="JI6" s="199"/>
-      <c r="JJ6" s="199"/>
-      <c r="JK6" s="199"/>
-      <c r="JL6" s="199"/>
-      <c r="JM6" s="199"/>
-      <c r="JN6" s="200"/>
-      <c r="JO6" s="194">
+      <c r="IL6" s="200"/>
+      <c r="IM6" s="200"/>
+      <c r="IN6" s="200"/>
+      <c r="IO6" s="200"/>
+      <c r="IP6" s="200"/>
+      <c r="IQ6" s="200"/>
+      <c r="IR6" s="200"/>
+      <c r="IS6" s="200"/>
+      <c r="IT6" s="200"/>
+      <c r="IU6" s="200"/>
+      <c r="IV6" s="200"/>
+      <c r="IW6" s="200"/>
+      <c r="IX6" s="200"/>
+      <c r="IY6" s="200"/>
+      <c r="IZ6" s="200"/>
+      <c r="JA6" s="200"/>
+      <c r="JB6" s="200"/>
+      <c r="JC6" s="200"/>
+      <c r="JD6" s="200"/>
+      <c r="JE6" s="200"/>
+      <c r="JF6" s="200"/>
+      <c r="JG6" s="200"/>
+      <c r="JH6" s="200"/>
+      <c r="JI6" s="200"/>
+      <c r="JJ6" s="200"/>
+      <c r="JK6" s="200"/>
+      <c r="JL6" s="200"/>
+      <c r="JM6" s="200"/>
+      <c r="JN6" s="201"/>
+      <c r="JO6" s="195">
         <v>10</v>
       </c>
-      <c r="JP6" s="194"/>
-      <c r="JQ6" s="194"/>
-      <c r="JR6" s="194"/>
-      <c r="JS6" s="194"/>
-      <c r="JT6" s="194"/>
-      <c r="JU6" s="194"/>
-      <c r="JV6" s="194"/>
-      <c r="JW6" s="194"/>
-      <c r="JX6" s="194"/>
-      <c r="JY6" s="194"/>
-      <c r="JZ6" s="194"/>
-      <c r="KA6" s="194"/>
-      <c r="KB6" s="194"/>
-      <c r="KC6" s="194"/>
-      <c r="KD6" s="194"/>
-      <c r="KE6" s="194"/>
-      <c r="KF6" s="194"/>
-      <c r="KG6" s="194"/>
-      <c r="KH6" s="194"/>
-      <c r="KI6" s="194"/>
-      <c r="KJ6" s="194"/>
-      <c r="KK6" s="194"/>
-      <c r="KL6" s="194"/>
-      <c r="KM6" s="194"/>
-      <c r="KN6" s="194"/>
-      <c r="KO6" s="194"/>
-      <c r="KP6" s="194"/>
-      <c r="KQ6" s="194"/>
-      <c r="KR6" s="194"/>
-      <c r="KS6" s="195"/>
-      <c r="KT6" s="198">
+      <c r="JP6" s="195"/>
+      <c r="JQ6" s="195"/>
+      <c r="JR6" s="195"/>
+      <c r="JS6" s="195"/>
+      <c r="JT6" s="195"/>
+      <c r="JU6" s="195"/>
+      <c r="JV6" s="195"/>
+      <c r="JW6" s="195"/>
+      <c r="JX6" s="195"/>
+      <c r="JY6" s="195"/>
+      <c r="JZ6" s="195"/>
+      <c r="KA6" s="195"/>
+      <c r="KB6" s="195"/>
+      <c r="KC6" s="195"/>
+      <c r="KD6" s="195"/>
+      <c r="KE6" s="195"/>
+      <c r="KF6" s="195"/>
+      <c r="KG6" s="195"/>
+      <c r="KH6" s="195"/>
+      <c r="KI6" s="195"/>
+      <c r="KJ6" s="195"/>
+      <c r="KK6" s="195"/>
+      <c r="KL6" s="195"/>
+      <c r="KM6" s="195"/>
+      <c r="KN6" s="195"/>
+      <c r="KO6" s="195"/>
+      <c r="KP6" s="195"/>
+      <c r="KQ6" s="195"/>
+      <c r="KR6" s="195"/>
+      <c r="KS6" s="196"/>
+      <c r="KT6" s="199">
         <v>11</v>
       </c>
-      <c r="KU6" s="199"/>
-      <c r="KV6" s="199"/>
-      <c r="KW6" s="199"/>
-      <c r="KX6" s="199"/>
-      <c r="KY6" s="199"/>
-      <c r="KZ6" s="199"/>
-      <c r="LA6" s="199"/>
-      <c r="LB6" s="199"/>
-      <c r="LC6" s="199"/>
-      <c r="LD6" s="199"/>
-      <c r="LE6" s="199"/>
-      <c r="LF6" s="199"/>
-      <c r="LG6" s="199"/>
-      <c r="LH6" s="199"/>
-      <c r="LI6" s="199"/>
-      <c r="LJ6" s="199"/>
-      <c r="LK6" s="199"/>
-      <c r="LL6" s="199"/>
-      <c r="LM6" s="199"/>
-      <c r="LN6" s="199"/>
-      <c r="LO6" s="199"/>
-      <c r="LP6" s="199"/>
-      <c r="LQ6" s="199"/>
-      <c r="LR6" s="199"/>
-      <c r="LS6" s="199"/>
-      <c r="LT6" s="199"/>
-      <c r="LU6" s="199"/>
-      <c r="LV6" s="199"/>
-      <c r="LW6" s="200"/>
-      <c r="LX6" s="194">
+      <c r="KU6" s="200"/>
+      <c r="KV6" s="200"/>
+      <c r="KW6" s="200"/>
+      <c r="KX6" s="200"/>
+      <c r="KY6" s="200"/>
+      <c r="KZ6" s="200"/>
+      <c r="LA6" s="200"/>
+      <c r="LB6" s="200"/>
+      <c r="LC6" s="200"/>
+      <c r="LD6" s="200"/>
+      <c r="LE6" s="200"/>
+      <c r="LF6" s="200"/>
+      <c r="LG6" s="200"/>
+      <c r="LH6" s="200"/>
+      <c r="LI6" s="200"/>
+      <c r="LJ6" s="200"/>
+      <c r="LK6" s="200"/>
+      <c r="LL6" s="200"/>
+      <c r="LM6" s="200"/>
+      <c r="LN6" s="200"/>
+      <c r="LO6" s="200"/>
+      <c r="LP6" s="200"/>
+      <c r="LQ6" s="200"/>
+      <c r="LR6" s="200"/>
+      <c r="LS6" s="200"/>
+      <c r="LT6" s="200"/>
+      <c r="LU6" s="200"/>
+      <c r="LV6" s="200"/>
+      <c r="LW6" s="201"/>
+      <c r="LX6" s="195">
         <v>12</v>
       </c>
-      <c r="LY6" s="194"/>
-      <c r="LZ6" s="194"/>
-      <c r="MA6" s="194"/>
-      <c r="MB6" s="194"/>
-      <c r="MC6" s="194"/>
-      <c r="MD6" s="194"/>
-      <c r="ME6" s="194"/>
-      <c r="MF6" s="194"/>
-      <c r="MG6" s="194"/>
-      <c r="MH6" s="194"/>
-      <c r="MI6" s="194"/>
-      <c r="MJ6" s="194"/>
-      <c r="MK6" s="194"/>
-      <c r="ML6" s="194"/>
-      <c r="MM6" s="194"/>
-      <c r="MN6" s="194"/>
-      <c r="MO6" s="194"/>
-      <c r="MP6" s="194"/>
-      <c r="MQ6" s="194"/>
-      <c r="MR6" s="194"/>
-      <c r="MS6" s="194"/>
-      <c r="MT6" s="194"/>
-      <c r="MU6" s="194"/>
-      <c r="MV6" s="194"/>
-      <c r="MW6" s="194"/>
-      <c r="MX6" s="194"/>
-      <c r="MY6" s="194"/>
-      <c r="MZ6" s="194"/>
-      <c r="NA6" s="194"/>
-      <c r="NB6" s="195"/>
+      <c r="LY6" s="195"/>
+      <c r="LZ6" s="195"/>
+      <c r="MA6" s="195"/>
+      <c r="MB6" s="195"/>
+      <c r="MC6" s="195"/>
+      <c r="MD6" s="195"/>
+      <c r="ME6" s="195"/>
+      <c r="MF6" s="195"/>
+      <c r="MG6" s="195"/>
+      <c r="MH6" s="195"/>
+      <c r="MI6" s="195"/>
+      <c r="MJ6" s="195"/>
+      <c r="MK6" s="195"/>
+      <c r="ML6" s="195"/>
+      <c r="MM6" s="195"/>
+      <c r="MN6" s="195"/>
+      <c r="MO6" s="195"/>
+      <c r="MP6" s="195"/>
+      <c r="MQ6" s="195"/>
+      <c r="MR6" s="195"/>
+      <c r="MS6" s="195"/>
+      <c r="MT6" s="195"/>
+      <c r="MU6" s="195"/>
+      <c r="MV6" s="195"/>
+      <c r="MW6" s="195"/>
+      <c r="MX6" s="195"/>
+      <c r="MY6" s="195"/>
+      <c r="MZ6" s="195"/>
+      <c r="NA6" s="195"/>
+      <c r="NB6" s="196"/>
     </row>
     <row r="7" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -17748,7 +17748,7 @@
       </c>
     </row>
     <row r="8" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="201" t="s">
+      <c r="A8" s="202" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="34"/>
@@ -18136,7 +18136,7 @@
       <c r="NB8" s="141"/>
     </row>
     <row r="9" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="201"/>
+      <c r="A9" s="202"/>
       <c r="B9" s="29"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -18516,7 +18516,7 @@
       <c r="NB9" s="32"/>
     </row>
     <row r="10" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="201"/>
+      <c r="A10" s="202"/>
       <c r="B10" s="29"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
@@ -18896,7 +18896,7 @@
       <c r="NB10" s="32"/>
     </row>
     <row r="11" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="201"/>
+      <c r="A11" s="202"/>
       <c r="B11" s="29"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
@@ -19272,7 +19272,7 @@
       <c r="NB11" s="32"/>
     </row>
     <row r="12" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="201"/>
+      <c r="A12" s="202"/>
       <c r="B12" s="29"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
@@ -19646,7 +19646,7 @@
       <c r="NB12" s="32"/>
     </row>
     <row r="13" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="201"/>
+      <c r="A13" s="202"/>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -20016,7 +20016,7 @@
       <c r="NB13" s="32"/>
     </row>
     <row r="14" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="201"/>
+      <c r="A14" s="202"/>
       <c r="B14" s="50"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51"/>
@@ -20386,7 +20386,7 @@
       <c r="NB14" s="65"/>
     </row>
     <row r="15" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="201" t="s">
+      <c r="A15" s="202" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="42"/>
@@ -20770,7 +20770,7 @@
       <c r="NB15" s="84"/>
     </row>
     <row r="16" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="201"/>
+      <c r="A16" s="202"/>
       <c r="B16" s="24"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -21150,7 +21150,7 @@
       <c r="NB16" s="25"/>
     </row>
     <row r="17" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="201"/>
+      <c r="A17" s="202"/>
       <c r="B17" s="24"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -21526,7 +21526,7 @@
       <c r="NB17" s="25"/>
     </row>
     <row r="18" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="201"/>
+      <c r="A18" s="202"/>
       <c r="B18" s="24"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -21902,7 +21902,7 @@
       <c r="NB18" s="25"/>
     </row>
     <row r="19" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="201"/>
+      <c r="A19" s="202"/>
       <c r="B19" s="26"/>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
@@ -22272,7 +22272,7 @@
       <c r="NB19" s="74"/>
     </row>
     <row r="20" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="201" t="s">
+      <c r="A20" s="202" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="75"/>
@@ -22650,7 +22650,7 @@
       <c r="NB20" s="84"/>
     </row>
     <row r="21" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="201"/>
+      <c r="A21" s="202"/>
       <c r="B21" s="24"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -23024,7 +23024,7 @@
       <c r="NB21" s="25"/>
     </row>
     <row r="22" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="201"/>
+      <c r="A22" s="202"/>
       <c r="B22" s="24"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -23396,7 +23396,7 @@
       <c r="NB22" s="25"/>
     </row>
     <row r="23" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="201"/>
+      <c r="A23" s="202"/>
       <c r="B23" s="24"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -23772,7 +23772,7 @@
       <c r="NB23" s="25"/>
     </row>
     <row r="24" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="201"/>
+      <c r="A24" s="202"/>
       <c r="B24" s="91"/>
       <c r="C24" s="92"/>
       <c r="D24" s="92"/>
@@ -24140,7 +24140,7 @@
       <c r="NB24" s="74"/>
     </row>
     <row r="25" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="202" t="s">
+      <c r="A25" s="203" t="s">
         <v>62</v>
       </c>
       <c r="B25" s="75"/>
@@ -24516,7 +24516,7 @@
       <c r="NB25" s="84"/>
     </row>
     <row r="26" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="201"/>
+      <c r="A26" s="202"/>
       <c r="B26" s="24"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -24888,7 +24888,7 @@
       <c r="NB26" s="25"/>
     </row>
     <row r="27" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="201"/>
+      <c r="A27" s="202"/>
       <c r="B27" s="24"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
@@ -25262,7 +25262,7 @@
       <c r="NB27" s="25"/>
     </row>
     <row r="28" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="201"/>
+      <c r="A28" s="202"/>
       <c r="B28" s="24"/>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
@@ -25634,7 +25634,7 @@
       <c r="NB28" s="25"/>
     </row>
     <row r="29" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="201"/>
+      <c r="A29" s="202"/>
       <c r="B29" s="85"/>
       <c r="C29" s="71"/>
       <c r="D29" s="71"/>
@@ -26004,7 +26004,7 @@
       <c r="NB29" s="74"/>
     </row>
     <row r="30" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="202" t="s">
+      <c r="A30" s="203" t="s">
         <v>63</v>
       </c>
       <c r="B30" s="75"/>
@@ -26376,7 +26376,7 @@
       <c r="NB30" s="84"/>
     </row>
     <row r="31" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="201"/>
+      <c r="A31" s="202"/>
       <c r="B31" s="24"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -26750,7 +26750,7 @@
       <c r="NB31" s="25"/>
     </row>
     <row r="32" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="201"/>
+      <c r="A32" s="202"/>
       <c r="B32" s="24"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
@@ -27124,7 +27124,7 @@
       <c r="NB32" s="25"/>
     </row>
     <row r="33" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="201"/>
+      <c r="A33" s="202"/>
       <c r="B33" s="24"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
@@ -27494,7 +27494,7 @@
       <c r="NB33" s="25"/>
     </row>
     <row r="34" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="201"/>
+      <c r="A34" s="202"/>
       <c r="B34" s="85"/>
       <c r="C34" s="71"/>
       <c r="D34" s="71"/>
@@ -27862,7 +27862,7 @@
       <c r="NB34" s="74"/>
     </row>
     <row r="35" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="201" t="s">
+      <c r="A35" s="202" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="42"/>
@@ -28244,7 +28244,7 @@
       <c r="NB35" s="47"/>
     </row>
     <row r="36" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="201"/>
+      <c r="A36" s="202"/>
       <c r="B36" s="24"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
@@ -28616,7 +28616,7 @@
       <c r="NB36" s="25"/>
     </row>
     <row r="37" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="201"/>
+      <c r="A37" s="202"/>
       <c r="B37" s="24"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -28994,7 +28994,7 @@
       <c r="NB37" s="25"/>
     </row>
     <row r="38" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="201"/>
+      <c r="A38" s="202"/>
       <c r="B38" s="24"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
@@ -29364,7 +29364,7 @@
       <c r="NB38" s="25"/>
     </row>
     <row r="39" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="201"/>
+      <c r="A39" s="202"/>
       <c r="B39" s="85"/>
       <c r="C39" s="71"/>
       <c r="D39" s="71"/>
@@ -29736,7 +29736,7 @@
       <c r="NB39" s="74"/>
     </row>
     <row r="40" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="201" t="s">
+      <c r="A40" s="202" t="s">
         <v>23</v>
       </c>
       <c r="B40" s="75"/>
@@ -30114,7 +30114,7 @@
       <c r="NB40" s="84"/>
     </row>
     <row r="41" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="201"/>
+      <c r="A41" s="202"/>
       <c r="B41" s="24"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
@@ -30488,7 +30488,7 @@
       <c r="NB41" s="25"/>
     </row>
     <row r="42" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="201"/>
+      <c r="A42" s="202"/>
       <c r="B42" s="24"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -30860,7 +30860,7 @@
       <c r="NB42" s="25"/>
     </row>
     <row r="43" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="201"/>
+      <c r="A43" s="202"/>
       <c r="B43" s="24"/>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
@@ -31230,7 +31230,7 @@
       <c r="NB43" s="25"/>
     </row>
     <row r="44" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="201"/>
+      <c r="A44" s="202"/>
       <c r="B44" s="85"/>
       <c r="C44" s="71"/>
       <c r="D44" s="71"/>
@@ -31598,7 +31598,7 @@
       <c r="NB44" s="74"/>
     </row>
     <row r="45" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="201" t="s">
+      <c r="A45" s="202" t="s">
         <v>22</v>
       </c>
       <c r="B45" s="75"/>
@@ -31978,7 +31978,7 @@
       <c r="NB45" s="84"/>
     </row>
     <row r="46" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="201"/>
+      <c r="A46" s="202"/>
       <c r="B46" s="24"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
@@ -32348,7 +32348,7 @@
       <c r="NB46" s="25"/>
     </row>
     <row r="47" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="201"/>
+      <c r="A47" s="202"/>
       <c r="B47" s="24"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
@@ -32724,7 +32724,7 @@
       <c r="NB47" s="25"/>
     </row>
     <row r="48" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="201"/>
+      <c r="A48" s="202"/>
       <c r="B48" s="24"/>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -33094,7 +33094,7 @@
       <c r="NB48" s="25"/>
     </row>
     <row r="49" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="201"/>
+      <c r="A49" s="202"/>
       <c r="B49" s="85"/>
       <c r="C49" s="71"/>
       <c r="D49" s="71"/>
@@ -33468,7 +33468,7 @@
       <c r="NB49" s="74"/>
     </row>
     <row r="50" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="201" t="s">
+      <c r="A50" s="202" t="s">
         <v>24</v>
       </c>
       <c r="B50" s="75"/>
@@ -33850,7 +33850,7 @@
       <c r="NB50" s="84"/>
     </row>
     <row r="51" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="201"/>
+      <c r="A51" s="202"/>
       <c r="B51" s="24"/>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
@@ -34228,7 +34228,7 @@
       <c r="NB51" s="25"/>
     </row>
     <row r="52" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="201"/>
+      <c r="A52" s="202"/>
       <c r="B52" s="24"/>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
@@ -34600,7 +34600,7 @@
       <c r="NB52" s="25"/>
     </row>
     <row r="53" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="201"/>
+      <c r="A53" s="202"/>
       <c r="B53" s="24"/>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
@@ -34970,7 +34970,7 @@
       <c r="NB53" s="25"/>
     </row>
     <row r="54" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="201"/>
+      <c r="A54" s="202"/>
       <c r="B54" s="85"/>
       <c r="C54" s="71"/>
       <c r="D54" s="71"/>
@@ -35356,6 +35356,11 @@
     <row r="71" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="GA6:HE6"/>
+    <mergeCell ref="HF6:IJ6"/>
+    <mergeCell ref="IK6:JN6"/>
+    <mergeCell ref="JO6:KS6"/>
+    <mergeCell ref="KT6:LW6"/>
     <mergeCell ref="LX6:NB6"/>
     <mergeCell ref="A50:A54"/>
     <mergeCell ref="A15:A19"/>
@@ -35372,11 +35377,6 @@
     <mergeCell ref="BI6:CM6"/>
     <mergeCell ref="CN6:DQ6"/>
     <mergeCell ref="DR6:EV6"/>
-    <mergeCell ref="GA6:HE6"/>
-    <mergeCell ref="HF6:IJ6"/>
-    <mergeCell ref="IK6:JN6"/>
-    <mergeCell ref="JO6:KS6"/>
-    <mergeCell ref="KT6:LW6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35429,395 +35429,395 @@
     </row>
     <row r="6" spans="1:366" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="197">
+      <c r="B6" s="198">
         <v>1</v>
       </c>
-      <c r="C6" s="194"/>
-      <c r="D6" s="194"/>
-      <c r="E6" s="194"/>
-      <c r="F6" s="194"/>
-      <c r="G6" s="194"/>
-      <c r="H6" s="194"/>
-      <c r="I6" s="194"/>
-      <c r="J6" s="194"/>
-      <c r="K6" s="194"/>
-      <c r="L6" s="194"/>
-      <c r="M6" s="194"/>
-      <c r="N6" s="194"/>
-      <c r="O6" s="194"/>
-      <c r="P6" s="194"/>
-      <c r="Q6" s="194"/>
-      <c r="R6" s="194"/>
-      <c r="S6" s="194"/>
-      <c r="T6" s="194"/>
-      <c r="U6" s="194"/>
-      <c r="V6" s="194"/>
-      <c r="W6" s="194"/>
-      <c r="X6" s="194"/>
-      <c r="Y6" s="194"/>
-      <c r="Z6" s="194"/>
-      <c r="AA6" s="194"/>
-      <c r="AB6" s="194"/>
-      <c r="AC6" s="194"/>
-      <c r="AD6" s="194"/>
-      <c r="AE6" s="194"/>
-      <c r="AF6" s="194"/>
-      <c r="AG6" s="197">
+      <c r="C6" s="195"/>
+      <c r="D6" s="195"/>
+      <c r="E6" s="195"/>
+      <c r="F6" s="195"/>
+      <c r="G6" s="195"/>
+      <c r="H6" s="195"/>
+      <c r="I6" s="195"/>
+      <c r="J6" s="195"/>
+      <c r="K6" s="195"/>
+      <c r="L6" s="195"/>
+      <c r="M6" s="195"/>
+      <c r="N6" s="195"/>
+      <c r="O6" s="195"/>
+      <c r="P6" s="195"/>
+      <c r="Q6" s="195"/>
+      <c r="R6" s="195"/>
+      <c r="S6" s="195"/>
+      <c r="T6" s="195"/>
+      <c r="U6" s="195"/>
+      <c r="V6" s="195"/>
+      <c r="W6" s="195"/>
+      <c r="X6" s="195"/>
+      <c r="Y6" s="195"/>
+      <c r="Z6" s="195"/>
+      <c r="AA6" s="195"/>
+      <c r="AB6" s="195"/>
+      <c r="AC6" s="195"/>
+      <c r="AD6" s="195"/>
+      <c r="AE6" s="195"/>
+      <c r="AF6" s="195"/>
+      <c r="AG6" s="198">
         <v>2</v>
       </c>
-      <c r="AH6" s="194"/>
-      <c r="AI6" s="194"/>
-      <c r="AJ6" s="194"/>
-      <c r="AK6" s="194"/>
-      <c r="AL6" s="194"/>
-      <c r="AM6" s="194"/>
-      <c r="AN6" s="194"/>
-      <c r="AO6" s="194"/>
-      <c r="AP6" s="194"/>
-      <c r="AQ6" s="194"/>
-      <c r="AR6" s="194"/>
-      <c r="AS6" s="194"/>
-      <c r="AT6" s="194"/>
-      <c r="AU6" s="194"/>
-      <c r="AV6" s="194"/>
-      <c r="AW6" s="194"/>
-      <c r="AX6" s="194"/>
-      <c r="AY6" s="194"/>
-      <c r="AZ6" s="194"/>
-      <c r="BA6" s="194"/>
-      <c r="BB6" s="194"/>
-      <c r="BC6" s="194"/>
-      <c r="BD6" s="194"/>
-      <c r="BE6" s="194"/>
-      <c r="BF6" s="194"/>
-      <c r="BG6" s="194"/>
-      <c r="BH6" s="195"/>
-      <c r="BI6" s="194">
+      <c r="AH6" s="195"/>
+      <c r="AI6" s="195"/>
+      <c r="AJ6" s="195"/>
+      <c r="AK6" s="195"/>
+      <c r="AL6" s="195"/>
+      <c r="AM6" s="195"/>
+      <c r="AN6" s="195"/>
+      <c r="AO6" s="195"/>
+      <c r="AP6" s="195"/>
+      <c r="AQ6" s="195"/>
+      <c r="AR6" s="195"/>
+      <c r="AS6" s="195"/>
+      <c r="AT6" s="195"/>
+      <c r="AU6" s="195"/>
+      <c r="AV6" s="195"/>
+      <c r="AW6" s="195"/>
+      <c r="AX6" s="195"/>
+      <c r="AY6" s="195"/>
+      <c r="AZ6" s="195"/>
+      <c r="BA6" s="195"/>
+      <c r="BB6" s="195"/>
+      <c r="BC6" s="195"/>
+      <c r="BD6" s="195"/>
+      <c r="BE6" s="195"/>
+      <c r="BF6" s="195"/>
+      <c r="BG6" s="195"/>
+      <c r="BH6" s="196"/>
+      <c r="BI6" s="195">
         <v>3</v>
       </c>
-      <c r="BJ6" s="194"/>
-      <c r="BK6" s="194"/>
-      <c r="BL6" s="194"/>
-      <c r="BM6" s="194"/>
-      <c r="BN6" s="194"/>
-      <c r="BO6" s="194"/>
-      <c r="BP6" s="194"/>
-      <c r="BQ6" s="194"/>
-      <c r="BR6" s="194"/>
-      <c r="BS6" s="194"/>
-      <c r="BT6" s="194"/>
-      <c r="BU6" s="194"/>
-      <c r="BV6" s="194"/>
-      <c r="BW6" s="194"/>
-      <c r="BX6" s="194"/>
-      <c r="BY6" s="194"/>
-      <c r="BZ6" s="194"/>
-      <c r="CA6" s="194"/>
-      <c r="CB6" s="194"/>
-      <c r="CC6" s="194"/>
-      <c r="CD6" s="194"/>
-      <c r="CE6" s="194"/>
-      <c r="CF6" s="194"/>
-      <c r="CG6" s="194"/>
-      <c r="CH6" s="194"/>
-      <c r="CI6" s="194"/>
-      <c r="CJ6" s="194"/>
-      <c r="CK6" s="194"/>
-      <c r="CL6" s="194"/>
-      <c r="CM6" s="194"/>
-      <c r="CN6" s="198">
+      <c r="BJ6" s="195"/>
+      <c r="BK6" s="195"/>
+      <c r="BL6" s="195"/>
+      <c r="BM6" s="195"/>
+      <c r="BN6" s="195"/>
+      <c r="BO6" s="195"/>
+      <c r="BP6" s="195"/>
+      <c r="BQ6" s="195"/>
+      <c r="BR6" s="195"/>
+      <c r="BS6" s="195"/>
+      <c r="BT6" s="195"/>
+      <c r="BU6" s="195"/>
+      <c r="BV6" s="195"/>
+      <c r="BW6" s="195"/>
+      <c r="BX6" s="195"/>
+      <c r="BY6" s="195"/>
+      <c r="BZ6" s="195"/>
+      <c r="CA6" s="195"/>
+      <c r="CB6" s="195"/>
+      <c r="CC6" s="195"/>
+      <c r="CD6" s="195"/>
+      <c r="CE6" s="195"/>
+      <c r="CF6" s="195"/>
+      <c r="CG6" s="195"/>
+      <c r="CH6" s="195"/>
+      <c r="CI6" s="195"/>
+      <c r="CJ6" s="195"/>
+      <c r="CK6" s="195"/>
+      <c r="CL6" s="195"/>
+      <c r="CM6" s="195"/>
+      <c r="CN6" s="199">
         <v>4</v>
       </c>
-      <c r="CO6" s="199"/>
-      <c r="CP6" s="199"/>
-      <c r="CQ6" s="199"/>
-      <c r="CR6" s="199"/>
-      <c r="CS6" s="199"/>
-      <c r="CT6" s="199"/>
-      <c r="CU6" s="199"/>
-      <c r="CV6" s="199"/>
-      <c r="CW6" s="199"/>
-      <c r="CX6" s="199"/>
-      <c r="CY6" s="199"/>
-      <c r="CZ6" s="199"/>
-      <c r="DA6" s="199"/>
-      <c r="DB6" s="199"/>
-      <c r="DC6" s="199"/>
-      <c r="DD6" s="199"/>
-      <c r="DE6" s="199"/>
-      <c r="DF6" s="199"/>
-      <c r="DG6" s="199"/>
-      <c r="DH6" s="199"/>
-      <c r="DI6" s="199"/>
-      <c r="DJ6" s="199"/>
-      <c r="DK6" s="199"/>
-      <c r="DL6" s="199"/>
-      <c r="DM6" s="199"/>
-      <c r="DN6" s="199"/>
-      <c r="DO6" s="199"/>
-      <c r="DP6" s="199"/>
-      <c r="DQ6" s="200"/>
-      <c r="DR6" s="194">
+      <c r="CO6" s="200"/>
+      <c r="CP6" s="200"/>
+      <c r="CQ6" s="200"/>
+      <c r="CR6" s="200"/>
+      <c r="CS6" s="200"/>
+      <c r="CT6" s="200"/>
+      <c r="CU6" s="200"/>
+      <c r="CV6" s="200"/>
+      <c r="CW6" s="200"/>
+      <c r="CX6" s="200"/>
+      <c r="CY6" s="200"/>
+      <c r="CZ6" s="200"/>
+      <c r="DA6" s="200"/>
+      <c r="DB6" s="200"/>
+      <c r="DC6" s="200"/>
+      <c r="DD6" s="200"/>
+      <c r="DE6" s="200"/>
+      <c r="DF6" s="200"/>
+      <c r="DG6" s="200"/>
+      <c r="DH6" s="200"/>
+      <c r="DI6" s="200"/>
+      <c r="DJ6" s="200"/>
+      <c r="DK6" s="200"/>
+      <c r="DL6" s="200"/>
+      <c r="DM6" s="200"/>
+      <c r="DN6" s="200"/>
+      <c r="DO6" s="200"/>
+      <c r="DP6" s="200"/>
+      <c r="DQ6" s="201"/>
+      <c r="DR6" s="195">
         <v>5</v>
       </c>
-      <c r="DS6" s="194"/>
-      <c r="DT6" s="194"/>
-      <c r="DU6" s="194"/>
-      <c r="DV6" s="194"/>
-      <c r="DW6" s="194"/>
-      <c r="DX6" s="194"/>
-      <c r="DY6" s="194"/>
-      <c r="DZ6" s="194"/>
-      <c r="EA6" s="194"/>
-      <c r="EB6" s="194"/>
-      <c r="EC6" s="194"/>
-      <c r="ED6" s="194"/>
-      <c r="EE6" s="194"/>
-      <c r="EF6" s="194"/>
-      <c r="EG6" s="194"/>
-      <c r="EH6" s="194"/>
-      <c r="EI6" s="194"/>
-      <c r="EJ6" s="194"/>
-      <c r="EK6" s="194"/>
-      <c r="EL6" s="194"/>
-      <c r="EM6" s="194"/>
-      <c r="EN6" s="194"/>
-      <c r="EO6" s="194"/>
-      <c r="EP6" s="194"/>
-      <c r="EQ6" s="194"/>
-      <c r="ER6" s="194"/>
-      <c r="ES6" s="194"/>
-      <c r="ET6" s="194"/>
-      <c r="EU6" s="194"/>
-      <c r="EV6" s="195"/>
-      <c r="EW6" s="198">
+      <c r="DS6" s="195"/>
+      <c r="DT6" s="195"/>
+      <c r="DU6" s="195"/>
+      <c r="DV6" s="195"/>
+      <c r="DW6" s="195"/>
+      <c r="DX6" s="195"/>
+      <c r="DY6" s="195"/>
+      <c r="DZ6" s="195"/>
+      <c r="EA6" s="195"/>
+      <c r="EB6" s="195"/>
+      <c r="EC6" s="195"/>
+      <c r="ED6" s="195"/>
+      <c r="EE6" s="195"/>
+      <c r="EF6" s="195"/>
+      <c r="EG6" s="195"/>
+      <c r="EH6" s="195"/>
+      <c r="EI6" s="195"/>
+      <c r="EJ6" s="195"/>
+      <c r="EK6" s="195"/>
+      <c r="EL6" s="195"/>
+      <c r="EM6" s="195"/>
+      <c r="EN6" s="195"/>
+      <c r="EO6" s="195"/>
+      <c r="EP6" s="195"/>
+      <c r="EQ6" s="195"/>
+      <c r="ER6" s="195"/>
+      <c r="ES6" s="195"/>
+      <c r="ET6" s="195"/>
+      <c r="EU6" s="195"/>
+      <c r="EV6" s="196"/>
+      <c r="EW6" s="199">
         <v>6</v>
       </c>
-      <c r="EX6" s="199"/>
-      <c r="EY6" s="199"/>
-      <c r="EZ6" s="199"/>
-      <c r="FA6" s="199"/>
-      <c r="FB6" s="199"/>
-      <c r="FC6" s="199"/>
-      <c r="FD6" s="199"/>
-      <c r="FE6" s="199"/>
-      <c r="FF6" s="199"/>
-      <c r="FG6" s="199"/>
-      <c r="FH6" s="199"/>
-      <c r="FI6" s="199"/>
-      <c r="FJ6" s="199"/>
-      <c r="FK6" s="199"/>
-      <c r="FL6" s="199"/>
-      <c r="FM6" s="199"/>
-      <c r="FN6" s="199"/>
-      <c r="FO6" s="199"/>
-      <c r="FP6" s="199"/>
-      <c r="FQ6" s="199"/>
-      <c r="FR6" s="199"/>
-      <c r="FS6" s="199"/>
-      <c r="FT6" s="199"/>
-      <c r="FU6" s="199"/>
-      <c r="FV6" s="199"/>
-      <c r="FW6" s="199"/>
-      <c r="FX6" s="199"/>
-      <c r="FY6" s="199"/>
-      <c r="FZ6" s="200"/>
-      <c r="GA6" s="194">
+      <c r="EX6" s="200"/>
+      <c r="EY6" s="200"/>
+      <c r="EZ6" s="200"/>
+      <c r="FA6" s="200"/>
+      <c r="FB6" s="200"/>
+      <c r="FC6" s="200"/>
+      <c r="FD6" s="200"/>
+      <c r="FE6" s="200"/>
+      <c r="FF6" s="200"/>
+      <c r="FG6" s="200"/>
+      <c r="FH6" s="200"/>
+      <c r="FI6" s="200"/>
+      <c r="FJ6" s="200"/>
+      <c r="FK6" s="200"/>
+      <c r="FL6" s="200"/>
+      <c r="FM6" s="200"/>
+      <c r="FN6" s="200"/>
+      <c r="FO6" s="200"/>
+      <c r="FP6" s="200"/>
+      <c r="FQ6" s="200"/>
+      <c r="FR6" s="200"/>
+      <c r="FS6" s="200"/>
+      <c r="FT6" s="200"/>
+      <c r="FU6" s="200"/>
+      <c r="FV6" s="200"/>
+      <c r="FW6" s="200"/>
+      <c r="FX6" s="200"/>
+      <c r="FY6" s="200"/>
+      <c r="FZ6" s="201"/>
+      <c r="GA6" s="195">
         <v>7</v>
       </c>
-      <c r="GB6" s="194"/>
-      <c r="GC6" s="194"/>
-      <c r="GD6" s="194"/>
-      <c r="GE6" s="194"/>
-      <c r="GF6" s="194"/>
-      <c r="GG6" s="194"/>
-      <c r="GH6" s="194"/>
-      <c r="GI6" s="194"/>
-      <c r="GJ6" s="194"/>
-      <c r="GK6" s="194"/>
-      <c r="GL6" s="194"/>
-      <c r="GM6" s="194"/>
-      <c r="GN6" s="194"/>
-      <c r="GO6" s="194"/>
-      <c r="GP6" s="194"/>
-      <c r="GQ6" s="194"/>
-      <c r="GR6" s="194"/>
-      <c r="GS6" s="194"/>
-      <c r="GT6" s="194"/>
-      <c r="GU6" s="194"/>
-      <c r="GV6" s="194"/>
-      <c r="GW6" s="194"/>
-      <c r="GX6" s="194"/>
-      <c r="GY6" s="194"/>
-      <c r="GZ6" s="194"/>
-      <c r="HA6" s="194"/>
-      <c r="HB6" s="194"/>
-      <c r="HC6" s="194"/>
-      <c r="HD6" s="194"/>
-      <c r="HE6" s="195"/>
-      <c r="HF6" s="194">
+      <c r="GB6" s="195"/>
+      <c r="GC6" s="195"/>
+      <c r="GD6" s="195"/>
+      <c r="GE6" s="195"/>
+      <c r="GF6" s="195"/>
+      <c r="GG6" s="195"/>
+      <c r="GH6" s="195"/>
+      <c r="GI6" s="195"/>
+      <c r="GJ6" s="195"/>
+      <c r="GK6" s="195"/>
+      <c r="GL6" s="195"/>
+      <c r="GM6" s="195"/>
+      <c r="GN6" s="195"/>
+      <c r="GO6" s="195"/>
+      <c r="GP6" s="195"/>
+      <c r="GQ6" s="195"/>
+      <c r="GR6" s="195"/>
+      <c r="GS6" s="195"/>
+      <c r="GT6" s="195"/>
+      <c r="GU6" s="195"/>
+      <c r="GV6" s="195"/>
+      <c r="GW6" s="195"/>
+      <c r="GX6" s="195"/>
+      <c r="GY6" s="195"/>
+      <c r="GZ6" s="195"/>
+      <c r="HA6" s="195"/>
+      <c r="HB6" s="195"/>
+      <c r="HC6" s="195"/>
+      <c r="HD6" s="195"/>
+      <c r="HE6" s="196"/>
+      <c r="HF6" s="195">
         <v>8</v>
       </c>
-      <c r="HG6" s="194"/>
-      <c r="HH6" s="194"/>
-      <c r="HI6" s="194"/>
-      <c r="HJ6" s="194"/>
-      <c r="HK6" s="194"/>
-      <c r="HL6" s="194"/>
-      <c r="HM6" s="194"/>
-      <c r="HN6" s="194"/>
-      <c r="HO6" s="194"/>
-      <c r="HP6" s="194"/>
-      <c r="HQ6" s="194"/>
-      <c r="HR6" s="194"/>
-      <c r="HS6" s="194"/>
-      <c r="HT6" s="194"/>
-      <c r="HU6" s="194"/>
-      <c r="HV6" s="194"/>
-      <c r="HW6" s="194"/>
-      <c r="HX6" s="194"/>
-      <c r="HY6" s="194"/>
-      <c r="HZ6" s="194"/>
-      <c r="IA6" s="194"/>
-      <c r="IB6" s="194"/>
-      <c r="IC6" s="194"/>
-      <c r="ID6" s="194"/>
-      <c r="IE6" s="194"/>
-      <c r="IF6" s="194"/>
-      <c r="IG6" s="194"/>
-      <c r="IH6" s="194"/>
-      <c r="II6" s="194"/>
-      <c r="IJ6" s="195"/>
-      <c r="IK6" s="198">
+      <c r="HG6" s="195"/>
+      <c r="HH6" s="195"/>
+      <c r="HI6" s="195"/>
+      <c r="HJ6" s="195"/>
+      <c r="HK6" s="195"/>
+      <c r="HL6" s="195"/>
+      <c r="HM6" s="195"/>
+      <c r="HN6" s="195"/>
+      <c r="HO6" s="195"/>
+      <c r="HP6" s="195"/>
+      <c r="HQ6" s="195"/>
+      <c r="HR6" s="195"/>
+      <c r="HS6" s="195"/>
+      <c r="HT6" s="195"/>
+      <c r="HU6" s="195"/>
+      <c r="HV6" s="195"/>
+      <c r="HW6" s="195"/>
+      <c r="HX6" s="195"/>
+      <c r="HY6" s="195"/>
+      <c r="HZ6" s="195"/>
+      <c r="IA6" s="195"/>
+      <c r="IB6" s="195"/>
+      <c r="IC6" s="195"/>
+      <c r="ID6" s="195"/>
+      <c r="IE6" s="195"/>
+      <c r="IF6" s="195"/>
+      <c r="IG6" s="195"/>
+      <c r="IH6" s="195"/>
+      <c r="II6" s="195"/>
+      <c r="IJ6" s="196"/>
+      <c r="IK6" s="199">
         <v>9</v>
       </c>
-      <c r="IL6" s="199"/>
-      <c r="IM6" s="199"/>
-      <c r="IN6" s="199"/>
-      <c r="IO6" s="199"/>
-      <c r="IP6" s="199"/>
-      <c r="IQ6" s="199"/>
-      <c r="IR6" s="199"/>
-      <c r="IS6" s="199"/>
-      <c r="IT6" s="199"/>
-      <c r="IU6" s="199"/>
-      <c r="IV6" s="199"/>
-      <c r="IW6" s="199"/>
-      <c r="IX6" s="199"/>
-      <c r="IY6" s="199"/>
-      <c r="IZ6" s="199"/>
-      <c r="JA6" s="199"/>
-      <c r="JB6" s="199"/>
-      <c r="JC6" s="199"/>
-      <c r="JD6" s="199"/>
-      <c r="JE6" s="199"/>
-      <c r="JF6" s="199"/>
-      <c r="JG6" s="199"/>
-      <c r="JH6" s="199"/>
-      <c r="JI6" s="199"/>
-      <c r="JJ6" s="199"/>
-      <c r="JK6" s="199"/>
-      <c r="JL6" s="199"/>
-      <c r="JM6" s="199"/>
-      <c r="JN6" s="200"/>
-      <c r="JO6" s="194">
+      <c r="IL6" s="200"/>
+      <c r="IM6" s="200"/>
+      <c r="IN6" s="200"/>
+      <c r="IO6" s="200"/>
+      <c r="IP6" s="200"/>
+      <c r="IQ6" s="200"/>
+      <c r="IR6" s="200"/>
+      <c r="IS6" s="200"/>
+      <c r="IT6" s="200"/>
+      <c r="IU6" s="200"/>
+      <c r="IV6" s="200"/>
+      <c r="IW6" s="200"/>
+      <c r="IX6" s="200"/>
+      <c r="IY6" s="200"/>
+      <c r="IZ6" s="200"/>
+      <c r="JA6" s="200"/>
+      <c r="JB6" s="200"/>
+      <c r="JC6" s="200"/>
+      <c r="JD6" s="200"/>
+      <c r="JE6" s="200"/>
+      <c r="JF6" s="200"/>
+      <c r="JG6" s="200"/>
+      <c r="JH6" s="200"/>
+      <c r="JI6" s="200"/>
+      <c r="JJ6" s="200"/>
+      <c r="JK6" s="200"/>
+      <c r="JL6" s="200"/>
+      <c r="JM6" s="200"/>
+      <c r="JN6" s="201"/>
+      <c r="JO6" s="195">
         <v>10</v>
       </c>
-      <c r="JP6" s="194"/>
-      <c r="JQ6" s="194"/>
-      <c r="JR6" s="194"/>
-      <c r="JS6" s="194"/>
-      <c r="JT6" s="194"/>
-      <c r="JU6" s="194"/>
-      <c r="JV6" s="194"/>
-      <c r="JW6" s="194"/>
-      <c r="JX6" s="194"/>
-      <c r="JY6" s="194"/>
-      <c r="JZ6" s="194"/>
-      <c r="KA6" s="194"/>
-      <c r="KB6" s="194"/>
-      <c r="KC6" s="194"/>
-      <c r="KD6" s="194"/>
-      <c r="KE6" s="194"/>
-      <c r="KF6" s="194"/>
-      <c r="KG6" s="194"/>
-      <c r="KH6" s="194"/>
-      <c r="KI6" s="194"/>
-      <c r="KJ6" s="194"/>
-      <c r="KK6" s="194"/>
-      <c r="KL6" s="194"/>
-      <c r="KM6" s="194"/>
-      <c r="KN6" s="194"/>
-      <c r="KO6" s="194"/>
-      <c r="KP6" s="194"/>
-      <c r="KQ6" s="194"/>
-      <c r="KR6" s="194"/>
-      <c r="KS6" s="195"/>
-      <c r="KT6" s="198">
+      <c r="JP6" s="195"/>
+      <c r="JQ6" s="195"/>
+      <c r="JR6" s="195"/>
+      <c r="JS6" s="195"/>
+      <c r="JT6" s="195"/>
+      <c r="JU6" s="195"/>
+      <c r="JV6" s="195"/>
+      <c r="JW6" s="195"/>
+      <c r="JX6" s="195"/>
+      <c r="JY6" s="195"/>
+      <c r="JZ6" s="195"/>
+      <c r="KA6" s="195"/>
+      <c r="KB6" s="195"/>
+      <c r="KC6" s="195"/>
+      <c r="KD6" s="195"/>
+      <c r="KE6" s="195"/>
+      <c r="KF6" s="195"/>
+      <c r="KG6" s="195"/>
+      <c r="KH6" s="195"/>
+      <c r="KI6" s="195"/>
+      <c r="KJ6" s="195"/>
+      <c r="KK6" s="195"/>
+      <c r="KL6" s="195"/>
+      <c r="KM6" s="195"/>
+      <c r="KN6" s="195"/>
+      <c r="KO6" s="195"/>
+      <c r="KP6" s="195"/>
+      <c r="KQ6" s="195"/>
+      <c r="KR6" s="195"/>
+      <c r="KS6" s="196"/>
+      <c r="KT6" s="199">
         <v>11</v>
       </c>
-      <c r="KU6" s="199"/>
-      <c r="KV6" s="199"/>
-      <c r="KW6" s="199"/>
-      <c r="KX6" s="199"/>
-      <c r="KY6" s="199"/>
-      <c r="KZ6" s="199"/>
-      <c r="LA6" s="199"/>
-      <c r="LB6" s="199"/>
-      <c r="LC6" s="199"/>
-      <c r="LD6" s="199"/>
-      <c r="LE6" s="199"/>
-      <c r="LF6" s="199"/>
-      <c r="LG6" s="199"/>
-      <c r="LH6" s="199"/>
-      <c r="LI6" s="199"/>
-      <c r="LJ6" s="199"/>
-      <c r="LK6" s="199"/>
-      <c r="LL6" s="199"/>
-      <c r="LM6" s="199"/>
-      <c r="LN6" s="199"/>
-      <c r="LO6" s="199"/>
-      <c r="LP6" s="199"/>
-      <c r="LQ6" s="199"/>
-      <c r="LR6" s="199"/>
-      <c r="LS6" s="199"/>
-      <c r="LT6" s="199"/>
-      <c r="LU6" s="199"/>
-      <c r="LV6" s="199"/>
-      <c r="LW6" s="200"/>
-      <c r="LX6" s="194">
+      <c r="KU6" s="200"/>
+      <c r="KV6" s="200"/>
+      <c r="KW6" s="200"/>
+      <c r="KX6" s="200"/>
+      <c r="KY6" s="200"/>
+      <c r="KZ6" s="200"/>
+      <c r="LA6" s="200"/>
+      <c r="LB6" s="200"/>
+      <c r="LC6" s="200"/>
+      <c r="LD6" s="200"/>
+      <c r="LE6" s="200"/>
+      <c r="LF6" s="200"/>
+      <c r="LG6" s="200"/>
+      <c r="LH6" s="200"/>
+      <c r="LI6" s="200"/>
+      <c r="LJ6" s="200"/>
+      <c r="LK6" s="200"/>
+      <c r="LL6" s="200"/>
+      <c r="LM6" s="200"/>
+      <c r="LN6" s="200"/>
+      <c r="LO6" s="200"/>
+      <c r="LP6" s="200"/>
+      <c r="LQ6" s="200"/>
+      <c r="LR6" s="200"/>
+      <c r="LS6" s="200"/>
+      <c r="LT6" s="200"/>
+      <c r="LU6" s="200"/>
+      <c r="LV6" s="200"/>
+      <c r="LW6" s="201"/>
+      <c r="LX6" s="195">
         <v>12</v>
       </c>
-      <c r="LY6" s="194"/>
-      <c r="LZ6" s="194"/>
-      <c r="MA6" s="194"/>
-      <c r="MB6" s="194"/>
-      <c r="MC6" s="194"/>
-      <c r="MD6" s="194"/>
-      <c r="ME6" s="194"/>
-      <c r="MF6" s="194"/>
-      <c r="MG6" s="194"/>
-      <c r="MH6" s="194"/>
-      <c r="MI6" s="194"/>
-      <c r="MJ6" s="194"/>
-      <c r="MK6" s="194"/>
-      <c r="ML6" s="194"/>
-      <c r="MM6" s="194"/>
-      <c r="MN6" s="194"/>
-      <c r="MO6" s="194"/>
-      <c r="MP6" s="194"/>
-      <c r="MQ6" s="194"/>
-      <c r="MR6" s="194"/>
-      <c r="MS6" s="194"/>
-      <c r="MT6" s="194"/>
-      <c r="MU6" s="194"/>
-      <c r="MV6" s="194"/>
-      <c r="MW6" s="194"/>
-      <c r="MX6" s="194"/>
-      <c r="MY6" s="194"/>
-      <c r="MZ6" s="194"/>
-      <c r="NA6" s="194"/>
-      <c r="NB6" s="195"/>
+      <c r="LY6" s="195"/>
+      <c r="LZ6" s="195"/>
+      <c r="MA6" s="195"/>
+      <c r="MB6" s="195"/>
+      <c r="MC6" s="195"/>
+      <c r="MD6" s="195"/>
+      <c r="ME6" s="195"/>
+      <c r="MF6" s="195"/>
+      <c r="MG6" s="195"/>
+      <c r="MH6" s="195"/>
+      <c r="MI6" s="195"/>
+      <c r="MJ6" s="195"/>
+      <c r="MK6" s="195"/>
+      <c r="ML6" s="195"/>
+      <c r="MM6" s="195"/>
+      <c r="MN6" s="195"/>
+      <c r="MO6" s="195"/>
+      <c r="MP6" s="195"/>
+      <c r="MQ6" s="195"/>
+      <c r="MR6" s="195"/>
+      <c r="MS6" s="195"/>
+      <c r="MT6" s="195"/>
+      <c r="MU6" s="195"/>
+      <c r="MV6" s="195"/>
+      <c r="MW6" s="195"/>
+      <c r="MX6" s="195"/>
+      <c r="MY6" s="195"/>
+      <c r="MZ6" s="195"/>
+      <c r="NA6" s="195"/>
+      <c r="NB6" s="196"/>
     </row>
     <row r="7" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -36918,7 +36918,7 @@
       </c>
     </row>
     <row r="8" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="201" t="s">
+      <c r="A8" s="202" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="34"/>
@@ -37310,7 +37310,7 @@
       <c r="NB8" s="141"/>
     </row>
     <row r="9" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="201"/>
+      <c r="A9" s="202"/>
       <c r="B9" s="29"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -37690,7 +37690,7 @@
       <c r="NB9" s="32"/>
     </row>
     <row r="10" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="201"/>
+      <c r="A10" s="202"/>
       <c r="B10" s="29"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
@@ -37820,7 +37820,7 @@
       <c r="DL10" s="30"/>
       <c r="DM10" s="30"/>
       <c r="DN10" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="DO10" s="31"/>
       <c r="DP10" s="31"/>
@@ -38072,7 +38072,7 @@
       <c r="NB10" s="32"/>
     </row>
     <row r="11" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="201"/>
+      <c r="A11" s="202"/>
       <c r="B11" s="29"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
@@ -38448,7 +38448,7 @@
       <c r="NB11" s="32"/>
     </row>
     <row r="12" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="201"/>
+      <c r="A12" s="202"/>
       <c r="B12" s="29"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
@@ -38822,7 +38822,7 @@
       <c r="NB12" s="32"/>
     </row>
     <row r="13" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="201"/>
+      <c r="A13" s="202"/>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -39192,7 +39192,7 @@
       <c r="NB13" s="32"/>
     </row>
     <row r="14" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="201"/>
+      <c r="A14" s="202"/>
       <c r="B14" s="50"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51"/>
@@ -39562,7 +39562,7 @@
       <c r="NB14" s="65"/>
     </row>
     <row r="15" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="202" t="s">
+      <c r="A15" s="203" t="s">
         <v>62</v>
       </c>
       <c r="B15" s="75"/>
@@ -39684,7 +39684,7 @@
       <c r="DN15" s="76"/>
       <c r="DO15" s="77"/>
       <c r="DP15" s="80" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="DQ15" s="84"/>
       <c r="DR15" s="82"/>
@@ -39942,7 +39942,7 @@
       <c r="NB15" s="84"/>
     </row>
     <row r="16" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="201"/>
+      <c r="A16" s="202"/>
       <c r="B16" s="24"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -40064,7 +40064,7 @@
       <c r="DP16" s="14"/>
       <c r="DQ16" s="25"/>
       <c r="DR16" s="189" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="DS16" s="16"/>
       <c r="DT16" s="16"/>
@@ -40314,7 +40314,7 @@
       <c r="NB16" s="25"/>
     </row>
     <row r="17" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="201"/>
+      <c r="A17" s="202"/>
       <c r="B17" s="24"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -40682,7 +40682,7 @@
       <c r="NB17" s="25"/>
     </row>
     <row r="18" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="201"/>
+      <c r="A18" s="202"/>
       <c r="B18" s="24"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -41052,7 +41052,7 @@
       <c r="NB18" s="25"/>
     </row>
     <row r="19" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="201"/>
+      <c r="A19" s="202"/>
       <c r="B19" s="85"/>
       <c r="C19" s="71"/>
       <c r="D19" s="71"/>
@@ -41420,7 +41420,7 @@
       <c r="NB19" s="74"/>
     </row>
     <row r="20" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="201" t="s">
+      <c r="A20" s="202" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="42"/>
@@ -41804,7 +41804,7 @@
       <c r="NB20" s="84"/>
     </row>
     <row r="21" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="201"/>
+      <c r="A21" s="202"/>
       <c r="B21" s="24"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -42181,7 +42181,7 @@
       <c r="NB21" s="25"/>
     </row>
     <row r="22" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="201"/>
+      <c r="A22" s="202"/>
       <c r="B22" s="24"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -42559,7 +42559,7 @@
       <c r="NB22" s="25"/>
     </row>
     <row r="23" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="201"/>
+      <c r="A23" s="202"/>
       <c r="B23" s="24"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
@@ -42935,7 +42935,7 @@
       <c r="NB23" s="25"/>
     </row>
     <row r="24" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="201"/>
+      <c r="A24" s="202"/>
       <c r="B24" s="26"/>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
@@ -43305,7 +43305,7 @@
       <c r="NB24" s="74"/>
     </row>
     <row r="25" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="201" t="s">
+      <c r="A25" s="202" t="s">
         <v>17</v>
       </c>
       <c r="B25" s="75"/>
@@ -43685,7 +43685,7 @@
       <c r="NB25" s="84"/>
     </row>
     <row r="26" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="201"/>
+      <c r="A26" s="202"/>
       <c r="B26" s="24"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -44061,7 +44061,7 @@
       <c r="NB26" s="25"/>
     </row>
     <row r="27" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="201"/>
+      <c r="A27" s="202"/>
       <c r="B27" s="24"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
@@ -44433,7 +44433,7 @@
       <c r="NB27" s="25"/>
     </row>
     <row r="28" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="201"/>
+      <c r="A28" s="202"/>
       <c r="B28" s="24"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -44809,7 +44809,7 @@
       <c r="NB28" s="25"/>
     </row>
     <row r="29" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="201"/>
+      <c r="A29" s="202"/>
       <c r="B29" s="91"/>
       <c r="C29" s="92"/>
       <c r="D29" s="92"/>
@@ -45177,7 +45177,7 @@
       <c r="NB29" s="74"/>
     </row>
     <row r="30" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="202" t="s">
+      <c r="A30" s="203" t="s">
         <v>63</v>
       </c>
       <c r="B30" s="75"/>
@@ -45549,7 +45549,7 @@
       <c r="NB30" s="84"/>
     </row>
     <row r="31" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="201"/>
+      <c r="A31" s="202"/>
       <c r="B31" s="24"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -45923,7 +45923,7 @@
       <c r="NB31" s="25"/>
     </row>
     <row r="32" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="201"/>
+      <c r="A32" s="202"/>
       <c r="B32" s="24"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
@@ -46297,7 +46297,7 @@
       <c r="NB32" s="25"/>
     </row>
     <row r="33" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="201"/>
+      <c r="A33" s="202"/>
       <c r="B33" s="24"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
@@ -46667,7 +46667,7 @@
       <c r="NB33" s="25"/>
     </row>
     <row r="34" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="201"/>
+      <c r="A34" s="202"/>
       <c r="B34" s="85"/>
       <c r="C34" s="71"/>
       <c r="D34" s="71"/>
@@ -47035,7 +47035,7 @@
       <c r="NB34" s="74"/>
     </row>
     <row r="35" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="201" t="s">
+      <c r="A35" s="202" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="42"/>
@@ -47417,7 +47417,7 @@
       <c r="NB35" s="47"/>
     </row>
     <row r="36" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="201"/>
+      <c r="A36" s="202"/>
       <c r="B36" s="24"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
@@ -47789,7 +47789,7 @@
       <c r="NB36" s="25"/>
     </row>
     <row r="37" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="201"/>
+      <c r="A37" s="202"/>
       <c r="B37" s="24"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -48165,7 +48165,7 @@
       <c r="NB37" s="25"/>
     </row>
     <row r="38" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="201"/>
+      <c r="A38" s="202"/>
       <c r="B38" s="24"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
@@ -48539,7 +48539,7 @@
       <c r="NB38" s="25"/>
     </row>
     <row r="39" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="201"/>
+      <c r="A39" s="202"/>
       <c r="B39" s="85"/>
       <c r="C39" s="71"/>
       <c r="D39" s="71"/>
@@ -48911,7 +48911,7 @@
       <c r="NB39" s="74"/>
     </row>
     <row r="40" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="201" t="s">
+      <c r="A40" s="202" t="s">
         <v>23</v>
       </c>
       <c r="B40" s="75"/>
@@ -49289,7 +49289,7 @@
       <c r="NB40" s="84"/>
     </row>
     <row r="41" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="201"/>
+      <c r="A41" s="202"/>
       <c r="B41" s="24"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
@@ -49665,7 +49665,7 @@
       <c r="NB41" s="25"/>
     </row>
     <row r="42" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="201"/>
+      <c r="A42" s="202"/>
       <c r="B42" s="24"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -50035,7 +50035,7 @@
       <c r="NB42" s="25"/>
     </row>
     <row r="43" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="201"/>
+      <c r="A43" s="202"/>
       <c r="B43" s="24"/>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
@@ -50405,7 +50405,7 @@
       <c r="NB43" s="25"/>
     </row>
     <row r="44" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="201"/>
+      <c r="A44" s="202"/>
       <c r="B44" s="85"/>
       <c r="C44" s="71"/>
       <c r="D44" s="71"/>
@@ -50773,7 +50773,7 @@
       <c r="NB44" s="74"/>
     </row>
     <row r="45" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="201" t="s">
+      <c r="A45" s="202" t="s">
         <v>22</v>
       </c>
       <c r="B45" s="75"/>
@@ -51153,7 +51153,7 @@
       <c r="NB45" s="84"/>
     </row>
     <row r="46" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="201"/>
+      <c r="A46" s="202"/>
       <c r="B46" s="24"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
@@ -51523,7 +51523,7 @@
       <c r="NB46" s="25"/>
     </row>
     <row r="47" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="201"/>
+      <c r="A47" s="202"/>
       <c r="B47" s="24"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
@@ -51899,7 +51899,7 @@
       <c r="NB47" s="25"/>
     </row>
     <row r="48" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="201"/>
+      <c r="A48" s="202"/>
       <c r="B48" s="24"/>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -52269,7 +52269,7 @@
       <c r="NB48" s="25"/>
     </row>
     <row r="49" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="201"/>
+      <c r="A49" s="202"/>
       <c r="B49" s="85"/>
       <c r="C49" s="71"/>
       <c r="D49" s="71"/>
@@ -52643,7 +52643,7 @@
       <c r="NB49" s="74"/>
     </row>
     <row r="50" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="201" t="s">
+      <c r="A50" s="202" t="s">
         <v>24</v>
       </c>
       <c r="B50" s="75"/>
@@ -53025,7 +53025,7 @@
       <c r="NB50" s="84"/>
     </row>
     <row r="51" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="201"/>
+      <c r="A51" s="202"/>
       <c r="B51" s="24"/>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
@@ -53403,7 +53403,7 @@
       <c r="NB51" s="25"/>
     </row>
     <row r="52" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="201"/>
+      <c r="A52" s="202"/>
       <c r="B52" s="24"/>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
@@ -53775,7 +53775,7 @@
       <c r="NB52" s="25"/>
     </row>
     <row r="53" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="201"/>
+      <c r="A53" s="202"/>
       <c r="B53" s="24"/>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
@@ -54145,7 +54145,7 @@
       <c r="NB53" s="25"/>
     </row>
     <row r="54" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="201"/>
+      <c r="A54" s="202"/>
       <c r="B54" s="85"/>
       <c r="C54" s="71"/>
       <c r="D54" s="71"/>
@@ -54533,15 +54533,6 @@
     <row r="71" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="A45:A49"/>
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A30:A34"/>
-    <mergeCell ref="A35:A39"/>
     <mergeCell ref="LX6:NB6"/>
     <mergeCell ref="B6:AF6"/>
     <mergeCell ref="AG6:BH6"/>
@@ -54554,6 +54545,15 @@
     <mergeCell ref="IK6:JN6"/>
     <mergeCell ref="JO6:KS6"/>
     <mergeCell ref="KT6:LW6"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="A35:A39"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -54568,7 +54568,7 @@
   <dimension ref="B1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -54582,20 +54582,20 @@
   <sheetData>
     <row r="1" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="203" t="s">
+      <c r="B2" s="204" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="205" t="s">
+      <c r="C2" s="206" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="206"/>
-      <c r="E2" s="207" t="s">
+      <c r="D2" s="207"/>
+      <c r="E2" s="208" t="s">
         <v>127</v>
       </c>
-      <c r="F2" s="206"/>
+      <c r="F2" s="207"/>
     </row>
     <row r="3" spans="2:6" s="167" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="204"/>
+      <c r="B3" s="205"/>
       <c r="C3" s="174" t="s">
         <v>122</v>
       </c>
@@ -54640,7 +54640,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="188" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
@@ -54651,7 +54651,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="188" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
@@ -54671,48 +54671,48 @@
       <c r="B8" s="209">
         <v>43221</v>
       </c>
-      <c r="C8" s="208">
+      <c r="C8" s="190">
         <v>2</v>
       </c>
       <c r="D8" s="188" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E8" s="185">
         <v>4</v>
       </c>
       <c r="F8" s="184" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="210"/>
-      <c r="C9" s="208">
+      <c r="C9" s="190">
         <v>2</v>
       </c>
       <c r="D9" s="188" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E9" s="185"/>
       <c r="F9" s="184"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="210"/>
-      <c r="C10" s="208">
+      <c r="C10" s="190">
         <v>1</v>
       </c>
       <c r="D10" s="188" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E10" s="185"/>
       <c r="F10" s="184"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="211"/>
-      <c r="C11" s="208">
+      <c r="C11" s="190">
         <v>1</v>
       </c>
       <c r="D11" s="188" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E11" s="185"/>
       <c r="F11" s="184"/>
@@ -54725,13 +54725,13 @@
         <v>1</v>
       </c>
       <c r="D12" s="184" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E12" s="185">
         <v>4</v>
       </c>
       <c r="F12" s="184" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
@@ -54740,21 +54740,31 @@
         <v>0.5</v>
       </c>
       <c r="D13" s="184" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E13" s="185">
         <v>4</v>
       </c>
       <c r="F13" s="188" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="187"/>
-      <c r="C14" s="183"/>
-      <c r="D14" s="184"/>
-      <c r="E14" s="185"/>
-      <c r="F14" s="184"/>
+      <c r="B14" s="187">
+        <v>43223</v>
+      </c>
+      <c r="C14" s="183">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="184" t="s">
+        <v>139</v>
+      </c>
+      <c r="E14" s="185">
+        <v>4</v>
+      </c>
+      <c r="F14" s="188" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="187"/>

</xml_diff>

<commit_message>
[DOC]LF Gen work update
</commit_message>
<xml_diff>
--- a/Femto Project schedule V1.0.xlsx
+++ b/Femto Project schedule V1.0.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645" activeTab="2"/>
@@ -17,7 +17,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">'20180328'!$A$1:$ND$54</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'20180423'!$A$1:$HT$54</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="153">
   <si>
     <t>◇PCB설계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -888,6 +888,14 @@
   </si>
   <si>
     <t>◇JTAG PCB제작(5ea)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LF Gen Main PCB Layout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LF Gen Main Schematic design</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1948,6 +1956,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2011,7 +2020,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -8924,167 +8932,167 @@
     </row>
     <row r="6" spans="1:152" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="198">
+      <c r="B6" s="199">
         <v>1</v>
       </c>
-      <c r="C6" s="195"/>
-      <c r="D6" s="195"/>
-      <c r="E6" s="195"/>
-      <c r="F6" s="195"/>
-      <c r="G6" s="195"/>
-      <c r="H6" s="195"/>
-      <c r="I6" s="195"/>
-      <c r="J6" s="195"/>
-      <c r="K6" s="195"/>
-      <c r="L6" s="195"/>
-      <c r="M6" s="195"/>
-      <c r="N6" s="195"/>
-      <c r="O6" s="195"/>
-      <c r="P6" s="195"/>
-      <c r="Q6" s="195"/>
-      <c r="R6" s="195"/>
-      <c r="S6" s="195"/>
-      <c r="T6" s="195"/>
-      <c r="U6" s="195"/>
-      <c r="V6" s="195"/>
-      <c r="W6" s="195"/>
-      <c r="X6" s="195"/>
-      <c r="Y6" s="195"/>
-      <c r="Z6" s="195"/>
-      <c r="AA6" s="195"/>
-      <c r="AB6" s="195"/>
-      <c r="AC6" s="195"/>
-      <c r="AD6" s="195"/>
-      <c r="AE6" s="195"/>
-      <c r="AF6" s="195"/>
-      <c r="AG6" s="198">
+      <c r="C6" s="196"/>
+      <c r="D6" s="196"/>
+      <c r="E6" s="196"/>
+      <c r="F6" s="196"/>
+      <c r="G6" s="196"/>
+      <c r="H6" s="196"/>
+      <c r="I6" s="196"/>
+      <c r="J6" s="196"/>
+      <c r="K6" s="196"/>
+      <c r="L6" s="196"/>
+      <c r="M6" s="196"/>
+      <c r="N6" s="196"/>
+      <c r="O6" s="196"/>
+      <c r="P6" s="196"/>
+      <c r="Q6" s="196"/>
+      <c r="R6" s="196"/>
+      <c r="S6" s="196"/>
+      <c r="T6" s="196"/>
+      <c r="U6" s="196"/>
+      <c r="V6" s="196"/>
+      <c r="W6" s="196"/>
+      <c r="X6" s="196"/>
+      <c r="Y6" s="196"/>
+      <c r="Z6" s="196"/>
+      <c r="AA6" s="196"/>
+      <c r="AB6" s="196"/>
+      <c r="AC6" s="196"/>
+      <c r="AD6" s="196"/>
+      <c r="AE6" s="196"/>
+      <c r="AF6" s="196"/>
+      <c r="AG6" s="199">
         <v>2</v>
       </c>
-      <c r="AH6" s="195"/>
-      <c r="AI6" s="195"/>
-      <c r="AJ6" s="195"/>
-      <c r="AK6" s="195"/>
-      <c r="AL6" s="195"/>
-      <c r="AM6" s="195"/>
-      <c r="AN6" s="195"/>
-      <c r="AO6" s="195"/>
-      <c r="AP6" s="195"/>
-      <c r="AQ6" s="195"/>
-      <c r="AR6" s="195"/>
-      <c r="AS6" s="195"/>
-      <c r="AT6" s="195"/>
-      <c r="AU6" s="195"/>
-      <c r="AV6" s="195"/>
-      <c r="AW6" s="195"/>
-      <c r="AX6" s="195"/>
-      <c r="AY6" s="195"/>
-      <c r="AZ6" s="195"/>
-      <c r="BA6" s="195"/>
-      <c r="BB6" s="195"/>
-      <c r="BC6" s="195"/>
-      <c r="BD6" s="195"/>
-      <c r="BE6" s="195"/>
-      <c r="BF6" s="195"/>
-      <c r="BG6" s="195"/>
-      <c r="BH6" s="196"/>
-      <c r="BI6" s="195">
+      <c r="AH6" s="196"/>
+      <c r="AI6" s="196"/>
+      <c r="AJ6" s="196"/>
+      <c r="AK6" s="196"/>
+      <c r="AL6" s="196"/>
+      <c r="AM6" s="196"/>
+      <c r="AN6" s="196"/>
+      <c r="AO6" s="196"/>
+      <c r="AP6" s="196"/>
+      <c r="AQ6" s="196"/>
+      <c r="AR6" s="196"/>
+      <c r="AS6" s="196"/>
+      <c r="AT6" s="196"/>
+      <c r="AU6" s="196"/>
+      <c r="AV6" s="196"/>
+      <c r="AW6" s="196"/>
+      <c r="AX6" s="196"/>
+      <c r="AY6" s="196"/>
+      <c r="AZ6" s="196"/>
+      <c r="BA6" s="196"/>
+      <c r="BB6" s="196"/>
+      <c r="BC6" s="196"/>
+      <c r="BD6" s="196"/>
+      <c r="BE6" s="196"/>
+      <c r="BF6" s="196"/>
+      <c r="BG6" s="196"/>
+      <c r="BH6" s="197"/>
+      <c r="BI6" s="196">
         <v>3</v>
       </c>
-      <c r="BJ6" s="195"/>
-      <c r="BK6" s="195"/>
-      <c r="BL6" s="195"/>
-      <c r="BM6" s="195"/>
-      <c r="BN6" s="195"/>
-      <c r="BO6" s="195"/>
-      <c r="BP6" s="195"/>
-      <c r="BQ6" s="195"/>
-      <c r="BR6" s="195"/>
-      <c r="BS6" s="195"/>
-      <c r="BT6" s="195"/>
-      <c r="BU6" s="195"/>
-      <c r="BV6" s="195"/>
-      <c r="BW6" s="195"/>
-      <c r="BX6" s="195"/>
-      <c r="BY6" s="195"/>
-      <c r="BZ6" s="195"/>
-      <c r="CA6" s="195"/>
-      <c r="CB6" s="195"/>
-      <c r="CC6" s="195"/>
-      <c r="CD6" s="195"/>
-      <c r="CE6" s="195"/>
-      <c r="CF6" s="195"/>
-      <c r="CG6" s="195"/>
-      <c r="CH6" s="195"/>
-      <c r="CI6" s="195"/>
-      <c r="CJ6" s="195"/>
-      <c r="CK6" s="195"/>
-      <c r="CL6" s="195"/>
-      <c r="CM6" s="195"/>
-      <c r="CN6" s="199">
+      <c r="BJ6" s="196"/>
+      <c r="BK6" s="196"/>
+      <c r="BL6" s="196"/>
+      <c r="BM6" s="196"/>
+      <c r="BN6" s="196"/>
+      <c r="BO6" s="196"/>
+      <c r="BP6" s="196"/>
+      <c r="BQ6" s="196"/>
+      <c r="BR6" s="196"/>
+      <c r="BS6" s="196"/>
+      <c r="BT6" s="196"/>
+      <c r="BU6" s="196"/>
+      <c r="BV6" s="196"/>
+      <c r="BW6" s="196"/>
+      <c r="BX6" s="196"/>
+      <c r="BY6" s="196"/>
+      <c r="BZ6" s="196"/>
+      <c r="CA6" s="196"/>
+      <c r="CB6" s="196"/>
+      <c r="CC6" s="196"/>
+      <c r="CD6" s="196"/>
+      <c r="CE6" s="196"/>
+      <c r="CF6" s="196"/>
+      <c r="CG6" s="196"/>
+      <c r="CH6" s="196"/>
+      <c r="CI6" s="196"/>
+      <c r="CJ6" s="196"/>
+      <c r="CK6" s="196"/>
+      <c r="CL6" s="196"/>
+      <c r="CM6" s="196"/>
+      <c r="CN6" s="200">
         <v>4</v>
       </c>
-      <c r="CO6" s="200"/>
-      <c r="CP6" s="200"/>
-      <c r="CQ6" s="200"/>
-      <c r="CR6" s="200"/>
-      <c r="CS6" s="200"/>
-      <c r="CT6" s="200"/>
-      <c r="CU6" s="200"/>
-      <c r="CV6" s="200"/>
-      <c r="CW6" s="200"/>
-      <c r="CX6" s="200"/>
-      <c r="CY6" s="200"/>
-      <c r="CZ6" s="200"/>
-      <c r="DA6" s="200"/>
-      <c r="DB6" s="200"/>
-      <c r="DC6" s="200"/>
-      <c r="DD6" s="200"/>
-      <c r="DE6" s="200"/>
-      <c r="DF6" s="200"/>
-      <c r="DG6" s="200"/>
-      <c r="DH6" s="200"/>
-      <c r="DI6" s="200"/>
-      <c r="DJ6" s="200"/>
-      <c r="DK6" s="200"/>
-      <c r="DL6" s="200"/>
-      <c r="DM6" s="200"/>
-      <c r="DN6" s="200"/>
-      <c r="DO6" s="200"/>
-      <c r="DP6" s="200"/>
-      <c r="DQ6" s="201"/>
-      <c r="DR6" s="195">
+      <c r="CO6" s="201"/>
+      <c r="CP6" s="201"/>
+      <c r="CQ6" s="201"/>
+      <c r="CR6" s="201"/>
+      <c r="CS6" s="201"/>
+      <c r="CT6" s="201"/>
+      <c r="CU6" s="201"/>
+      <c r="CV6" s="201"/>
+      <c r="CW6" s="201"/>
+      <c r="CX6" s="201"/>
+      <c r="CY6" s="201"/>
+      <c r="CZ6" s="201"/>
+      <c r="DA6" s="201"/>
+      <c r="DB6" s="201"/>
+      <c r="DC6" s="201"/>
+      <c r="DD6" s="201"/>
+      <c r="DE6" s="201"/>
+      <c r="DF6" s="201"/>
+      <c r="DG6" s="201"/>
+      <c r="DH6" s="201"/>
+      <c r="DI6" s="201"/>
+      <c r="DJ6" s="201"/>
+      <c r="DK6" s="201"/>
+      <c r="DL6" s="201"/>
+      <c r="DM6" s="201"/>
+      <c r="DN6" s="201"/>
+      <c r="DO6" s="201"/>
+      <c r="DP6" s="201"/>
+      <c r="DQ6" s="202"/>
+      <c r="DR6" s="196">
         <v>5</v>
       </c>
-      <c r="DS6" s="195"/>
-      <c r="DT6" s="195"/>
-      <c r="DU6" s="195"/>
-      <c r="DV6" s="195"/>
-      <c r="DW6" s="195"/>
-      <c r="DX6" s="195"/>
-      <c r="DY6" s="195"/>
-      <c r="DZ6" s="195"/>
-      <c r="EA6" s="195"/>
-      <c r="EB6" s="195"/>
-      <c r="EC6" s="195"/>
-      <c r="ED6" s="195"/>
-      <c r="EE6" s="195"/>
-      <c r="EF6" s="195"/>
-      <c r="EG6" s="195"/>
-      <c r="EH6" s="195"/>
-      <c r="EI6" s="195"/>
-      <c r="EJ6" s="195"/>
-      <c r="EK6" s="195"/>
-      <c r="EL6" s="195"/>
-      <c r="EM6" s="195"/>
-      <c r="EN6" s="195"/>
-      <c r="EO6" s="195"/>
-      <c r="EP6" s="195"/>
-      <c r="EQ6" s="195"/>
-      <c r="ER6" s="195"/>
-      <c r="ES6" s="195"/>
-      <c r="ET6" s="195"/>
-      <c r="EU6" s="195"/>
-      <c r="EV6" s="196"/>
+      <c r="DS6" s="196"/>
+      <c r="DT6" s="196"/>
+      <c r="DU6" s="196"/>
+      <c r="DV6" s="196"/>
+      <c r="DW6" s="196"/>
+      <c r="DX6" s="196"/>
+      <c r="DY6" s="196"/>
+      <c r="DZ6" s="196"/>
+      <c r="EA6" s="196"/>
+      <c r="EB6" s="196"/>
+      <c r="EC6" s="196"/>
+      <c r="ED6" s="196"/>
+      <c r="EE6" s="196"/>
+      <c r="EF6" s="196"/>
+      <c r="EG6" s="196"/>
+      <c r="EH6" s="196"/>
+      <c r="EI6" s="196"/>
+      <c r="EJ6" s="196"/>
+      <c r="EK6" s="196"/>
+      <c r="EL6" s="196"/>
+      <c r="EM6" s="196"/>
+      <c r="EN6" s="196"/>
+      <c r="EO6" s="196"/>
+      <c r="EP6" s="196"/>
+      <c r="EQ6" s="196"/>
+      <c r="ER6" s="196"/>
+      <c r="ES6" s="196"/>
+      <c r="ET6" s="196"/>
+      <c r="EU6" s="196"/>
+      <c r="EV6" s="197"/>
     </row>
     <row r="7" spans="1:152" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -9543,7 +9551,7 @@
       </c>
     </row>
     <row r="8" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A8" s="192" t="s">
+      <c r="A8" s="193" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="34"/>
@@ -9707,7 +9715,7 @@
       <c r="EV8" s="99"/>
     </row>
     <row r="9" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A9" s="192"/>
+      <c r="A9" s="193"/>
       <c r="B9" s="29"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -9867,7 +9875,7 @@
       <c r="EV9" s="33"/>
     </row>
     <row r="10" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A10" s="192"/>
+      <c r="A10" s="193"/>
       <c r="B10" s="29"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
@@ -10027,7 +10035,7 @@
       <c r="EV10" s="33"/>
     </row>
     <row r="11" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A11" s="192"/>
+      <c r="A11" s="193"/>
       <c r="B11" s="29"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
@@ -10185,7 +10193,7 @@
       <c r="EV11" s="33"/>
     </row>
     <row r="12" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A12" s="192"/>
+      <c r="A12" s="193"/>
       <c r="B12" s="29"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
@@ -10343,7 +10351,7 @@
       <c r="EV12" s="33"/>
     </row>
     <row r="13" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A13" s="192"/>
+      <c r="A13" s="193"/>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -10499,7 +10507,7 @@
       <c r="EV13" s="33"/>
     </row>
     <row r="14" spans="1:152" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="197"/>
+      <c r="A14" s="198"/>
       <c r="B14" s="50"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51"/>
@@ -10653,7 +10661,7 @@
       <c r="EV14" s="100"/>
     </row>
     <row r="15" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A15" s="194" t="s">
+      <c r="A15" s="195" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="42"/>
@@ -10815,7 +10823,7 @@
       <c r="EV15" s="102"/>
     </row>
     <row r="16" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A16" s="192"/>
+      <c r="A16" s="193"/>
       <c r="B16" s="24"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -10973,7 +10981,7 @@
       <c r="EV16" s="17"/>
     </row>
     <row r="17" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A17" s="192"/>
+      <c r="A17" s="193"/>
       <c r="B17" s="24"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -11133,7 +11141,7 @@
       <c r="EV17" s="17"/>
     </row>
     <row r="18" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A18" s="192"/>
+      <c r="A18" s="193"/>
       <c r="B18" s="24"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -11289,7 +11297,7 @@
       <c r="EV18" s="17"/>
     </row>
     <row r="19" spans="1:152" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="192"/>
+      <c r="A19" s="193"/>
       <c r="B19" s="26"/>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
@@ -11445,7 +11453,7 @@
       <c r="EV19" s="98"/>
     </row>
     <row r="20" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="194" t="s">
+      <c r="A20" s="195" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="75"/>
@@ -11607,7 +11615,7 @@
       <c r="EV20" s="102"/>
     </row>
     <row r="21" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="192"/>
+      <c r="A21" s="193"/>
       <c r="B21" s="24"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -11765,7 +11773,7 @@
       <c r="EV21" s="17"/>
     </row>
     <row r="22" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="192"/>
+      <c r="A22" s="193"/>
       <c r="B22" s="24"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -11923,7 +11931,7 @@
       <c r="EV22" s="17"/>
     </row>
     <row r="23" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="192"/>
+      <c r="A23" s="193"/>
       <c r="B23" s="24"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -12081,7 +12089,7 @@
       <c r="EV23" s="17"/>
     </row>
     <row r="24" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="193"/>
+      <c r="A24" s="194"/>
       <c r="B24" s="91"/>
       <c r="C24" s="92"/>
       <c r="D24" s="92"/>
@@ -12235,7 +12243,7 @@
       <c r="EV24" s="98"/>
     </row>
     <row r="25" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="194" t="s">
+      <c r="A25" s="195" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="75"/>
@@ -12391,7 +12399,7 @@
       <c r="EV25" s="102"/>
     </row>
     <row r="26" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="192"/>
+      <c r="A26" s="193"/>
       <c r="B26" s="24"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -12545,7 +12553,7 @@
       <c r="EV26" s="17"/>
     </row>
     <row r="27" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="192"/>
+      <c r="A27" s="193"/>
       <c r="B27" s="24"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
@@ -12699,7 +12707,7 @@
       <c r="EV27" s="17"/>
     </row>
     <row r="28" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="192"/>
+      <c r="A28" s="193"/>
       <c r="B28" s="24"/>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
@@ -12853,7 +12861,7 @@
       <c r="EV28" s="17"/>
     </row>
     <row r="29" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="192"/>
+      <c r="A29" s="193"/>
       <c r="B29" s="85"/>
       <c r="C29" s="71"/>
       <c r="D29" s="71"/>
@@ -13007,7 +13015,7 @@
       <c r="EV29" s="98"/>
     </row>
     <row r="30" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="191" t="s">
+      <c r="A30" s="192" t="s">
         <v>20</v>
       </c>
       <c r="B30" s="75"/>
@@ -13173,7 +13181,7 @@
       <c r="EV30" s="102"/>
     </row>
     <row r="31" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="192"/>
+      <c r="A31" s="193"/>
       <c r="B31" s="24"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -13331,7 +13339,7 @@
       <c r="EV31" s="17"/>
     </row>
     <row r="32" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="192"/>
+      <c r="A32" s="193"/>
       <c r="B32" s="24"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
@@ -13489,7 +13497,7 @@
       <c r="EV32" s="17"/>
     </row>
     <row r="33" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="192"/>
+      <c r="A33" s="193"/>
       <c r="B33" s="24"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
@@ -13645,7 +13653,7 @@
       <c r="EV33" s="17"/>
     </row>
     <row r="34" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="193"/>
+      <c r="A34" s="194"/>
       <c r="B34" s="85"/>
       <c r="C34" s="71"/>
       <c r="D34" s="71"/>
@@ -13801,7 +13809,7 @@
       <c r="EV34" s="98"/>
     </row>
     <row r="35" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="192" t="s">
+      <c r="A35" s="193" t="s">
         <v>23</v>
       </c>
       <c r="B35" s="75"/>
@@ -13959,7 +13967,7 @@
       <c r="EV35" s="102"/>
     </row>
     <row r="36" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="192"/>
+      <c r="A36" s="193"/>
       <c r="B36" s="24"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
@@ -14115,7 +14123,7 @@
       <c r="EV36" s="17"/>
     </row>
     <row r="37" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="192"/>
+      <c r="A37" s="193"/>
       <c r="B37" s="24"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -14269,7 +14277,7 @@
       <c r="EV37" s="17"/>
     </row>
     <row r="38" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="192"/>
+      <c r="A38" s="193"/>
       <c r="B38" s="24"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
@@ -14423,7 +14431,7 @@
       <c r="EV38" s="17"/>
     </row>
     <row r="39" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="192"/>
+      <c r="A39" s="193"/>
       <c r="B39" s="85"/>
       <c r="C39" s="71"/>
       <c r="D39" s="71"/>
@@ -14577,7 +14585,7 @@
       <c r="EV39" s="98"/>
     </row>
     <row r="40" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="191" t="s">
+      <c r="A40" s="192" t="s">
         <v>22</v>
       </c>
       <c r="B40" s="75"/>
@@ -14739,7 +14747,7 @@
       <c r="EV40" s="102"/>
     </row>
     <row r="41" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="192"/>
+      <c r="A41" s="193"/>
       <c r="B41" s="24"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
@@ -14895,7 +14903,7 @@
       <c r="EV41" s="17"/>
     </row>
     <row r="42" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="192"/>
+      <c r="A42" s="193"/>
       <c r="B42" s="24"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -15053,7 +15061,7 @@
       <c r="EV42" s="17"/>
     </row>
     <row r="43" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="192"/>
+      <c r="A43" s="193"/>
       <c r="B43" s="24"/>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
@@ -15209,7 +15217,7 @@
       <c r="EV43" s="17"/>
     </row>
     <row r="44" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="193"/>
+      <c r="A44" s="194"/>
       <c r="B44" s="85"/>
       <c r="C44" s="71"/>
       <c r="D44" s="71"/>
@@ -15365,7 +15373,7 @@
       <c r="EV44" s="98"/>
     </row>
     <row r="45" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="192" t="s">
+      <c r="A45" s="193" t="s">
         <v>24</v>
       </c>
       <c r="B45" s="75"/>
@@ -15527,7 +15535,7 @@
       <c r="EV45" s="102"/>
     </row>
     <row r="46" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="192"/>
+      <c r="A46" s="193"/>
       <c r="B46" s="24"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
@@ -15683,7 +15691,7 @@
       <c r="EV46" s="17"/>
     </row>
     <row r="47" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="192"/>
+      <c r="A47" s="193"/>
       <c r="B47" s="24"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
@@ -15841,7 +15849,7 @@
       <c r="EV47" s="17"/>
     </row>
     <row r="48" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="192"/>
+      <c r="A48" s="193"/>
       <c r="B48" s="24"/>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -15997,7 +16005,7 @@
       <c r="EV48" s="17"/>
     </row>
     <row r="49" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="193"/>
+      <c r="A49" s="194"/>
       <c r="B49" s="85"/>
       <c r="C49" s="71"/>
       <c r="D49" s="71"/>
@@ -16233,395 +16241,395 @@
     </row>
     <row r="6" spans="1:366" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="198">
+      <c r="B6" s="199">
         <v>1</v>
       </c>
-      <c r="C6" s="195"/>
-      <c r="D6" s="195"/>
-      <c r="E6" s="195"/>
-      <c r="F6" s="195"/>
-      <c r="G6" s="195"/>
-      <c r="H6" s="195"/>
-      <c r="I6" s="195"/>
-      <c r="J6" s="195"/>
-      <c r="K6" s="195"/>
-      <c r="L6" s="195"/>
-      <c r="M6" s="195"/>
-      <c r="N6" s="195"/>
-      <c r="O6" s="195"/>
-      <c r="P6" s="195"/>
-      <c r="Q6" s="195"/>
-      <c r="R6" s="195"/>
-      <c r="S6" s="195"/>
-      <c r="T6" s="195"/>
-      <c r="U6" s="195"/>
-      <c r="V6" s="195"/>
-      <c r="W6" s="195"/>
-      <c r="X6" s="195"/>
-      <c r="Y6" s="195"/>
-      <c r="Z6" s="195"/>
-      <c r="AA6" s="195"/>
-      <c r="AB6" s="195"/>
-      <c r="AC6" s="195"/>
-      <c r="AD6" s="195"/>
-      <c r="AE6" s="195"/>
-      <c r="AF6" s="195"/>
-      <c r="AG6" s="198">
+      <c r="C6" s="196"/>
+      <c r="D6" s="196"/>
+      <c r="E6" s="196"/>
+      <c r="F6" s="196"/>
+      <c r="G6" s="196"/>
+      <c r="H6" s="196"/>
+      <c r="I6" s="196"/>
+      <c r="J6" s="196"/>
+      <c r="K6" s="196"/>
+      <c r="L6" s="196"/>
+      <c r="M6" s="196"/>
+      <c r="N6" s="196"/>
+      <c r="O6" s="196"/>
+      <c r="P6" s="196"/>
+      <c r="Q6" s="196"/>
+      <c r="R6" s="196"/>
+      <c r="S6" s="196"/>
+      <c r="T6" s="196"/>
+      <c r="U6" s="196"/>
+      <c r="V6" s="196"/>
+      <c r="W6" s="196"/>
+      <c r="X6" s="196"/>
+      <c r="Y6" s="196"/>
+      <c r="Z6" s="196"/>
+      <c r="AA6" s="196"/>
+      <c r="AB6" s="196"/>
+      <c r="AC6" s="196"/>
+      <c r="AD6" s="196"/>
+      <c r="AE6" s="196"/>
+      <c r="AF6" s="196"/>
+      <c r="AG6" s="199">
         <v>2</v>
       </c>
-      <c r="AH6" s="195"/>
-      <c r="AI6" s="195"/>
-      <c r="AJ6" s="195"/>
-      <c r="AK6" s="195"/>
-      <c r="AL6" s="195"/>
-      <c r="AM6" s="195"/>
-      <c r="AN6" s="195"/>
-      <c r="AO6" s="195"/>
-      <c r="AP6" s="195"/>
-      <c r="AQ6" s="195"/>
-      <c r="AR6" s="195"/>
-      <c r="AS6" s="195"/>
-      <c r="AT6" s="195"/>
-      <c r="AU6" s="195"/>
-      <c r="AV6" s="195"/>
-      <c r="AW6" s="195"/>
-      <c r="AX6" s="195"/>
-      <c r="AY6" s="195"/>
-      <c r="AZ6" s="195"/>
-      <c r="BA6" s="195"/>
-      <c r="BB6" s="195"/>
-      <c r="BC6" s="195"/>
-      <c r="BD6" s="195"/>
-      <c r="BE6" s="195"/>
-      <c r="BF6" s="195"/>
-      <c r="BG6" s="195"/>
-      <c r="BH6" s="196"/>
-      <c r="BI6" s="195">
+      <c r="AH6" s="196"/>
+      <c r="AI6" s="196"/>
+      <c r="AJ6" s="196"/>
+      <c r="AK6" s="196"/>
+      <c r="AL6" s="196"/>
+      <c r="AM6" s="196"/>
+      <c r="AN6" s="196"/>
+      <c r="AO6" s="196"/>
+      <c r="AP6" s="196"/>
+      <c r="AQ6" s="196"/>
+      <c r="AR6" s="196"/>
+      <c r="AS6" s="196"/>
+      <c r="AT6" s="196"/>
+      <c r="AU6" s="196"/>
+      <c r="AV6" s="196"/>
+      <c r="AW6" s="196"/>
+      <c r="AX6" s="196"/>
+      <c r="AY6" s="196"/>
+      <c r="AZ6" s="196"/>
+      <c r="BA6" s="196"/>
+      <c r="BB6" s="196"/>
+      <c r="BC6" s="196"/>
+      <c r="BD6" s="196"/>
+      <c r="BE6" s="196"/>
+      <c r="BF6" s="196"/>
+      <c r="BG6" s="196"/>
+      <c r="BH6" s="197"/>
+      <c r="BI6" s="196">
         <v>3</v>
       </c>
-      <c r="BJ6" s="195"/>
-      <c r="BK6" s="195"/>
-      <c r="BL6" s="195"/>
-      <c r="BM6" s="195"/>
-      <c r="BN6" s="195"/>
-      <c r="BO6" s="195"/>
-      <c r="BP6" s="195"/>
-      <c r="BQ6" s="195"/>
-      <c r="BR6" s="195"/>
-      <c r="BS6" s="195"/>
-      <c r="BT6" s="195"/>
-      <c r="BU6" s="195"/>
-      <c r="BV6" s="195"/>
-      <c r="BW6" s="195"/>
-      <c r="BX6" s="195"/>
-      <c r="BY6" s="195"/>
-      <c r="BZ6" s="195"/>
-      <c r="CA6" s="195"/>
-      <c r="CB6" s="195"/>
-      <c r="CC6" s="195"/>
-      <c r="CD6" s="195"/>
-      <c r="CE6" s="195"/>
-      <c r="CF6" s="195"/>
-      <c r="CG6" s="195"/>
-      <c r="CH6" s="195"/>
-      <c r="CI6" s="195"/>
-      <c r="CJ6" s="195"/>
-      <c r="CK6" s="195"/>
-      <c r="CL6" s="195"/>
-      <c r="CM6" s="195"/>
-      <c r="CN6" s="199">
+      <c r="BJ6" s="196"/>
+      <c r="BK6" s="196"/>
+      <c r="BL6" s="196"/>
+      <c r="BM6" s="196"/>
+      <c r="BN6" s="196"/>
+      <c r="BO6" s="196"/>
+      <c r="BP6" s="196"/>
+      <c r="BQ6" s="196"/>
+      <c r="BR6" s="196"/>
+      <c r="BS6" s="196"/>
+      <c r="BT6" s="196"/>
+      <c r="BU6" s="196"/>
+      <c r="BV6" s="196"/>
+      <c r="BW6" s="196"/>
+      <c r="BX6" s="196"/>
+      <c r="BY6" s="196"/>
+      <c r="BZ6" s="196"/>
+      <c r="CA6" s="196"/>
+      <c r="CB6" s="196"/>
+      <c r="CC6" s="196"/>
+      <c r="CD6" s="196"/>
+      <c r="CE6" s="196"/>
+      <c r="CF6" s="196"/>
+      <c r="CG6" s="196"/>
+      <c r="CH6" s="196"/>
+      <c r="CI6" s="196"/>
+      <c r="CJ6" s="196"/>
+      <c r="CK6" s="196"/>
+      <c r="CL6" s="196"/>
+      <c r="CM6" s="196"/>
+      <c r="CN6" s="200">
         <v>4</v>
       </c>
-      <c r="CO6" s="200"/>
-      <c r="CP6" s="200"/>
-      <c r="CQ6" s="200"/>
-      <c r="CR6" s="200"/>
-      <c r="CS6" s="200"/>
-      <c r="CT6" s="200"/>
-      <c r="CU6" s="200"/>
-      <c r="CV6" s="200"/>
-      <c r="CW6" s="200"/>
-      <c r="CX6" s="200"/>
-      <c r="CY6" s="200"/>
-      <c r="CZ6" s="200"/>
-      <c r="DA6" s="200"/>
-      <c r="DB6" s="200"/>
-      <c r="DC6" s="200"/>
-      <c r="DD6" s="200"/>
-      <c r="DE6" s="200"/>
-      <c r="DF6" s="200"/>
-      <c r="DG6" s="200"/>
-      <c r="DH6" s="200"/>
-      <c r="DI6" s="200"/>
-      <c r="DJ6" s="200"/>
-      <c r="DK6" s="200"/>
-      <c r="DL6" s="200"/>
-      <c r="DM6" s="200"/>
-      <c r="DN6" s="200"/>
-      <c r="DO6" s="200"/>
-      <c r="DP6" s="200"/>
-      <c r="DQ6" s="201"/>
-      <c r="DR6" s="195">
+      <c r="CO6" s="201"/>
+      <c r="CP6" s="201"/>
+      <c r="CQ6" s="201"/>
+      <c r="CR6" s="201"/>
+      <c r="CS6" s="201"/>
+      <c r="CT6" s="201"/>
+      <c r="CU6" s="201"/>
+      <c r="CV6" s="201"/>
+      <c r="CW6" s="201"/>
+      <c r="CX6" s="201"/>
+      <c r="CY6" s="201"/>
+      <c r="CZ6" s="201"/>
+      <c r="DA6" s="201"/>
+      <c r="DB6" s="201"/>
+      <c r="DC6" s="201"/>
+      <c r="DD6" s="201"/>
+      <c r="DE6" s="201"/>
+      <c r="DF6" s="201"/>
+      <c r="DG6" s="201"/>
+      <c r="DH6" s="201"/>
+      <c r="DI6" s="201"/>
+      <c r="DJ6" s="201"/>
+      <c r="DK6" s="201"/>
+      <c r="DL6" s="201"/>
+      <c r="DM6" s="201"/>
+      <c r="DN6" s="201"/>
+      <c r="DO6" s="201"/>
+      <c r="DP6" s="201"/>
+      <c r="DQ6" s="202"/>
+      <c r="DR6" s="196">
         <v>5</v>
       </c>
-      <c r="DS6" s="195"/>
-      <c r="DT6" s="195"/>
-      <c r="DU6" s="195"/>
-      <c r="DV6" s="195"/>
-      <c r="DW6" s="195"/>
-      <c r="DX6" s="195"/>
-      <c r="DY6" s="195"/>
-      <c r="DZ6" s="195"/>
-      <c r="EA6" s="195"/>
-      <c r="EB6" s="195"/>
-      <c r="EC6" s="195"/>
-      <c r="ED6" s="195"/>
-      <c r="EE6" s="195"/>
-      <c r="EF6" s="195"/>
-      <c r="EG6" s="195"/>
-      <c r="EH6" s="195"/>
-      <c r="EI6" s="195"/>
-      <c r="EJ6" s="195"/>
-      <c r="EK6" s="195"/>
-      <c r="EL6" s="195"/>
-      <c r="EM6" s="195"/>
-      <c r="EN6" s="195"/>
-      <c r="EO6" s="195"/>
-      <c r="EP6" s="195"/>
-      <c r="EQ6" s="195"/>
-      <c r="ER6" s="195"/>
-      <c r="ES6" s="195"/>
-      <c r="ET6" s="195"/>
-      <c r="EU6" s="195"/>
-      <c r="EV6" s="196"/>
-      <c r="EW6" s="199">
+      <c r="DS6" s="196"/>
+      <c r="DT6" s="196"/>
+      <c r="DU6" s="196"/>
+      <c r="DV6" s="196"/>
+      <c r="DW6" s="196"/>
+      <c r="DX6" s="196"/>
+      <c r="DY6" s="196"/>
+      <c r="DZ6" s="196"/>
+      <c r="EA6" s="196"/>
+      <c r="EB6" s="196"/>
+      <c r="EC6" s="196"/>
+      <c r="ED6" s="196"/>
+      <c r="EE6" s="196"/>
+      <c r="EF6" s="196"/>
+      <c r="EG6" s="196"/>
+      <c r="EH6" s="196"/>
+      <c r="EI6" s="196"/>
+      <c r="EJ6" s="196"/>
+      <c r="EK6" s="196"/>
+      <c r="EL6" s="196"/>
+      <c r="EM6" s="196"/>
+      <c r="EN6" s="196"/>
+      <c r="EO6" s="196"/>
+      <c r="EP6" s="196"/>
+      <c r="EQ6" s="196"/>
+      <c r="ER6" s="196"/>
+      <c r="ES6" s="196"/>
+      <c r="ET6" s="196"/>
+      <c r="EU6" s="196"/>
+      <c r="EV6" s="197"/>
+      <c r="EW6" s="200">
         <v>6</v>
       </c>
-      <c r="EX6" s="200"/>
-      <c r="EY6" s="200"/>
-      <c r="EZ6" s="200"/>
-      <c r="FA6" s="200"/>
-      <c r="FB6" s="200"/>
-      <c r="FC6" s="200"/>
-      <c r="FD6" s="200"/>
-      <c r="FE6" s="200"/>
-      <c r="FF6" s="200"/>
-      <c r="FG6" s="200"/>
-      <c r="FH6" s="200"/>
-      <c r="FI6" s="200"/>
-      <c r="FJ6" s="200"/>
-      <c r="FK6" s="200"/>
-      <c r="FL6" s="200"/>
-      <c r="FM6" s="200"/>
-      <c r="FN6" s="200"/>
-      <c r="FO6" s="200"/>
-      <c r="FP6" s="200"/>
-      <c r="FQ6" s="200"/>
-      <c r="FR6" s="200"/>
-      <c r="FS6" s="200"/>
-      <c r="FT6" s="200"/>
-      <c r="FU6" s="200"/>
-      <c r="FV6" s="200"/>
-      <c r="FW6" s="200"/>
-      <c r="FX6" s="200"/>
-      <c r="FY6" s="200"/>
-      <c r="FZ6" s="201"/>
-      <c r="GA6" s="195">
+      <c r="EX6" s="201"/>
+      <c r="EY6" s="201"/>
+      <c r="EZ6" s="201"/>
+      <c r="FA6" s="201"/>
+      <c r="FB6" s="201"/>
+      <c r="FC6" s="201"/>
+      <c r="FD6" s="201"/>
+      <c r="FE6" s="201"/>
+      <c r="FF6" s="201"/>
+      <c r="FG6" s="201"/>
+      <c r="FH6" s="201"/>
+      <c r="FI6" s="201"/>
+      <c r="FJ6" s="201"/>
+      <c r="FK6" s="201"/>
+      <c r="FL6" s="201"/>
+      <c r="FM6" s="201"/>
+      <c r="FN6" s="201"/>
+      <c r="FO6" s="201"/>
+      <c r="FP6" s="201"/>
+      <c r="FQ6" s="201"/>
+      <c r="FR6" s="201"/>
+      <c r="FS6" s="201"/>
+      <c r="FT6" s="201"/>
+      <c r="FU6" s="201"/>
+      <c r="FV6" s="201"/>
+      <c r="FW6" s="201"/>
+      <c r="FX6" s="201"/>
+      <c r="FY6" s="201"/>
+      <c r="FZ6" s="202"/>
+      <c r="GA6" s="196">
         <v>7</v>
       </c>
-      <c r="GB6" s="195"/>
-      <c r="GC6" s="195"/>
-      <c r="GD6" s="195"/>
-      <c r="GE6" s="195"/>
-      <c r="GF6" s="195"/>
-      <c r="GG6" s="195"/>
-      <c r="GH6" s="195"/>
-      <c r="GI6" s="195"/>
-      <c r="GJ6" s="195"/>
-      <c r="GK6" s="195"/>
-      <c r="GL6" s="195"/>
-      <c r="GM6" s="195"/>
-      <c r="GN6" s="195"/>
-      <c r="GO6" s="195"/>
-      <c r="GP6" s="195"/>
-      <c r="GQ6" s="195"/>
-      <c r="GR6" s="195"/>
-      <c r="GS6" s="195"/>
-      <c r="GT6" s="195"/>
-      <c r="GU6" s="195"/>
-      <c r="GV6" s="195"/>
-      <c r="GW6" s="195"/>
-      <c r="GX6" s="195"/>
-      <c r="GY6" s="195"/>
-      <c r="GZ6" s="195"/>
-      <c r="HA6" s="195"/>
-      <c r="HB6" s="195"/>
-      <c r="HC6" s="195"/>
-      <c r="HD6" s="195"/>
-      <c r="HE6" s="196"/>
-      <c r="HF6" s="195">
+      <c r="GB6" s="196"/>
+      <c r="GC6" s="196"/>
+      <c r="GD6" s="196"/>
+      <c r="GE6" s="196"/>
+      <c r="GF6" s="196"/>
+      <c r="GG6" s="196"/>
+      <c r="GH6" s="196"/>
+      <c r="GI6" s="196"/>
+      <c r="GJ6" s="196"/>
+      <c r="GK6" s="196"/>
+      <c r="GL6" s="196"/>
+      <c r="GM6" s="196"/>
+      <c r="GN6" s="196"/>
+      <c r="GO6" s="196"/>
+      <c r="GP6" s="196"/>
+      <c r="GQ6" s="196"/>
+      <c r="GR6" s="196"/>
+      <c r="GS6" s="196"/>
+      <c r="GT6" s="196"/>
+      <c r="GU6" s="196"/>
+      <c r="GV6" s="196"/>
+      <c r="GW6" s="196"/>
+      <c r="GX6" s="196"/>
+      <c r="GY6" s="196"/>
+      <c r="GZ6" s="196"/>
+      <c r="HA6" s="196"/>
+      <c r="HB6" s="196"/>
+      <c r="HC6" s="196"/>
+      <c r="HD6" s="196"/>
+      <c r="HE6" s="197"/>
+      <c r="HF6" s="196">
         <v>8</v>
       </c>
-      <c r="HG6" s="195"/>
-      <c r="HH6" s="195"/>
-      <c r="HI6" s="195"/>
-      <c r="HJ6" s="195"/>
-      <c r="HK6" s="195"/>
-      <c r="HL6" s="195"/>
-      <c r="HM6" s="195"/>
-      <c r="HN6" s="195"/>
-      <c r="HO6" s="195"/>
-      <c r="HP6" s="195"/>
-      <c r="HQ6" s="195"/>
-      <c r="HR6" s="195"/>
-      <c r="HS6" s="195"/>
-      <c r="HT6" s="195"/>
-      <c r="HU6" s="195"/>
-      <c r="HV6" s="195"/>
-      <c r="HW6" s="195"/>
-      <c r="HX6" s="195"/>
-      <c r="HY6" s="195"/>
-      <c r="HZ6" s="195"/>
-      <c r="IA6" s="195"/>
-      <c r="IB6" s="195"/>
-      <c r="IC6" s="195"/>
-      <c r="ID6" s="195"/>
-      <c r="IE6" s="195"/>
-      <c r="IF6" s="195"/>
-      <c r="IG6" s="195"/>
-      <c r="IH6" s="195"/>
-      <c r="II6" s="195"/>
-      <c r="IJ6" s="196"/>
-      <c r="IK6" s="199">
+      <c r="HG6" s="196"/>
+      <c r="HH6" s="196"/>
+      <c r="HI6" s="196"/>
+      <c r="HJ6" s="196"/>
+      <c r="HK6" s="196"/>
+      <c r="HL6" s="196"/>
+      <c r="HM6" s="196"/>
+      <c r="HN6" s="196"/>
+      <c r="HO6" s="196"/>
+      <c r="HP6" s="196"/>
+      <c r="HQ6" s="196"/>
+      <c r="HR6" s="196"/>
+      <c r="HS6" s="196"/>
+      <c r="HT6" s="196"/>
+      <c r="HU6" s="196"/>
+      <c r="HV6" s="196"/>
+      <c r="HW6" s="196"/>
+      <c r="HX6" s="196"/>
+      <c r="HY6" s="196"/>
+      <c r="HZ6" s="196"/>
+      <c r="IA6" s="196"/>
+      <c r="IB6" s="196"/>
+      <c r="IC6" s="196"/>
+      <c r="ID6" s="196"/>
+      <c r="IE6" s="196"/>
+      <c r="IF6" s="196"/>
+      <c r="IG6" s="196"/>
+      <c r="IH6" s="196"/>
+      <c r="II6" s="196"/>
+      <c r="IJ6" s="197"/>
+      <c r="IK6" s="200">
         <v>9</v>
       </c>
-      <c r="IL6" s="200"/>
-      <c r="IM6" s="200"/>
-      <c r="IN6" s="200"/>
-      <c r="IO6" s="200"/>
-      <c r="IP6" s="200"/>
-      <c r="IQ6" s="200"/>
-      <c r="IR6" s="200"/>
-      <c r="IS6" s="200"/>
-      <c r="IT6" s="200"/>
-      <c r="IU6" s="200"/>
-      <c r="IV6" s="200"/>
-      <c r="IW6" s="200"/>
-      <c r="IX6" s="200"/>
-      <c r="IY6" s="200"/>
-      <c r="IZ6" s="200"/>
-      <c r="JA6" s="200"/>
-      <c r="JB6" s="200"/>
-      <c r="JC6" s="200"/>
-      <c r="JD6" s="200"/>
-      <c r="JE6" s="200"/>
-      <c r="JF6" s="200"/>
-      <c r="JG6" s="200"/>
-      <c r="JH6" s="200"/>
-      <c r="JI6" s="200"/>
-      <c r="JJ6" s="200"/>
-      <c r="JK6" s="200"/>
-      <c r="JL6" s="200"/>
-      <c r="JM6" s="200"/>
-      <c r="JN6" s="201"/>
-      <c r="JO6" s="195">
+      <c r="IL6" s="201"/>
+      <c r="IM6" s="201"/>
+      <c r="IN6" s="201"/>
+      <c r="IO6" s="201"/>
+      <c r="IP6" s="201"/>
+      <c r="IQ6" s="201"/>
+      <c r="IR6" s="201"/>
+      <c r="IS6" s="201"/>
+      <c r="IT6" s="201"/>
+      <c r="IU6" s="201"/>
+      <c r="IV6" s="201"/>
+      <c r="IW6" s="201"/>
+      <c r="IX6" s="201"/>
+      <c r="IY6" s="201"/>
+      <c r="IZ6" s="201"/>
+      <c r="JA6" s="201"/>
+      <c r="JB6" s="201"/>
+      <c r="JC6" s="201"/>
+      <c r="JD6" s="201"/>
+      <c r="JE6" s="201"/>
+      <c r="JF6" s="201"/>
+      <c r="JG6" s="201"/>
+      <c r="JH6" s="201"/>
+      <c r="JI6" s="201"/>
+      <c r="JJ6" s="201"/>
+      <c r="JK6" s="201"/>
+      <c r="JL6" s="201"/>
+      <c r="JM6" s="201"/>
+      <c r="JN6" s="202"/>
+      <c r="JO6" s="196">
         <v>10</v>
       </c>
-      <c r="JP6" s="195"/>
-      <c r="JQ6" s="195"/>
-      <c r="JR6" s="195"/>
-      <c r="JS6" s="195"/>
-      <c r="JT6" s="195"/>
-      <c r="JU6" s="195"/>
-      <c r="JV6" s="195"/>
-      <c r="JW6" s="195"/>
-      <c r="JX6" s="195"/>
-      <c r="JY6" s="195"/>
-      <c r="JZ6" s="195"/>
-      <c r="KA6" s="195"/>
-      <c r="KB6" s="195"/>
-      <c r="KC6" s="195"/>
-      <c r="KD6" s="195"/>
-      <c r="KE6" s="195"/>
-      <c r="KF6" s="195"/>
-      <c r="KG6" s="195"/>
-      <c r="KH6" s="195"/>
-      <c r="KI6" s="195"/>
-      <c r="KJ6" s="195"/>
-      <c r="KK6" s="195"/>
-      <c r="KL6" s="195"/>
-      <c r="KM6" s="195"/>
-      <c r="KN6" s="195"/>
-      <c r="KO6" s="195"/>
-      <c r="KP6" s="195"/>
-      <c r="KQ6" s="195"/>
-      <c r="KR6" s="195"/>
-      <c r="KS6" s="196"/>
-      <c r="KT6" s="199">
+      <c r="JP6" s="196"/>
+      <c r="JQ6" s="196"/>
+      <c r="JR6" s="196"/>
+      <c r="JS6" s="196"/>
+      <c r="JT6" s="196"/>
+      <c r="JU6" s="196"/>
+      <c r="JV6" s="196"/>
+      <c r="JW6" s="196"/>
+      <c r="JX6" s="196"/>
+      <c r="JY6" s="196"/>
+      <c r="JZ6" s="196"/>
+      <c r="KA6" s="196"/>
+      <c r="KB6" s="196"/>
+      <c r="KC6" s="196"/>
+      <c r="KD6" s="196"/>
+      <c r="KE6" s="196"/>
+      <c r="KF6" s="196"/>
+      <c r="KG6" s="196"/>
+      <c r="KH6" s="196"/>
+      <c r="KI6" s="196"/>
+      <c r="KJ6" s="196"/>
+      <c r="KK6" s="196"/>
+      <c r="KL6" s="196"/>
+      <c r="KM6" s="196"/>
+      <c r="KN6" s="196"/>
+      <c r="KO6" s="196"/>
+      <c r="KP6" s="196"/>
+      <c r="KQ6" s="196"/>
+      <c r="KR6" s="196"/>
+      <c r="KS6" s="197"/>
+      <c r="KT6" s="200">
         <v>11</v>
       </c>
-      <c r="KU6" s="200"/>
-      <c r="KV6" s="200"/>
-      <c r="KW6" s="200"/>
-      <c r="KX6" s="200"/>
-      <c r="KY6" s="200"/>
-      <c r="KZ6" s="200"/>
-      <c r="LA6" s="200"/>
-      <c r="LB6" s="200"/>
-      <c r="LC6" s="200"/>
-      <c r="LD6" s="200"/>
-      <c r="LE6" s="200"/>
-      <c r="LF6" s="200"/>
-      <c r="LG6" s="200"/>
-      <c r="LH6" s="200"/>
-      <c r="LI6" s="200"/>
-      <c r="LJ6" s="200"/>
-      <c r="LK6" s="200"/>
-      <c r="LL6" s="200"/>
-      <c r="LM6" s="200"/>
-      <c r="LN6" s="200"/>
-      <c r="LO6" s="200"/>
-      <c r="LP6" s="200"/>
-      <c r="LQ6" s="200"/>
-      <c r="LR6" s="200"/>
-      <c r="LS6" s="200"/>
-      <c r="LT6" s="200"/>
-      <c r="LU6" s="200"/>
-      <c r="LV6" s="200"/>
-      <c r="LW6" s="201"/>
-      <c r="LX6" s="195">
+      <c r="KU6" s="201"/>
+      <c r="KV6" s="201"/>
+      <c r="KW6" s="201"/>
+      <c r="KX6" s="201"/>
+      <c r="KY6" s="201"/>
+      <c r="KZ6" s="201"/>
+      <c r="LA6" s="201"/>
+      <c r="LB6" s="201"/>
+      <c r="LC6" s="201"/>
+      <c r="LD6" s="201"/>
+      <c r="LE6" s="201"/>
+      <c r="LF6" s="201"/>
+      <c r="LG6" s="201"/>
+      <c r="LH6" s="201"/>
+      <c r="LI6" s="201"/>
+      <c r="LJ6" s="201"/>
+      <c r="LK6" s="201"/>
+      <c r="LL6" s="201"/>
+      <c r="LM6" s="201"/>
+      <c r="LN6" s="201"/>
+      <c r="LO6" s="201"/>
+      <c r="LP6" s="201"/>
+      <c r="LQ6" s="201"/>
+      <c r="LR6" s="201"/>
+      <c r="LS6" s="201"/>
+      <c r="LT6" s="201"/>
+      <c r="LU6" s="201"/>
+      <c r="LV6" s="201"/>
+      <c r="LW6" s="202"/>
+      <c r="LX6" s="196">
         <v>12</v>
       </c>
-      <c r="LY6" s="195"/>
-      <c r="LZ6" s="195"/>
-      <c r="MA6" s="195"/>
-      <c r="MB6" s="195"/>
-      <c r="MC6" s="195"/>
-      <c r="MD6" s="195"/>
-      <c r="ME6" s="195"/>
-      <c r="MF6" s="195"/>
-      <c r="MG6" s="195"/>
-      <c r="MH6" s="195"/>
-      <c r="MI6" s="195"/>
-      <c r="MJ6" s="195"/>
-      <c r="MK6" s="195"/>
-      <c r="ML6" s="195"/>
-      <c r="MM6" s="195"/>
-      <c r="MN6" s="195"/>
-      <c r="MO6" s="195"/>
-      <c r="MP6" s="195"/>
-      <c r="MQ6" s="195"/>
-      <c r="MR6" s="195"/>
-      <c r="MS6" s="195"/>
-      <c r="MT6" s="195"/>
-      <c r="MU6" s="195"/>
-      <c r="MV6" s="195"/>
-      <c r="MW6" s="195"/>
-      <c r="MX6" s="195"/>
-      <c r="MY6" s="195"/>
-      <c r="MZ6" s="195"/>
-      <c r="NA6" s="195"/>
-      <c r="NB6" s="196"/>
+      <c r="LY6" s="196"/>
+      <c r="LZ6" s="196"/>
+      <c r="MA6" s="196"/>
+      <c r="MB6" s="196"/>
+      <c r="MC6" s="196"/>
+      <c r="MD6" s="196"/>
+      <c r="ME6" s="196"/>
+      <c r="MF6" s="196"/>
+      <c r="MG6" s="196"/>
+      <c r="MH6" s="196"/>
+      <c r="MI6" s="196"/>
+      <c r="MJ6" s="196"/>
+      <c r="MK6" s="196"/>
+      <c r="ML6" s="196"/>
+      <c r="MM6" s="196"/>
+      <c r="MN6" s="196"/>
+      <c r="MO6" s="196"/>
+      <c r="MP6" s="196"/>
+      <c r="MQ6" s="196"/>
+      <c r="MR6" s="196"/>
+      <c r="MS6" s="196"/>
+      <c r="MT6" s="196"/>
+      <c r="MU6" s="196"/>
+      <c r="MV6" s="196"/>
+      <c r="MW6" s="196"/>
+      <c r="MX6" s="196"/>
+      <c r="MY6" s="196"/>
+      <c r="MZ6" s="196"/>
+      <c r="NA6" s="196"/>
+      <c r="NB6" s="197"/>
     </row>
     <row r="7" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -17722,7 +17730,7 @@
       </c>
     </row>
     <row r="8" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="202" t="s">
+      <c r="A8" s="203" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="34"/>
@@ -18110,7 +18118,7 @@
       <c r="NB8" s="141"/>
     </row>
     <row r="9" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="202"/>
+      <c r="A9" s="203"/>
       <c r="B9" s="29"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -18490,7 +18498,7 @@
       <c r="NB9" s="32"/>
     </row>
     <row r="10" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="202"/>
+      <c r="A10" s="203"/>
       <c r="B10" s="29"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
@@ -18870,7 +18878,7 @@
       <c r="NB10" s="32"/>
     </row>
     <row r="11" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="202"/>
+      <c r="A11" s="203"/>
       <c r="B11" s="29"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
@@ -19246,7 +19254,7 @@
       <c r="NB11" s="32"/>
     </row>
     <row r="12" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="202"/>
+      <c r="A12" s="203"/>
       <c r="B12" s="29"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
@@ -19620,7 +19628,7 @@
       <c r="NB12" s="32"/>
     </row>
     <row r="13" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="202"/>
+      <c r="A13" s="203"/>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -19990,7 +19998,7 @@
       <c r="NB13" s="32"/>
     </row>
     <row r="14" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="202"/>
+      <c r="A14" s="203"/>
       <c r="B14" s="50"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51"/>
@@ -20360,7 +20368,7 @@
       <c r="NB14" s="65"/>
     </row>
     <row r="15" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="202" t="s">
+      <c r="A15" s="203" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="42"/>
@@ -20744,7 +20752,7 @@
       <c r="NB15" s="84"/>
     </row>
     <row r="16" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="202"/>
+      <c r="A16" s="203"/>
       <c r="B16" s="24"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -21124,7 +21132,7 @@
       <c r="NB16" s="25"/>
     </row>
     <row r="17" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="202"/>
+      <c r="A17" s="203"/>
       <c r="B17" s="24"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -21500,7 +21508,7 @@
       <c r="NB17" s="25"/>
     </row>
     <row r="18" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="202"/>
+      <c r="A18" s="203"/>
       <c r="B18" s="24"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -21876,7 +21884,7 @@
       <c r="NB18" s="25"/>
     </row>
     <row r="19" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="202"/>
+      <c r="A19" s="203"/>
       <c r="B19" s="26"/>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
@@ -22246,7 +22254,7 @@
       <c r="NB19" s="74"/>
     </row>
     <row r="20" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="202" t="s">
+      <c r="A20" s="203" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="75"/>
@@ -22624,7 +22632,7 @@
       <c r="NB20" s="84"/>
     </row>
     <row r="21" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="202"/>
+      <c r="A21" s="203"/>
       <c r="B21" s="24"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -22998,7 +23006,7 @@
       <c r="NB21" s="25"/>
     </row>
     <row r="22" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="202"/>
+      <c r="A22" s="203"/>
       <c r="B22" s="24"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -23370,7 +23378,7 @@
       <c r="NB22" s="25"/>
     </row>
     <row r="23" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="202"/>
+      <c r="A23" s="203"/>
       <c r="B23" s="24"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -23746,7 +23754,7 @@
       <c r="NB23" s="25"/>
     </row>
     <row r="24" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="202"/>
+      <c r="A24" s="203"/>
       <c r="B24" s="91"/>
       <c r="C24" s="92"/>
       <c r="D24" s="92"/>
@@ -24114,7 +24122,7 @@
       <c r="NB24" s="74"/>
     </row>
     <row r="25" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="203" t="s">
+      <c r="A25" s="204" t="s">
         <v>62</v>
       </c>
       <c r="B25" s="75"/>
@@ -24490,7 +24498,7 @@
       <c r="NB25" s="84"/>
     </row>
     <row r="26" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="202"/>
+      <c r="A26" s="203"/>
       <c r="B26" s="24"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -24862,7 +24870,7 @@
       <c r="NB26" s="25"/>
     </row>
     <row r="27" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="202"/>
+      <c r="A27" s="203"/>
       <c r="B27" s="24"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
@@ -25236,7 +25244,7 @@
       <c r="NB27" s="25"/>
     </row>
     <row r="28" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="202"/>
+      <c r="A28" s="203"/>
       <c r="B28" s="24"/>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
@@ -25608,7 +25616,7 @@
       <c r="NB28" s="25"/>
     </row>
     <row r="29" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="202"/>
+      <c r="A29" s="203"/>
       <c r="B29" s="85"/>
       <c r="C29" s="71"/>
       <c r="D29" s="71"/>
@@ -25978,7 +25986,7 @@
       <c r="NB29" s="74"/>
     </row>
     <row r="30" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="203" t="s">
+      <c r="A30" s="204" t="s">
         <v>63</v>
       </c>
       <c r="B30" s="75"/>
@@ -26350,7 +26358,7 @@
       <c r="NB30" s="84"/>
     </row>
     <row r="31" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="202"/>
+      <c r="A31" s="203"/>
       <c r="B31" s="24"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -26724,7 +26732,7 @@
       <c r="NB31" s="25"/>
     </row>
     <row r="32" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="202"/>
+      <c r="A32" s="203"/>
       <c r="B32" s="24"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
@@ -27098,7 +27106,7 @@
       <c r="NB32" s="25"/>
     </row>
     <row r="33" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="202"/>
+      <c r="A33" s="203"/>
       <c r="B33" s="24"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
@@ -27468,7 +27476,7 @@
       <c r="NB33" s="25"/>
     </row>
     <row r="34" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="202"/>
+      <c r="A34" s="203"/>
       <c r="B34" s="85"/>
       <c r="C34" s="71"/>
       <c r="D34" s="71"/>
@@ -27836,7 +27844,7 @@
       <c r="NB34" s="74"/>
     </row>
     <row r="35" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="202" t="s">
+      <c r="A35" s="203" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="42"/>
@@ -28218,7 +28226,7 @@
       <c r="NB35" s="47"/>
     </row>
     <row r="36" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="202"/>
+      <c r="A36" s="203"/>
       <c r="B36" s="24"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
@@ -28590,7 +28598,7 @@
       <c r="NB36" s="25"/>
     </row>
     <row r="37" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="202"/>
+      <c r="A37" s="203"/>
       <c r="B37" s="24"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -28968,7 +28976,7 @@
       <c r="NB37" s="25"/>
     </row>
     <row r="38" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="202"/>
+      <c r="A38" s="203"/>
       <c r="B38" s="24"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
@@ -29338,7 +29346,7 @@
       <c r="NB38" s="25"/>
     </row>
     <row r="39" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="202"/>
+      <c r="A39" s="203"/>
       <c r="B39" s="85"/>
       <c r="C39" s="71"/>
       <c r="D39" s="71"/>
@@ -29710,7 +29718,7 @@
       <c r="NB39" s="74"/>
     </row>
     <row r="40" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="202" t="s">
+      <c r="A40" s="203" t="s">
         <v>23</v>
       </c>
       <c r="B40" s="75"/>
@@ -30088,7 +30096,7 @@
       <c r="NB40" s="84"/>
     </row>
     <row r="41" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="202"/>
+      <c r="A41" s="203"/>
       <c r="B41" s="24"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
@@ -30462,7 +30470,7 @@
       <c r="NB41" s="25"/>
     </row>
     <row r="42" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="202"/>
+      <c r="A42" s="203"/>
       <c r="B42" s="24"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -30834,7 +30842,7 @@
       <c r="NB42" s="25"/>
     </row>
     <row r="43" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="202"/>
+      <c r="A43" s="203"/>
       <c r="B43" s="24"/>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
@@ -31204,7 +31212,7 @@
       <c r="NB43" s="25"/>
     </row>
     <row r="44" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="202"/>
+      <c r="A44" s="203"/>
       <c r="B44" s="85"/>
       <c r="C44" s="71"/>
       <c r="D44" s="71"/>
@@ -31572,7 +31580,7 @@
       <c r="NB44" s="74"/>
     </row>
     <row r="45" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="202" t="s">
+      <c r="A45" s="203" t="s">
         <v>22</v>
       </c>
       <c r="B45" s="75"/>
@@ -31952,7 +31960,7 @@
       <c r="NB45" s="84"/>
     </row>
     <row r="46" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="202"/>
+      <c r="A46" s="203"/>
       <c r="B46" s="24"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
@@ -32322,7 +32330,7 @@
       <c r="NB46" s="25"/>
     </row>
     <row r="47" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="202"/>
+      <c r="A47" s="203"/>
       <c r="B47" s="24"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
@@ -32698,7 +32706,7 @@
       <c r="NB47" s="25"/>
     </row>
     <row r="48" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="202"/>
+      <c r="A48" s="203"/>
       <c r="B48" s="24"/>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -33068,7 +33076,7 @@
       <c r="NB48" s="25"/>
     </row>
     <row r="49" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="202"/>
+      <c r="A49" s="203"/>
       <c r="B49" s="85"/>
       <c r="C49" s="71"/>
       <c r="D49" s="71"/>
@@ -33442,7 +33450,7 @@
       <c r="NB49" s="74"/>
     </row>
     <row r="50" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="202" t="s">
+      <c r="A50" s="203" t="s">
         <v>24</v>
       </c>
       <c r="B50" s="75"/>
@@ -33824,7 +33832,7 @@
       <c r="NB50" s="84"/>
     </row>
     <row r="51" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="202"/>
+      <c r="A51" s="203"/>
       <c r="B51" s="24"/>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
@@ -34202,7 +34210,7 @@
       <c r="NB51" s="25"/>
     </row>
     <row r="52" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="202"/>
+      <c r="A52" s="203"/>
       <c r="B52" s="24"/>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
@@ -34574,7 +34582,7 @@
       <c r="NB52" s="25"/>
     </row>
     <row r="53" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="202"/>
+      <c r="A53" s="203"/>
       <c r="B53" s="24"/>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
@@ -34944,7 +34952,7 @@
       <c r="NB53" s="25"/>
     </row>
     <row r="54" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="202"/>
+      <c r="A54" s="203"/>
       <c r="B54" s="85"/>
       <c r="C54" s="71"/>
       <c r="D54" s="71"/>
@@ -35330,11 +35338,6 @@
     <row r="71" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="GA6:HE6"/>
-    <mergeCell ref="HF6:IJ6"/>
-    <mergeCell ref="IK6:JN6"/>
-    <mergeCell ref="JO6:KS6"/>
-    <mergeCell ref="KT6:LW6"/>
     <mergeCell ref="LX6:NB6"/>
     <mergeCell ref="A50:A54"/>
     <mergeCell ref="A15:A19"/>
@@ -35351,6 +35354,11 @@
     <mergeCell ref="BI6:CM6"/>
     <mergeCell ref="CN6:DQ6"/>
     <mergeCell ref="DR6:EV6"/>
+    <mergeCell ref="GA6:HE6"/>
+    <mergeCell ref="HF6:IJ6"/>
+    <mergeCell ref="IK6:JN6"/>
+    <mergeCell ref="JO6:KS6"/>
+    <mergeCell ref="KT6:LW6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35366,7 +35374,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CP1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="FT23" sqref="FT23"/>
+      <selection pane="topRight" activeCell="EJ39" sqref="EJ39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -35403,395 +35411,395 @@
     </row>
     <row r="6" spans="1:366" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="198">
+      <c r="B6" s="199">
         <v>1</v>
       </c>
-      <c r="C6" s="195"/>
-      <c r="D6" s="195"/>
-      <c r="E6" s="195"/>
-      <c r="F6" s="195"/>
-      <c r="G6" s="195"/>
-      <c r="H6" s="195"/>
-      <c r="I6" s="195"/>
-      <c r="J6" s="195"/>
-      <c r="K6" s="195"/>
-      <c r="L6" s="195"/>
-      <c r="M6" s="195"/>
-      <c r="N6" s="195"/>
-      <c r="O6" s="195"/>
-      <c r="P6" s="195"/>
-      <c r="Q6" s="195"/>
-      <c r="R6" s="195"/>
-      <c r="S6" s="195"/>
-      <c r="T6" s="195"/>
-      <c r="U6" s="195"/>
-      <c r="V6" s="195"/>
-      <c r="W6" s="195"/>
-      <c r="X6" s="195"/>
-      <c r="Y6" s="195"/>
-      <c r="Z6" s="195"/>
-      <c r="AA6" s="195"/>
-      <c r="AB6" s="195"/>
-      <c r="AC6" s="195"/>
-      <c r="AD6" s="195"/>
-      <c r="AE6" s="195"/>
-      <c r="AF6" s="195"/>
-      <c r="AG6" s="198">
+      <c r="C6" s="196"/>
+      <c r="D6" s="196"/>
+      <c r="E6" s="196"/>
+      <c r="F6" s="196"/>
+      <c r="G6" s="196"/>
+      <c r="H6" s="196"/>
+      <c r="I6" s="196"/>
+      <c r="J6" s="196"/>
+      <c r="K6" s="196"/>
+      <c r="L6" s="196"/>
+      <c r="M6" s="196"/>
+      <c r="N6" s="196"/>
+      <c r="O6" s="196"/>
+      <c r="P6" s="196"/>
+      <c r="Q6" s="196"/>
+      <c r="R6" s="196"/>
+      <c r="S6" s="196"/>
+      <c r="T6" s="196"/>
+      <c r="U6" s="196"/>
+      <c r="V6" s="196"/>
+      <c r="W6" s="196"/>
+      <c r="X6" s="196"/>
+      <c r="Y6" s="196"/>
+      <c r="Z6" s="196"/>
+      <c r="AA6" s="196"/>
+      <c r="AB6" s="196"/>
+      <c r="AC6" s="196"/>
+      <c r="AD6" s="196"/>
+      <c r="AE6" s="196"/>
+      <c r="AF6" s="196"/>
+      <c r="AG6" s="199">
         <v>2</v>
       </c>
-      <c r="AH6" s="195"/>
-      <c r="AI6" s="195"/>
-      <c r="AJ6" s="195"/>
-      <c r="AK6" s="195"/>
-      <c r="AL6" s="195"/>
-      <c r="AM6" s="195"/>
-      <c r="AN6" s="195"/>
-      <c r="AO6" s="195"/>
-      <c r="AP6" s="195"/>
-      <c r="AQ6" s="195"/>
-      <c r="AR6" s="195"/>
-      <c r="AS6" s="195"/>
-      <c r="AT6" s="195"/>
-      <c r="AU6" s="195"/>
-      <c r="AV6" s="195"/>
-      <c r="AW6" s="195"/>
-      <c r="AX6" s="195"/>
-      <c r="AY6" s="195"/>
-      <c r="AZ6" s="195"/>
-      <c r="BA6" s="195"/>
-      <c r="BB6" s="195"/>
-      <c r="BC6" s="195"/>
-      <c r="BD6" s="195"/>
-      <c r="BE6" s="195"/>
-      <c r="BF6" s="195"/>
-      <c r="BG6" s="195"/>
-      <c r="BH6" s="196"/>
-      <c r="BI6" s="195">
+      <c r="AH6" s="196"/>
+      <c r="AI6" s="196"/>
+      <c r="AJ6" s="196"/>
+      <c r="AK6" s="196"/>
+      <c r="AL6" s="196"/>
+      <c r="AM6" s="196"/>
+      <c r="AN6" s="196"/>
+      <c r="AO6" s="196"/>
+      <c r="AP6" s="196"/>
+      <c r="AQ6" s="196"/>
+      <c r="AR6" s="196"/>
+      <c r="AS6" s="196"/>
+      <c r="AT6" s="196"/>
+      <c r="AU6" s="196"/>
+      <c r="AV6" s="196"/>
+      <c r="AW6" s="196"/>
+      <c r="AX6" s="196"/>
+      <c r="AY6" s="196"/>
+      <c r="AZ6" s="196"/>
+      <c r="BA6" s="196"/>
+      <c r="BB6" s="196"/>
+      <c r="BC6" s="196"/>
+      <c r="BD6" s="196"/>
+      <c r="BE6" s="196"/>
+      <c r="BF6" s="196"/>
+      <c r="BG6" s="196"/>
+      <c r="BH6" s="197"/>
+      <c r="BI6" s="196">
         <v>3</v>
       </c>
-      <c r="BJ6" s="195"/>
-      <c r="BK6" s="195"/>
-      <c r="BL6" s="195"/>
-      <c r="BM6" s="195"/>
-      <c r="BN6" s="195"/>
-      <c r="BO6" s="195"/>
-      <c r="BP6" s="195"/>
-      <c r="BQ6" s="195"/>
-      <c r="BR6" s="195"/>
-      <c r="BS6" s="195"/>
-      <c r="BT6" s="195"/>
-      <c r="BU6" s="195"/>
-      <c r="BV6" s="195"/>
-      <c r="BW6" s="195"/>
-      <c r="BX6" s="195"/>
-      <c r="BY6" s="195"/>
-      <c r="BZ6" s="195"/>
-      <c r="CA6" s="195"/>
-      <c r="CB6" s="195"/>
-      <c r="CC6" s="195"/>
-      <c r="CD6" s="195"/>
-      <c r="CE6" s="195"/>
-      <c r="CF6" s="195"/>
-      <c r="CG6" s="195"/>
-      <c r="CH6" s="195"/>
-      <c r="CI6" s="195"/>
-      <c r="CJ6" s="195"/>
-      <c r="CK6" s="195"/>
-      <c r="CL6" s="195"/>
-      <c r="CM6" s="195"/>
-      <c r="CN6" s="199">
+      <c r="BJ6" s="196"/>
+      <c r="BK6" s="196"/>
+      <c r="BL6" s="196"/>
+      <c r="BM6" s="196"/>
+      <c r="BN6" s="196"/>
+      <c r="BO6" s="196"/>
+      <c r="BP6" s="196"/>
+      <c r="BQ6" s="196"/>
+      <c r="BR6" s="196"/>
+      <c r="BS6" s="196"/>
+      <c r="BT6" s="196"/>
+      <c r="BU6" s="196"/>
+      <c r="BV6" s="196"/>
+      <c r="BW6" s="196"/>
+      <c r="BX6" s="196"/>
+      <c r="BY6" s="196"/>
+      <c r="BZ6" s="196"/>
+      <c r="CA6" s="196"/>
+      <c r="CB6" s="196"/>
+      <c r="CC6" s="196"/>
+      <c r="CD6" s="196"/>
+      <c r="CE6" s="196"/>
+      <c r="CF6" s="196"/>
+      <c r="CG6" s="196"/>
+      <c r="CH6" s="196"/>
+      <c r="CI6" s="196"/>
+      <c r="CJ6" s="196"/>
+      <c r="CK6" s="196"/>
+      <c r="CL6" s="196"/>
+      <c r="CM6" s="196"/>
+      <c r="CN6" s="200">
         <v>4</v>
       </c>
-      <c r="CO6" s="200"/>
-      <c r="CP6" s="200"/>
-      <c r="CQ6" s="200"/>
-      <c r="CR6" s="200"/>
-      <c r="CS6" s="200"/>
-      <c r="CT6" s="200"/>
-      <c r="CU6" s="200"/>
-      <c r="CV6" s="200"/>
-      <c r="CW6" s="200"/>
-      <c r="CX6" s="200"/>
-      <c r="CY6" s="200"/>
-      <c r="CZ6" s="200"/>
-      <c r="DA6" s="200"/>
-      <c r="DB6" s="200"/>
-      <c r="DC6" s="200"/>
-      <c r="DD6" s="200"/>
-      <c r="DE6" s="200"/>
-      <c r="DF6" s="200"/>
-      <c r="DG6" s="200"/>
-      <c r="DH6" s="200"/>
-      <c r="DI6" s="200"/>
-      <c r="DJ6" s="200"/>
-      <c r="DK6" s="200"/>
-      <c r="DL6" s="200"/>
-      <c r="DM6" s="200"/>
-      <c r="DN6" s="200"/>
-      <c r="DO6" s="200"/>
-      <c r="DP6" s="200"/>
-      <c r="DQ6" s="201"/>
-      <c r="DR6" s="195">
+      <c r="CO6" s="201"/>
+      <c r="CP6" s="201"/>
+      <c r="CQ6" s="201"/>
+      <c r="CR6" s="201"/>
+      <c r="CS6" s="201"/>
+      <c r="CT6" s="201"/>
+      <c r="CU6" s="201"/>
+      <c r="CV6" s="201"/>
+      <c r="CW6" s="201"/>
+      <c r="CX6" s="201"/>
+      <c r="CY6" s="201"/>
+      <c r="CZ6" s="201"/>
+      <c r="DA6" s="201"/>
+      <c r="DB6" s="201"/>
+      <c r="DC6" s="201"/>
+      <c r="DD6" s="201"/>
+      <c r="DE6" s="201"/>
+      <c r="DF6" s="201"/>
+      <c r="DG6" s="201"/>
+      <c r="DH6" s="201"/>
+      <c r="DI6" s="201"/>
+      <c r="DJ6" s="201"/>
+      <c r="DK6" s="201"/>
+      <c r="DL6" s="201"/>
+      <c r="DM6" s="201"/>
+      <c r="DN6" s="201"/>
+      <c r="DO6" s="201"/>
+      <c r="DP6" s="201"/>
+      <c r="DQ6" s="202"/>
+      <c r="DR6" s="196">
         <v>5</v>
       </c>
-      <c r="DS6" s="195"/>
-      <c r="DT6" s="195"/>
-      <c r="DU6" s="195"/>
-      <c r="DV6" s="195"/>
-      <c r="DW6" s="195"/>
-      <c r="DX6" s="195"/>
-      <c r="DY6" s="195"/>
-      <c r="DZ6" s="195"/>
-      <c r="EA6" s="195"/>
-      <c r="EB6" s="195"/>
-      <c r="EC6" s="195"/>
-      <c r="ED6" s="195"/>
-      <c r="EE6" s="195"/>
-      <c r="EF6" s="195"/>
-      <c r="EG6" s="195"/>
-      <c r="EH6" s="195"/>
-      <c r="EI6" s="195"/>
-      <c r="EJ6" s="195"/>
-      <c r="EK6" s="195"/>
-      <c r="EL6" s="195"/>
-      <c r="EM6" s="195"/>
-      <c r="EN6" s="195"/>
-      <c r="EO6" s="195"/>
-      <c r="EP6" s="195"/>
-      <c r="EQ6" s="195"/>
-      <c r="ER6" s="195"/>
-      <c r="ES6" s="195"/>
-      <c r="ET6" s="195"/>
-      <c r="EU6" s="195"/>
-      <c r="EV6" s="196"/>
-      <c r="EW6" s="199">
+      <c r="DS6" s="196"/>
+      <c r="DT6" s="196"/>
+      <c r="DU6" s="196"/>
+      <c r="DV6" s="196"/>
+      <c r="DW6" s="196"/>
+      <c r="DX6" s="196"/>
+      <c r="DY6" s="196"/>
+      <c r="DZ6" s="196"/>
+      <c r="EA6" s="196"/>
+      <c r="EB6" s="196"/>
+      <c r="EC6" s="196"/>
+      <c r="ED6" s="196"/>
+      <c r="EE6" s="196"/>
+      <c r="EF6" s="196"/>
+      <c r="EG6" s="196"/>
+      <c r="EH6" s="196"/>
+      <c r="EI6" s="196"/>
+      <c r="EJ6" s="196"/>
+      <c r="EK6" s="196"/>
+      <c r="EL6" s="196"/>
+      <c r="EM6" s="196"/>
+      <c r="EN6" s="196"/>
+      <c r="EO6" s="196"/>
+      <c r="EP6" s="196"/>
+      <c r="EQ6" s="196"/>
+      <c r="ER6" s="196"/>
+      <c r="ES6" s="196"/>
+      <c r="ET6" s="196"/>
+      <c r="EU6" s="196"/>
+      <c r="EV6" s="197"/>
+      <c r="EW6" s="200">
         <v>6</v>
       </c>
-      <c r="EX6" s="200"/>
-      <c r="EY6" s="200"/>
-      <c r="EZ6" s="200"/>
-      <c r="FA6" s="200"/>
-      <c r="FB6" s="200"/>
-      <c r="FC6" s="200"/>
-      <c r="FD6" s="200"/>
-      <c r="FE6" s="200"/>
-      <c r="FF6" s="200"/>
-      <c r="FG6" s="200"/>
-      <c r="FH6" s="200"/>
-      <c r="FI6" s="200"/>
-      <c r="FJ6" s="200"/>
-      <c r="FK6" s="200"/>
-      <c r="FL6" s="200"/>
-      <c r="FM6" s="200"/>
-      <c r="FN6" s="200"/>
-      <c r="FO6" s="200"/>
-      <c r="FP6" s="200"/>
-      <c r="FQ6" s="200"/>
-      <c r="FR6" s="200"/>
-      <c r="FS6" s="200"/>
-      <c r="FT6" s="200"/>
-      <c r="FU6" s="200"/>
-      <c r="FV6" s="200"/>
-      <c r="FW6" s="200"/>
-      <c r="FX6" s="200"/>
-      <c r="FY6" s="200"/>
-      <c r="FZ6" s="201"/>
-      <c r="GA6" s="195">
+      <c r="EX6" s="201"/>
+      <c r="EY6" s="201"/>
+      <c r="EZ6" s="201"/>
+      <c r="FA6" s="201"/>
+      <c r="FB6" s="201"/>
+      <c r="FC6" s="201"/>
+      <c r="FD6" s="201"/>
+      <c r="FE6" s="201"/>
+      <c r="FF6" s="201"/>
+      <c r="FG6" s="201"/>
+      <c r="FH6" s="201"/>
+      <c r="FI6" s="201"/>
+      <c r="FJ6" s="201"/>
+      <c r="FK6" s="201"/>
+      <c r="FL6" s="201"/>
+      <c r="FM6" s="201"/>
+      <c r="FN6" s="201"/>
+      <c r="FO6" s="201"/>
+      <c r="FP6" s="201"/>
+      <c r="FQ6" s="201"/>
+      <c r="FR6" s="201"/>
+      <c r="FS6" s="201"/>
+      <c r="FT6" s="201"/>
+      <c r="FU6" s="201"/>
+      <c r="FV6" s="201"/>
+      <c r="FW6" s="201"/>
+      <c r="FX6" s="201"/>
+      <c r="FY6" s="201"/>
+      <c r="FZ6" s="202"/>
+      <c r="GA6" s="196">
         <v>7</v>
       </c>
-      <c r="GB6" s="195"/>
-      <c r="GC6" s="195"/>
-      <c r="GD6" s="195"/>
-      <c r="GE6" s="195"/>
-      <c r="GF6" s="195"/>
-      <c r="GG6" s="195"/>
-      <c r="GH6" s="195"/>
-      <c r="GI6" s="195"/>
-      <c r="GJ6" s="195"/>
-      <c r="GK6" s="195"/>
-      <c r="GL6" s="195"/>
-      <c r="GM6" s="195"/>
-      <c r="GN6" s="195"/>
-      <c r="GO6" s="195"/>
-      <c r="GP6" s="195"/>
-      <c r="GQ6" s="195"/>
-      <c r="GR6" s="195"/>
-      <c r="GS6" s="195"/>
-      <c r="GT6" s="195"/>
-      <c r="GU6" s="195"/>
-      <c r="GV6" s="195"/>
-      <c r="GW6" s="195"/>
-      <c r="GX6" s="195"/>
-      <c r="GY6" s="195"/>
-      <c r="GZ6" s="195"/>
-      <c r="HA6" s="195"/>
-      <c r="HB6" s="195"/>
-      <c r="HC6" s="195"/>
-      <c r="HD6" s="195"/>
-      <c r="HE6" s="196"/>
-      <c r="HF6" s="195">
+      <c r="GB6" s="196"/>
+      <c r="GC6" s="196"/>
+      <c r="GD6" s="196"/>
+      <c r="GE6" s="196"/>
+      <c r="GF6" s="196"/>
+      <c r="GG6" s="196"/>
+      <c r="GH6" s="196"/>
+      <c r="GI6" s="196"/>
+      <c r="GJ6" s="196"/>
+      <c r="GK6" s="196"/>
+      <c r="GL6" s="196"/>
+      <c r="GM6" s="196"/>
+      <c r="GN6" s="196"/>
+      <c r="GO6" s="196"/>
+      <c r="GP6" s="196"/>
+      <c r="GQ6" s="196"/>
+      <c r="GR6" s="196"/>
+      <c r="GS6" s="196"/>
+      <c r="GT6" s="196"/>
+      <c r="GU6" s="196"/>
+      <c r="GV6" s="196"/>
+      <c r="GW6" s="196"/>
+      <c r="GX6" s="196"/>
+      <c r="GY6" s="196"/>
+      <c r="GZ6" s="196"/>
+      <c r="HA6" s="196"/>
+      <c r="HB6" s="196"/>
+      <c r="HC6" s="196"/>
+      <c r="HD6" s="196"/>
+      <c r="HE6" s="197"/>
+      <c r="HF6" s="196">
         <v>8</v>
       </c>
-      <c r="HG6" s="195"/>
-      <c r="HH6" s="195"/>
-      <c r="HI6" s="195"/>
-      <c r="HJ6" s="195"/>
-      <c r="HK6" s="195"/>
-      <c r="HL6" s="195"/>
-      <c r="HM6" s="195"/>
-      <c r="HN6" s="195"/>
-      <c r="HO6" s="195"/>
-      <c r="HP6" s="195"/>
-      <c r="HQ6" s="195"/>
-      <c r="HR6" s="195"/>
-      <c r="HS6" s="195"/>
-      <c r="HT6" s="195"/>
-      <c r="HU6" s="195"/>
-      <c r="HV6" s="195"/>
-      <c r="HW6" s="195"/>
-      <c r="HX6" s="195"/>
-      <c r="HY6" s="195"/>
-      <c r="HZ6" s="195"/>
-      <c r="IA6" s="195"/>
-      <c r="IB6" s="195"/>
-      <c r="IC6" s="195"/>
-      <c r="ID6" s="195"/>
-      <c r="IE6" s="195"/>
-      <c r="IF6" s="195"/>
-      <c r="IG6" s="195"/>
-      <c r="IH6" s="195"/>
-      <c r="II6" s="195"/>
-      <c r="IJ6" s="196"/>
-      <c r="IK6" s="199">
+      <c r="HG6" s="196"/>
+      <c r="HH6" s="196"/>
+      <c r="HI6" s="196"/>
+      <c r="HJ6" s="196"/>
+      <c r="HK6" s="196"/>
+      <c r="HL6" s="196"/>
+      <c r="HM6" s="196"/>
+      <c r="HN6" s="196"/>
+      <c r="HO6" s="196"/>
+      <c r="HP6" s="196"/>
+      <c r="HQ6" s="196"/>
+      <c r="HR6" s="196"/>
+      <c r="HS6" s="196"/>
+      <c r="HT6" s="196"/>
+      <c r="HU6" s="196"/>
+      <c r="HV6" s="196"/>
+      <c r="HW6" s="196"/>
+      <c r="HX6" s="196"/>
+      <c r="HY6" s="196"/>
+      <c r="HZ6" s="196"/>
+      <c r="IA6" s="196"/>
+      <c r="IB6" s="196"/>
+      <c r="IC6" s="196"/>
+      <c r="ID6" s="196"/>
+      <c r="IE6" s="196"/>
+      <c r="IF6" s="196"/>
+      <c r="IG6" s="196"/>
+      <c r="IH6" s="196"/>
+      <c r="II6" s="196"/>
+      <c r="IJ6" s="197"/>
+      <c r="IK6" s="200">
         <v>9</v>
       </c>
-      <c r="IL6" s="200"/>
-      <c r="IM6" s="200"/>
-      <c r="IN6" s="200"/>
-      <c r="IO6" s="200"/>
-      <c r="IP6" s="200"/>
-      <c r="IQ6" s="200"/>
-      <c r="IR6" s="200"/>
-      <c r="IS6" s="200"/>
-      <c r="IT6" s="200"/>
-      <c r="IU6" s="200"/>
-      <c r="IV6" s="200"/>
-      <c r="IW6" s="200"/>
-      <c r="IX6" s="200"/>
-      <c r="IY6" s="200"/>
-      <c r="IZ6" s="200"/>
-      <c r="JA6" s="200"/>
-      <c r="JB6" s="200"/>
-      <c r="JC6" s="200"/>
-      <c r="JD6" s="200"/>
-      <c r="JE6" s="200"/>
-      <c r="JF6" s="200"/>
-      <c r="JG6" s="200"/>
-      <c r="JH6" s="200"/>
-      <c r="JI6" s="200"/>
-      <c r="JJ6" s="200"/>
-      <c r="JK6" s="200"/>
-      <c r="JL6" s="200"/>
-      <c r="JM6" s="200"/>
-      <c r="JN6" s="201"/>
-      <c r="JO6" s="195">
+      <c r="IL6" s="201"/>
+      <c r="IM6" s="201"/>
+      <c r="IN6" s="201"/>
+      <c r="IO6" s="201"/>
+      <c r="IP6" s="201"/>
+      <c r="IQ6" s="201"/>
+      <c r="IR6" s="201"/>
+      <c r="IS6" s="201"/>
+      <c r="IT6" s="201"/>
+      <c r="IU6" s="201"/>
+      <c r="IV6" s="201"/>
+      <c r="IW6" s="201"/>
+      <c r="IX6" s="201"/>
+      <c r="IY6" s="201"/>
+      <c r="IZ6" s="201"/>
+      <c r="JA6" s="201"/>
+      <c r="JB6" s="201"/>
+      <c r="JC6" s="201"/>
+      <c r="JD6" s="201"/>
+      <c r="JE6" s="201"/>
+      <c r="JF6" s="201"/>
+      <c r="JG6" s="201"/>
+      <c r="JH6" s="201"/>
+      <c r="JI6" s="201"/>
+      <c r="JJ6" s="201"/>
+      <c r="JK6" s="201"/>
+      <c r="JL6" s="201"/>
+      <c r="JM6" s="201"/>
+      <c r="JN6" s="202"/>
+      <c r="JO6" s="196">
         <v>10</v>
       </c>
-      <c r="JP6" s="195"/>
-      <c r="JQ6" s="195"/>
-      <c r="JR6" s="195"/>
-      <c r="JS6" s="195"/>
-      <c r="JT6" s="195"/>
-      <c r="JU6" s="195"/>
-      <c r="JV6" s="195"/>
-      <c r="JW6" s="195"/>
-      <c r="JX6" s="195"/>
-      <c r="JY6" s="195"/>
-      <c r="JZ6" s="195"/>
-      <c r="KA6" s="195"/>
-      <c r="KB6" s="195"/>
-      <c r="KC6" s="195"/>
-      <c r="KD6" s="195"/>
-      <c r="KE6" s="195"/>
-      <c r="KF6" s="195"/>
-      <c r="KG6" s="195"/>
-      <c r="KH6" s="195"/>
-      <c r="KI6" s="195"/>
-      <c r="KJ6" s="195"/>
-      <c r="KK6" s="195"/>
-      <c r="KL6" s="195"/>
-      <c r="KM6" s="195"/>
-      <c r="KN6" s="195"/>
-      <c r="KO6" s="195"/>
-      <c r="KP6" s="195"/>
-      <c r="KQ6" s="195"/>
-      <c r="KR6" s="195"/>
-      <c r="KS6" s="196"/>
-      <c r="KT6" s="199">
+      <c r="JP6" s="196"/>
+      <c r="JQ6" s="196"/>
+      <c r="JR6" s="196"/>
+      <c r="JS6" s="196"/>
+      <c r="JT6" s="196"/>
+      <c r="JU6" s="196"/>
+      <c r="JV6" s="196"/>
+      <c r="JW6" s="196"/>
+      <c r="JX6" s="196"/>
+      <c r="JY6" s="196"/>
+      <c r="JZ6" s="196"/>
+      <c r="KA6" s="196"/>
+      <c r="KB6" s="196"/>
+      <c r="KC6" s="196"/>
+      <c r="KD6" s="196"/>
+      <c r="KE6" s="196"/>
+      <c r="KF6" s="196"/>
+      <c r="KG6" s="196"/>
+      <c r="KH6" s="196"/>
+      <c r="KI6" s="196"/>
+      <c r="KJ6" s="196"/>
+      <c r="KK6" s="196"/>
+      <c r="KL6" s="196"/>
+      <c r="KM6" s="196"/>
+      <c r="KN6" s="196"/>
+      <c r="KO6" s="196"/>
+      <c r="KP6" s="196"/>
+      <c r="KQ6" s="196"/>
+      <c r="KR6" s="196"/>
+      <c r="KS6" s="197"/>
+      <c r="KT6" s="200">
         <v>11</v>
       </c>
-      <c r="KU6" s="200"/>
-      <c r="KV6" s="200"/>
-      <c r="KW6" s="200"/>
-      <c r="KX6" s="200"/>
-      <c r="KY6" s="200"/>
-      <c r="KZ6" s="200"/>
-      <c r="LA6" s="200"/>
-      <c r="LB6" s="200"/>
-      <c r="LC6" s="200"/>
-      <c r="LD6" s="200"/>
-      <c r="LE6" s="200"/>
-      <c r="LF6" s="200"/>
-      <c r="LG6" s="200"/>
-      <c r="LH6" s="200"/>
-      <c r="LI6" s="200"/>
-      <c r="LJ6" s="200"/>
-      <c r="LK6" s="200"/>
-      <c r="LL6" s="200"/>
-      <c r="LM6" s="200"/>
-      <c r="LN6" s="200"/>
-      <c r="LO6" s="200"/>
-      <c r="LP6" s="200"/>
-      <c r="LQ6" s="200"/>
-      <c r="LR6" s="200"/>
-      <c r="LS6" s="200"/>
-      <c r="LT6" s="200"/>
-      <c r="LU6" s="200"/>
-      <c r="LV6" s="200"/>
-      <c r="LW6" s="201"/>
-      <c r="LX6" s="195">
+      <c r="KU6" s="201"/>
+      <c r="KV6" s="201"/>
+      <c r="KW6" s="201"/>
+      <c r="KX6" s="201"/>
+      <c r="KY6" s="201"/>
+      <c r="KZ6" s="201"/>
+      <c r="LA6" s="201"/>
+      <c r="LB6" s="201"/>
+      <c r="LC6" s="201"/>
+      <c r="LD6" s="201"/>
+      <c r="LE6" s="201"/>
+      <c r="LF6" s="201"/>
+      <c r="LG6" s="201"/>
+      <c r="LH6" s="201"/>
+      <c r="LI6" s="201"/>
+      <c r="LJ6" s="201"/>
+      <c r="LK6" s="201"/>
+      <c r="LL6" s="201"/>
+      <c r="LM6" s="201"/>
+      <c r="LN6" s="201"/>
+      <c r="LO6" s="201"/>
+      <c r="LP6" s="201"/>
+      <c r="LQ6" s="201"/>
+      <c r="LR6" s="201"/>
+      <c r="LS6" s="201"/>
+      <c r="LT6" s="201"/>
+      <c r="LU6" s="201"/>
+      <c r="LV6" s="201"/>
+      <c r="LW6" s="202"/>
+      <c r="LX6" s="196">
         <v>12</v>
       </c>
-      <c r="LY6" s="195"/>
-      <c r="LZ6" s="195"/>
-      <c r="MA6" s="195"/>
-      <c r="MB6" s="195"/>
-      <c r="MC6" s="195"/>
-      <c r="MD6" s="195"/>
-      <c r="ME6" s="195"/>
-      <c r="MF6" s="195"/>
-      <c r="MG6" s="195"/>
-      <c r="MH6" s="195"/>
-      <c r="MI6" s="195"/>
-      <c r="MJ6" s="195"/>
-      <c r="MK6" s="195"/>
-      <c r="ML6" s="195"/>
-      <c r="MM6" s="195"/>
-      <c r="MN6" s="195"/>
-      <c r="MO6" s="195"/>
-      <c r="MP6" s="195"/>
-      <c r="MQ6" s="195"/>
-      <c r="MR6" s="195"/>
-      <c r="MS6" s="195"/>
-      <c r="MT6" s="195"/>
-      <c r="MU6" s="195"/>
-      <c r="MV6" s="195"/>
-      <c r="MW6" s="195"/>
-      <c r="MX6" s="195"/>
-      <c r="MY6" s="195"/>
-      <c r="MZ6" s="195"/>
-      <c r="NA6" s="195"/>
-      <c r="NB6" s="196"/>
+      <c r="LY6" s="196"/>
+      <c r="LZ6" s="196"/>
+      <c r="MA6" s="196"/>
+      <c r="MB6" s="196"/>
+      <c r="MC6" s="196"/>
+      <c r="MD6" s="196"/>
+      <c r="ME6" s="196"/>
+      <c r="MF6" s="196"/>
+      <c r="MG6" s="196"/>
+      <c r="MH6" s="196"/>
+      <c r="MI6" s="196"/>
+      <c r="MJ6" s="196"/>
+      <c r="MK6" s="196"/>
+      <c r="ML6" s="196"/>
+      <c r="MM6" s="196"/>
+      <c r="MN6" s="196"/>
+      <c r="MO6" s="196"/>
+      <c r="MP6" s="196"/>
+      <c r="MQ6" s="196"/>
+      <c r="MR6" s="196"/>
+      <c r="MS6" s="196"/>
+      <c r="MT6" s="196"/>
+      <c r="MU6" s="196"/>
+      <c r="MV6" s="196"/>
+      <c r="MW6" s="196"/>
+      <c r="MX6" s="196"/>
+      <c r="MY6" s="196"/>
+      <c r="MZ6" s="196"/>
+      <c r="NA6" s="196"/>
+      <c r="NB6" s="197"/>
     </row>
     <row r="7" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -36892,7 +36900,7 @@
       </c>
     </row>
     <row r="8" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="202" t="s">
+      <c r="A8" s="203" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="34"/>
@@ -37284,7 +37292,7 @@
       <c r="NB8" s="141"/>
     </row>
     <row r="9" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="202"/>
+      <c r="A9" s="203"/>
       <c r="B9" s="29"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -37664,7 +37672,7 @@
       <c r="NB9" s="32"/>
     </row>
     <row r="10" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="202"/>
+      <c r="A10" s="203"/>
       <c r="B10" s="29"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
@@ -38046,7 +38054,7 @@
       <c r="NB10" s="32"/>
     </row>
     <row r="11" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="202"/>
+      <c r="A11" s="203"/>
       <c r="B11" s="29"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
@@ -38422,7 +38430,7 @@
       <c r="NB11" s="32"/>
     </row>
     <row r="12" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="202"/>
+      <c r="A12" s="203"/>
       <c r="B12" s="29"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
@@ -38796,7 +38804,7 @@
       <c r="NB12" s="32"/>
     </row>
     <row r="13" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="202"/>
+      <c r="A13" s="203"/>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -39166,7 +39174,7 @@
       <c r="NB13" s="32"/>
     </row>
     <row r="14" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="202"/>
+      <c r="A14" s="203"/>
       <c r="B14" s="50"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51"/>
@@ -39536,7 +39544,7 @@
       <c r="NB14" s="65"/>
     </row>
     <row r="15" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="203" t="s">
+      <c r="A15" s="204" t="s">
         <v>62</v>
       </c>
       <c r="B15" s="75"/>
@@ -39916,7 +39924,7 @@
       <c r="NB15" s="84"/>
     </row>
     <row r="16" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="202"/>
+      <c r="A16" s="203"/>
       <c r="B16" s="24"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -40288,7 +40296,7 @@
       <c r="NB16" s="25"/>
     </row>
     <row r="17" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="202"/>
+      <c r="A17" s="203"/>
       <c r="B17" s="24"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -40656,7 +40664,7 @@
       <c r="NB17" s="25"/>
     </row>
     <row r="18" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="202"/>
+      <c r="A18" s="203"/>
       <c r="B18" s="24"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -41026,7 +41034,7 @@
       <c r="NB18" s="25"/>
     </row>
     <row r="19" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="202"/>
+      <c r="A19" s="203"/>
       <c r="B19" s="85"/>
       <c r="C19" s="71"/>
       <c r="D19" s="71"/>
@@ -41394,7 +41402,7 @@
       <c r="NB19" s="74"/>
     </row>
     <row r="20" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="202" t="s">
+      <c r="A20" s="203" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="42"/>
@@ -41778,7 +41786,7 @@
       <c r="NB20" s="84"/>
     </row>
     <row r="21" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="202"/>
+      <c r="A21" s="203"/>
       <c r="B21" s="24"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -42155,7 +42163,7 @@
       <c r="NB21" s="25"/>
     </row>
     <row r="22" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="202"/>
+      <c r="A22" s="203"/>
       <c r="B22" s="24"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -42535,7 +42543,7 @@
       <c r="NB22" s="25"/>
     </row>
     <row r="23" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="202"/>
+      <c r="A23" s="203"/>
       <c r="B23" s="24"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
@@ -42911,7 +42919,7 @@
       <c r="NB23" s="25"/>
     </row>
     <row r="24" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="202"/>
+      <c r="A24" s="203"/>
       <c r="B24" s="26"/>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
@@ -43281,7 +43289,7 @@
       <c r="NB24" s="74"/>
     </row>
     <row r="25" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="202" t="s">
+      <c r="A25" s="203" t="s">
         <v>17</v>
       </c>
       <c r="B25" s="75"/>
@@ -43661,7 +43669,7 @@
       <c r="NB25" s="84"/>
     </row>
     <row r="26" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="202"/>
+      <c r="A26" s="203"/>
       <c r="B26" s="24"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -44037,7 +44045,7 @@
       <c r="NB26" s="25"/>
     </row>
     <row r="27" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="202"/>
+      <c r="A27" s="203"/>
       <c r="B27" s="24"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
@@ -44409,7 +44417,7 @@
       <c r="NB27" s="25"/>
     </row>
     <row r="28" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="202"/>
+      <c r="A28" s="203"/>
       <c r="B28" s="24"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -44782,7 +44790,7 @@
       <c r="NB28" s="25"/>
     </row>
     <row r="29" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="202"/>
+      <c r="A29" s="203"/>
       <c r="B29" s="91"/>
       <c r="C29" s="92"/>
       <c r="D29" s="92"/>
@@ -44908,7 +44916,7 @@
       <c r="DT29" s="71"/>
       <c r="DU29" s="71"/>
       <c r="DV29" s="72"/>
-      <c r="DW29" s="212" t="s">
+      <c r="DW29" s="191" t="s">
         <v>146</v>
       </c>
       <c r="DX29" s="72"/>
@@ -45152,7 +45160,7 @@
       <c r="NB29" s="74"/>
     </row>
     <row r="30" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="203" t="s">
+      <c r="A30" s="204" t="s">
         <v>63</v>
       </c>
       <c r="B30" s="75"/>
@@ -45524,7 +45532,7 @@
       <c r="NB30" s="84"/>
     </row>
     <row r="31" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="202"/>
+      <c r="A31" s="203"/>
       <c r="B31" s="24"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -45898,7 +45906,7 @@
       <c r="NB31" s="25"/>
     </row>
     <row r="32" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="202"/>
+      <c r="A32" s="203"/>
       <c r="B32" s="24"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
@@ -46272,7 +46280,7 @@
       <c r="NB32" s="25"/>
     </row>
     <row r="33" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="202"/>
+      <c r="A33" s="203"/>
       <c r="B33" s="24"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
@@ -46642,7 +46650,7 @@
       <c r="NB33" s="25"/>
     </row>
     <row r="34" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="202"/>
+      <c r="A34" s="203"/>
       <c r="B34" s="85"/>
       <c r="C34" s="71"/>
       <c r="D34" s="71"/>
@@ -47010,7 +47018,7 @@
       <c r="NB34" s="74"/>
     </row>
     <row r="35" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="202" t="s">
+      <c r="A35" s="203" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="42"/>
@@ -47392,7 +47400,7 @@
       <c r="NB35" s="47"/>
     </row>
     <row r="36" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="202"/>
+      <c r="A36" s="203"/>
       <c r="B36" s="24"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
@@ -47764,7 +47772,7 @@
       <c r="NB36" s="25"/>
     </row>
     <row r="37" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="202"/>
+      <c r="A37" s="203"/>
       <c r="B37" s="24"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -48140,7 +48148,7 @@
       <c r="NB37" s="25"/>
     </row>
     <row r="38" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="202"/>
+      <c r="A38" s="203"/>
       <c r="B38" s="24"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
@@ -48514,7 +48522,7 @@
       <c r="NB38" s="25"/>
     </row>
     <row r="39" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="202"/>
+      <c r="A39" s="203"/>
       <c r="B39" s="85"/>
       <c r="C39" s="71"/>
       <c r="D39" s="71"/>
@@ -48886,7 +48894,7 @@
       <c r="NB39" s="74"/>
     </row>
     <row r="40" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="202" t="s">
+      <c r="A40" s="203" t="s">
         <v>23</v>
       </c>
       <c r="B40" s="75"/>
@@ -49264,7 +49272,7 @@
       <c r="NB40" s="84"/>
     </row>
     <row r="41" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="202"/>
+      <c r="A41" s="203"/>
       <c r="B41" s="24"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
@@ -49398,7 +49406,7 @@
         <v>0</v>
       </c>
       <c r="DV41" s="14"/>
-      <c r="DW41" s="14"/>
+      <c r="DW41" s="56"/>
       <c r="DX41" s="14"/>
       <c r="DY41" s="16"/>
       <c r="DZ41" s="16"/>
@@ -49640,7 +49648,7 @@
       <c r="NB41" s="25"/>
     </row>
     <row r="42" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="202"/>
+      <c r="A42" s="203"/>
       <c r="B42" s="24"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -50010,7 +50018,7 @@
       <c r="NB42" s="25"/>
     </row>
     <row r="43" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="202"/>
+      <c r="A43" s="203"/>
       <c r="B43" s="24"/>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
@@ -50380,7 +50388,7 @@
       <c r="NB43" s="25"/>
     </row>
     <row r="44" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="202"/>
+      <c r="A44" s="203"/>
       <c r="B44" s="85"/>
       <c r="C44" s="71"/>
       <c r="D44" s="71"/>
@@ -50748,7 +50756,7 @@
       <c r="NB44" s="74"/>
     </row>
     <row r="45" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="202" t="s">
+      <c r="A45" s="203" t="s">
         <v>22</v>
       </c>
       <c r="B45" s="75"/>
@@ -51128,7 +51136,7 @@
       <c r="NB45" s="84"/>
     </row>
     <row r="46" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="202"/>
+      <c r="A46" s="203"/>
       <c r="B46" s="24"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
@@ -51498,7 +51506,7 @@
       <c r="NB46" s="25"/>
     </row>
     <row r="47" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="202"/>
+      <c r="A47" s="203"/>
       <c r="B47" s="24"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
@@ -51874,7 +51882,7 @@
       <c r="NB47" s="25"/>
     </row>
     <row r="48" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="202"/>
+      <c r="A48" s="203"/>
       <c r="B48" s="24"/>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -52244,7 +52252,7 @@
       <c r="NB48" s="25"/>
     </row>
     <row r="49" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="202"/>
+      <c r="A49" s="203"/>
       <c r="B49" s="85"/>
       <c r="C49" s="71"/>
       <c r="D49" s="71"/>
@@ -52618,7 +52626,7 @@
       <c r="NB49" s="74"/>
     </row>
     <row r="50" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="202" t="s">
+      <c r="A50" s="203" t="s">
         <v>24</v>
       </c>
       <c r="B50" s="75"/>
@@ -53000,7 +53008,7 @@
       <c r="NB50" s="84"/>
     </row>
     <row r="51" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="202"/>
+      <c r="A51" s="203"/>
       <c r="B51" s="24"/>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
@@ -53378,7 +53386,7 @@
       <c r="NB51" s="25"/>
     </row>
     <row r="52" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="202"/>
+      <c r="A52" s="203"/>
       <c r="B52" s="24"/>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
@@ -53750,7 +53758,7 @@
       <c r="NB52" s="25"/>
     </row>
     <row r="53" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="202"/>
+      <c r="A53" s="203"/>
       <c r="B53" s="24"/>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
@@ -54120,7 +54128,7 @@
       <c r="NB53" s="25"/>
     </row>
     <row r="54" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="202"/>
+      <c r="A54" s="203"/>
       <c r="B54" s="85"/>
       <c r="C54" s="71"/>
       <c r="D54" s="71"/>
@@ -54508,6 +54516,15 @@
     <row r="71" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="A35:A39"/>
     <mergeCell ref="LX6:NB6"/>
     <mergeCell ref="B6:AF6"/>
     <mergeCell ref="AG6:BH6"/>
@@ -54520,15 +54537,6 @@
     <mergeCell ref="IK6:JN6"/>
     <mergeCell ref="JO6:KS6"/>
     <mergeCell ref="KT6:LW6"/>
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="A45:A49"/>
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A30:A34"/>
-    <mergeCell ref="A35:A39"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -54543,7 +54551,7 @@
   <dimension ref="B1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -54557,20 +54565,20 @@
   <sheetData>
     <row r="1" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="204" t="s">
+      <c r="B2" s="205" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="206" t="s">
+      <c r="C2" s="207" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="207"/>
-      <c r="E2" s="208" t="s">
+      <c r="D2" s="208"/>
+      <c r="E2" s="209" t="s">
         <v>127</v>
       </c>
-      <c r="F2" s="207"/>
+      <c r="F2" s="208"/>
     </row>
     <row r="3" spans="2:6" s="167" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="205"/>
+      <c r="B3" s="206"/>
       <c r="C3" s="174" t="s">
         <v>122</v>
       </c>
@@ -54602,7 +54610,7 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="209">
+      <c r="B5" s="210">
         <v>43219</v>
       </c>
       <c r="C5" s="183">
@@ -54619,7 +54627,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="211"/>
+      <c r="B6" s="212"/>
       <c r="C6" s="183"/>
       <c r="D6" s="184"/>
       <c r="E6" s="185">
@@ -54643,7 +54651,7 @@
       <c r="F7" s="184"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="209">
+      <c r="B8" s="210">
         <v>43221</v>
       </c>
       <c r="C8" s="190">
@@ -54660,7 +54668,7 @@
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="210"/>
+      <c r="B9" s="211"/>
       <c r="C9" s="190">
         <v>2</v>
       </c>
@@ -54671,7 +54679,7 @@
       <c r="F9" s="184"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="210"/>
+      <c r="B10" s="211"/>
       <c r="C10" s="190">
         <v>1</v>
       </c>
@@ -54682,7 +54690,7 @@
       <c r="F10" s="184"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="211"/>
+      <c r="B11" s="212"/>
       <c r="C11" s="190">
         <v>1</v>
       </c>
@@ -54745,8 +54753,12 @@
       <c r="B15" s="187">
         <v>43226</v>
       </c>
-      <c r="C15" s="183"/>
-      <c r="D15" s="184"/>
+      <c r="C15" s="183">
+        <v>1</v>
+      </c>
+      <c r="D15" s="184" t="s">
+        <v>152</v>
+      </c>
       <c r="E15" s="185">
         <v>3</v>
       </c>
@@ -54769,8 +54781,12 @@
       <c r="B17" s="187"/>
       <c r="C17" s="183"/>
       <c r="D17" s="184"/>
-      <c r="E17" s="185"/>
-      <c r="F17" s="184"/>
+      <c r="E17" s="185">
+        <v>3</v>
+      </c>
+      <c r="F17" s="184" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="187"/>

</xml_diff>

<commit_message>
[GEN MAIN] working time update
</commit_message>
<xml_diff>
--- a/Femto Project schedule V1.0.xlsx
+++ b/Femto Project schedule V1.0.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="20180207" sheetId="18" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <author>만든 이</author>
   </authors>
   <commentList>
-    <comment ref="EM7" authorId="0">
+    <comment ref="EM7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -42,7 +42,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FB7" authorId="0">
+    <comment ref="FB7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FI7" authorId="0">
+    <comment ref="FI7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="HT7" authorId="0">
+    <comment ref="HT7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -87,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="JH7" authorId="0">
+    <comment ref="JH7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="JQ7" authorId="0">
+    <comment ref="JQ7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -117,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="JW7" authorId="0">
+    <comment ref="JW7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -132,7 +132,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="MV7" authorId="0">
+    <comment ref="MV7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -157,7 +157,7 @@
     <author>만든 이</author>
   </authors>
   <commentList>
-    <comment ref="EM7" authorId="0">
+    <comment ref="EM7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -172,7 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FB7" authorId="0">
+    <comment ref="FB7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -187,7 +187,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FI7" authorId="0">
+    <comment ref="FI7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -202,7 +202,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="HT7" authorId="0">
+    <comment ref="HT7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -217,7 +217,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="JH7" authorId="0">
+    <comment ref="JH7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -232,7 +232,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="JQ7" authorId="0">
+    <comment ref="JQ7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -247,7 +247,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="JW7" authorId="0">
+    <comment ref="JW7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -262,7 +262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="MV7" authorId="0">
+    <comment ref="MV7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="154">
   <si>
     <t>◇PCB설계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -896,6 +896,10 @@
   </si>
   <si>
     <t>LF Gen Main Schematic design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LF Gen Main Simulation - Tr current</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1688,7 +1692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="213">
+  <cellXfs count="214">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1957,6 +1961,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -8648,7 +8653,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8683,7 +8688,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8932,167 +8937,167 @@
     </row>
     <row r="6" spans="1:152" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="199">
+      <c r="B6" s="200">
         <v>1</v>
       </c>
-      <c r="C6" s="196"/>
-      <c r="D6" s="196"/>
-      <c r="E6" s="196"/>
-      <c r="F6" s="196"/>
-      <c r="G6" s="196"/>
-      <c r="H6" s="196"/>
-      <c r="I6" s="196"/>
-      <c r="J6" s="196"/>
-      <c r="K6" s="196"/>
-      <c r="L6" s="196"/>
-      <c r="M6" s="196"/>
-      <c r="N6" s="196"/>
-      <c r="O6" s="196"/>
-      <c r="P6" s="196"/>
-      <c r="Q6" s="196"/>
-      <c r="R6" s="196"/>
-      <c r="S6" s="196"/>
-      <c r="T6" s="196"/>
-      <c r="U6" s="196"/>
-      <c r="V6" s="196"/>
-      <c r="W6" s="196"/>
-      <c r="X6" s="196"/>
-      <c r="Y6" s="196"/>
-      <c r="Z6" s="196"/>
-      <c r="AA6" s="196"/>
-      <c r="AB6" s="196"/>
-      <c r="AC6" s="196"/>
-      <c r="AD6" s="196"/>
-      <c r="AE6" s="196"/>
-      <c r="AF6" s="196"/>
-      <c r="AG6" s="199">
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="197"/>
+      <c r="F6" s="197"/>
+      <c r="G6" s="197"/>
+      <c r="H6" s="197"/>
+      <c r="I6" s="197"/>
+      <c r="J6" s="197"/>
+      <c r="K6" s="197"/>
+      <c r="L6" s="197"/>
+      <c r="M6" s="197"/>
+      <c r="N6" s="197"/>
+      <c r="O6" s="197"/>
+      <c r="P6" s="197"/>
+      <c r="Q6" s="197"/>
+      <c r="R6" s="197"/>
+      <c r="S6" s="197"/>
+      <c r="T6" s="197"/>
+      <c r="U6" s="197"/>
+      <c r="V6" s="197"/>
+      <c r="W6" s="197"/>
+      <c r="X6" s="197"/>
+      <c r="Y6" s="197"/>
+      <c r="Z6" s="197"/>
+      <c r="AA6" s="197"/>
+      <c r="AB6" s="197"/>
+      <c r="AC6" s="197"/>
+      <c r="AD6" s="197"/>
+      <c r="AE6" s="197"/>
+      <c r="AF6" s="197"/>
+      <c r="AG6" s="200">
         <v>2</v>
       </c>
-      <c r="AH6" s="196"/>
-      <c r="AI6" s="196"/>
-      <c r="AJ6" s="196"/>
-      <c r="AK6" s="196"/>
-      <c r="AL6" s="196"/>
-      <c r="AM6" s="196"/>
-      <c r="AN6" s="196"/>
-      <c r="AO6" s="196"/>
-      <c r="AP6" s="196"/>
-      <c r="AQ6" s="196"/>
-      <c r="AR6" s="196"/>
-      <c r="AS6" s="196"/>
-      <c r="AT6" s="196"/>
-      <c r="AU6" s="196"/>
-      <c r="AV6" s="196"/>
-      <c r="AW6" s="196"/>
-      <c r="AX6" s="196"/>
-      <c r="AY6" s="196"/>
-      <c r="AZ6" s="196"/>
-      <c r="BA6" s="196"/>
-      <c r="BB6" s="196"/>
-      <c r="BC6" s="196"/>
-      <c r="BD6" s="196"/>
-      <c r="BE6" s="196"/>
-      <c r="BF6" s="196"/>
-      <c r="BG6" s="196"/>
-      <c r="BH6" s="197"/>
-      <c r="BI6" s="196">
+      <c r="AH6" s="197"/>
+      <c r="AI6" s="197"/>
+      <c r="AJ6" s="197"/>
+      <c r="AK6" s="197"/>
+      <c r="AL6" s="197"/>
+      <c r="AM6" s="197"/>
+      <c r="AN6" s="197"/>
+      <c r="AO6" s="197"/>
+      <c r="AP6" s="197"/>
+      <c r="AQ6" s="197"/>
+      <c r="AR6" s="197"/>
+      <c r="AS6" s="197"/>
+      <c r="AT6" s="197"/>
+      <c r="AU6" s="197"/>
+      <c r="AV6" s="197"/>
+      <c r="AW6" s="197"/>
+      <c r="AX6" s="197"/>
+      <c r="AY6" s="197"/>
+      <c r="AZ6" s="197"/>
+      <c r="BA6" s="197"/>
+      <c r="BB6" s="197"/>
+      <c r="BC6" s="197"/>
+      <c r="BD6" s="197"/>
+      <c r="BE6" s="197"/>
+      <c r="BF6" s="197"/>
+      <c r="BG6" s="197"/>
+      <c r="BH6" s="198"/>
+      <c r="BI6" s="197">
         <v>3</v>
       </c>
-      <c r="BJ6" s="196"/>
-      <c r="BK6" s="196"/>
-      <c r="BL6" s="196"/>
-      <c r="BM6" s="196"/>
-      <c r="BN6" s="196"/>
-      <c r="BO6" s="196"/>
-      <c r="BP6" s="196"/>
-      <c r="BQ6" s="196"/>
-      <c r="BR6" s="196"/>
-      <c r="BS6" s="196"/>
-      <c r="BT6" s="196"/>
-      <c r="BU6" s="196"/>
-      <c r="BV6" s="196"/>
-      <c r="BW6" s="196"/>
-      <c r="BX6" s="196"/>
-      <c r="BY6" s="196"/>
-      <c r="BZ6" s="196"/>
-      <c r="CA6" s="196"/>
-      <c r="CB6" s="196"/>
-      <c r="CC6" s="196"/>
-      <c r="CD6" s="196"/>
-      <c r="CE6" s="196"/>
-      <c r="CF6" s="196"/>
-      <c r="CG6" s="196"/>
-      <c r="CH6" s="196"/>
-      <c r="CI6" s="196"/>
-      <c r="CJ6" s="196"/>
-      <c r="CK6" s="196"/>
-      <c r="CL6" s="196"/>
-      <c r="CM6" s="196"/>
-      <c r="CN6" s="200">
+      <c r="BJ6" s="197"/>
+      <c r="BK6" s="197"/>
+      <c r="BL6" s="197"/>
+      <c r="BM6" s="197"/>
+      <c r="BN6" s="197"/>
+      <c r="BO6" s="197"/>
+      <c r="BP6" s="197"/>
+      <c r="BQ6" s="197"/>
+      <c r="BR6" s="197"/>
+      <c r="BS6" s="197"/>
+      <c r="BT6" s="197"/>
+      <c r="BU6" s="197"/>
+      <c r="BV6" s="197"/>
+      <c r="BW6" s="197"/>
+      <c r="BX6" s="197"/>
+      <c r="BY6" s="197"/>
+      <c r="BZ6" s="197"/>
+      <c r="CA6" s="197"/>
+      <c r="CB6" s="197"/>
+      <c r="CC6" s="197"/>
+      <c r="CD6" s="197"/>
+      <c r="CE6" s="197"/>
+      <c r="CF6" s="197"/>
+      <c r="CG6" s="197"/>
+      <c r="CH6" s="197"/>
+      <c r="CI6" s="197"/>
+      <c r="CJ6" s="197"/>
+      <c r="CK6" s="197"/>
+      <c r="CL6" s="197"/>
+      <c r="CM6" s="197"/>
+      <c r="CN6" s="201">
         <v>4</v>
       </c>
-      <c r="CO6" s="201"/>
-      <c r="CP6" s="201"/>
-      <c r="CQ6" s="201"/>
-      <c r="CR6" s="201"/>
-      <c r="CS6" s="201"/>
-      <c r="CT6" s="201"/>
-      <c r="CU6" s="201"/>
-      <c r="CV6" s="201"/>
-      <c r="CW6" s="201"/>
-      <c r="CX6" s="201"/>
-      <c r="CY6" s="201"/>
-      <c r="CZ6" s="201"/>
-      <c r="DA6" s="201"/>
-      <c r="DB6" s="201"/>
-      <c r="DC6" s="201"/>
-      <c r="DD6" s="201"/>
-      <c r="DE6" s="201"/>
-      <c r="DF6" s="201"/>
-      <c r="DG6" s="201"/>
-      <c r="DH6" s="201"/>
-      <c r="DI6" s="201"/>
-      <c r="DJ6" s="201"/>
-      <c r="DK6" s="201"/>
-      <c r="DL6" s="201"/>
-      <c r="DM6" s="201"/>
-      <c r="DN6" s="201"/>
-      <c r="DO6" s="201"/>
-      <c r="DP6" s="201"/>
-      <c r="DQ6" s="202"/>
-      <c r="DR6" s="196">
+      <c r="CO6" s="202"/>
+      <c r="CP6" s="202"/>
+      <c r="CQ6" s="202"/>
+      <c r="CR6" s="202"/>
+      <c r="CS6" s="202"/>
+      <c r="CT6" s="202"/>
+      <c r="CU6" s="202"/>
+      <c r="CV6" s="202"/>
+      <c r="CW6" s="202"/>
+      <c r="CX6" s="202"/>
+      <c r="CY6" s="202"/>
+      <c r="CZ6" s="202"/>
+      <c r="DA6" s="202"/>
+      <c r="DB6" s="202"/>
+      <c r="DC6" s="202"/>
+      <c r="DD6" s="202"/>
+      <c r="DE6" s="202"/>
+      <c r="DF6" s="202"/>
+      <c r="DG6" s="202"/>
+      <c r="DH6" s="202"/>
+      <c r="DI6" s="202"/>
+      <c r="DJ6" s="202"/>
+      <c r="DK6" s="202"/>
+      <c r="DL6" s="202"/>
+      <c r="DM6" s="202"/>
+      <c r="DN6" s="202"/>
+      <c r="DO6" s="202"/>
+      <c r="DP6" s="202"/>
+      <c r="DQ6" s="203"/>
+      <c r="DR6" s="197">
         <v>5</v>
       </c>
-      <c r="DS6" s="196"/>
-      <c r="DT6" s="196"/>
-      <c r="DU6" s="196"/>
-      <c r="DV6" s="196"/>
-      <c r="DW6" s="196"/>
-      <c r="DX6" s="196"/>
-      <c r="DY6" s="196"/>
-      <c r="DZ6" s="196"/>
-      <c r="EA6" s="196"/>
-      <c r="EB6" s="196"/>
-      <c r="EC6" s="196"/>
-      <c r="ED6" s="196"/>
-      <c r="EE6" s="196"/>
-      <c r="EF6" s="196"/>
-      <c r="EG6" s="196"/>
-      <c r="EH6" s="196"/>
-      <c r="EI6" s="196"/>
-      <c r="EJ6" s="196"/>
-      <c r="EK6" s="196"/>
-      <c r="EL6" s="196"/>
-      <c r="EM6" s="196"/>
-      <c r="EN6" s="196"/>
-      <c r="EO6" s="196"/>
-      <c r="EP6" s="196"/>
-      <c r="EQ6" s="196"/>
-      <c r="ER6" s="196"/>
-      <c r="ES6" s="196"/>
-      <c r="ET6" s="196"/>
-      <c r="EU6" s="196"/>
-      <c r="EV6" s="197"/>
+      <c r="DS6" s="197"/>
+      <c r="DT6" s="197"/>
+      <c r="DU6" s="197"/>
+      <c r="DV6" s="197"/>
+      <c r="DW6" s="197"/>
+      <c r="DX6" s="197"/>
+      <c r="DY6" s="197"/>
+      <c r="DZ6" s="197"/>
+      <c r="EA6" s="197"/>
+      <c r="EB6" s="197"/>
+      <c r="EC6" s="197"/>
+      <c r="ED6" s="197"/>
+      <c r="EE6" s="197"/>
+      <c r="EF6" s="197"/>
+      <c r="EG6" s="197"/>
+      <c r="EH6" s="197"/>
+      <c r="EI6" s="197"/>
+      <c r="EJ6" s="197"/>
+      <c r="EK6" s="197"/>
+      <c r="EL6" s="197"/>
+      <c r="EM6" s="197"/>
+      <c r="EN6" s="197"/>
+      <c r="EO6" s="197"/>
+      <c r="EP6" s="197"/>
+      <c r="EQ6" s="197"/>
+      <c r="ER6" s="197"/>
+      <c r="ES6" s="197"/>
+      <c r="ET6" s="197"/>
+      <c r="EU6" s="197"/>
+      <c r="EV6" s="198"/>
     </row>
     <row r="7" spans="1:152" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -9551,7 +9556,7 @@
       </c>
     </row>
     <row r="8" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A8" s="193" t="s">
+      <c r="A8" s="194" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="34"/>
@@ -9715,7 +9720,7 @@
       <c r="EV8" s="99"/>
     </row>
     <row r="9" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A9" s="193"/>
+      <c r="A9" s="194"/>
       <c r="B9" s="29"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -9875,7 +9880,7 @@
       <c r="EV9" s="33"/>
     </row>
     <row r="10" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A10" s="193"/>
+      <c r="A10" s="194"/>
       <c r="B10" s="29"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
@@ -10035,7 +10040,7 @@
       <c r="EV10" s="33"/>
     </row>
     <row r="11" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A11" s="193"/>
+      <c r="A11" s="194"/>
       <c r="B11" s="29"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
@@ -10193,7 +10198,7 @@
       <c r="EV11" s="33"/>
     </row>
     <row r="12" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A12" s="193"/>
+      <c r="A12" s="194"/>
       <c r="B12" s="29"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
@@ -10351,7 +10356,7 @@
       <c r="EV12" s="33"/>
     </row>
     <row r="13" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A13" s="193"/>
+      <c r="A13" s="194"/>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -10507,7 +10512,7 @@
       <c r="EV13" s="33"/>
     </row>
     <row r="14" spans="1:152" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="198"/>
+      <c r="A14" s="199"/>
       <c r="B14" s="50"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51"/>
@@ -10661,7 +10666,7 @@
       <c r="EV14" s="100"/>
     </row>
     <row r="15" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A15" s="195" t="s">
+      <c r="A15" s="196" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="42"/>
@@ -10823,7 +10828,7 @@
       <c r="EV15" s="102"/>
     </row>
     <row r="16" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A16" s="193"/>
+      <c r="A16" s="194"/>
       <c r="B16" s="24"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -10981,7 +10986,7 @@
       <c r="EV16" s="17"/>
     </row>
     <row r="17" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A17" s="193"/>
+      <c r="A17" s="194"/>
       <c r="B17" s="24"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -11141,7 +11146,7 @@
       <c r="EV17" s="17"/>
     </row>
     <row r="18" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A18" s="193"/>
+      <c r="A18" s="194"/>
       <c r="B18" s="24"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -11297,7 +11302,7 @@
       <c r="EV18" s="17"/>
     </row>
     <row r="19" spans="1:152" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="193"/>
+      <c r="A19" s="194"/>
       <c r="B19" s="26"/>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
@@ -11453,7 +11458,7 @@
       <c r="EV19" s="98"/>
     </row>
     <row r="20" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="195" t="s">
+      <c r="A20" s="196" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="75"/>
@@ -11615,7 +11620,7 @@
       <c r="EV20" s="102"/>
     </row>
     <row r="21" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="193"/>
+      <c r="A21" s="194"/>
       <c r="B21" s="24"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -11773,7 +11778,7 @@
       <c r="EV21" s="17"/>
     </row>
     <row r="22" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="193"/>
+      <c r="A22" s="194"/>
       <c r="B22" s="24"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -11931,7 +11936,7 @@
       <c r="EV22" s="17"/>
     </row>
     <row r="23" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="193"/>
+      <c r="A23" s="194"/>
       <c r="B23" s="24"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -12089,7 +12094,7 @@
       <c r="EV23" s="17"/>
     </row>
     <row r="24" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="194"/>
+      <c r="A24" s="195"/>
       <c r="B24" s="91"/>
       <c r="C24" s="92"/>
       <c r="D24" s="92"/>
@@ -12243,7 +12248,7 @@
       <c r="EV24" s="98"/>
     </row>
     <row r="25" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="195" t="s">
+      <c r="A25" s="196" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="75"/>
@@ -12399,7 +12404,7 @@
       <c r="EV25" s="102"/>
     </row>
     <row r="26" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="193"/>
+      <c r="A26" s="194"/>
       <c r="B26" s="24"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -12553,7 +12558,7 @@
       <c r="EV26" s="17"/>
     </row>
     <row r="27" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="193"/>
+      <c r="A27" s="194"/>
       <c r="B27" s="24"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
@@ -12707,7 +12712,7 @@
       <c r="EV27" s="17"/>
     </row>
     <row r="28" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="193"/>
+      <c r="A28" s="194"/>
       <c r="B28" s="24"/>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
@@ -12861,7 +12866,7 @@
       <c r="EV28" s="17"/>
     </row>
     <row r="29" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="193"/>
+      <c r="A29" s="194"/>
       <c r="B29" s="85"/>
       <c r="C29" s="71"/>
       <c r="D29" s="71"/>
@@ -13015,7 +13020,7 @@
       <c r="EV29" s="98"/>
     </row>
     <row r="30" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="192" t="s">
+      <c r="A30" s="193" t="s">
         <v>20</v>
       </c>
       <c r="B30" s="75"/>
@@ -13181,7 +13186,7 @@
       <c r="EV30" s="102"/>
     </row>
     <row r="31" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="193"/>
+      <c r="A31" s="194"/>
       <c r="B31" s="24"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -13339,7 +13344,7 @@
       <c r="EV31" s="17"/>
     </row>
     <row r="32" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="193"/>
+      <c r="A32" s="194"/>
       <c r="B32" s="24"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
@@ -13497,7 +13502,7 @@
       <c r="EV32" s="17"/>
     </row>
     <row r="33" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="193"/>
+      <c r="A33" s="194"/>
       <c r="B33" s="24"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
@@ -13653,7 +13658,7 @@
       <c r="EV33" s="17"/>
     </row>
     <row r="34" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="194"/>
+      <c r="A34" s="195"/>
       <c r="B34" s="85"/>
       <c r="C34" s="71"/>
       <c r="D34" s="71"/>
@@ -13809,7 +13814,7 @@
       <c r="EV34" s="98"/>
     </row>
     <row r="35" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="193" t="s">
+      <c r="A35" s="194" t="s">
         <v>23</v>
       </c>
       <c r="B35" s="75"/>
@@ -13967,7 +13972,7 @@
       <c r="EV35" s="102"/>
     </row>
     <row r="36" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="193"/>
+      <c r="A36" s="194"/>
       <c r="B36" s="24"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
@@ -14123,7 +14128,7 @@
       <c r="EV36" s="17"/>
     </row>
     <row r="37" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="193"/>
+      <c r="A37" s="194"/>
       <c r="B37" s="24"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -14277,7 +14282,7 @@
       <c r="EV37" s="17"/>
     </row>
     <row r="38" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="193"/>
+      <c r="A38" s="194"/>
       <c r="B38" s="24"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
@@ -14431,7 +14436,7 @@
       <c r="EV38" s="17"/>
     </row>
     <row r="39" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="193"/>
+      <c r="A39" s="194"/>
       <c r="B39" s="85"/>
       <c r="C39" s="71"/>
       <c r="D39" s="71"/>
@@ -14585,7 +14590,7 @@
       <c r="EV39" s="98"/>
     </row>
     <row r="40" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="192" t="s">
+      <c r="A40" s="193" t="s">
         <v>22</v>
       </c>
       <c r="B40" s="75"/>
@@ -14747,7 +14752,7 @@
       <c r="EV40" s="102"/>
     </row>
     <row r="41" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="193"/>
+      <c r="A41" s="194"/>
       <c r="B41" s="24"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
@@ -14903,7 +14908,7 @@
       <c r="EV41" s="17"/>
     </row>
     <row r="42" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="193"/>
+      <c r="A42" s="194"/>
       <c r="B42" s="24"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -15061,7 +15066,7 @@
       <c r="EV42" s="17"/>
     </row>
     <row r="43" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="193"/>
+      <c r="A43" s="194"/>
       <c r="B43" s="24"/>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
@@ -15217,7 +15222,7 @@
       <c r="EV43" s="17"/>
     </row>
     <row r="44" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="194"/>
+      <c r="A44" s="195"/>
       <c r="B44" s="85"/>
       <c r="C44" s="71"/>
       <c r="D44" s="71"/>
@@ -15373,7 +15378,7 @@
       <c r="EV44" s="98"/>
     </row>
     <row r="45" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="193" t="s">
+      <c r="A45" s="194" t="s">
         <v>24</v>
       </c>
       <c r="B45" s="75"/>
@@ -15535,7 +15540,7 @@
       <c r="EV45" s="102"/>
     </row>
     <row r="46" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="193"/>
+      <c r="A46" s="194"/>
       <c r="B46" s="24"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
@@ -15691,7 +15696,7 @@
       <c r="EV46" s="17"/>
     </row>
     <row r="47" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="193"/>
+      <c r="A47" s="194"/>
       <c r="B47" s="24"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
@@ -15849,7 +15854,7 @@
       <c r="EV47" s="17"/>
     </row>
     <row r="48" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="193"/>
+      <c r="A48" s="194"/>
       <c r="B48" s="24"/>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -16005,7 +16010,7 @@
       <c r="EV48" s="17"/>
     </row>
     <row r="49" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="194"/>
+      <c r="A49" s="195"/>
       <c r="B49" s="85"/>
       <c r="C49" s="71"/>
       <c r="D49" s="71"/>
@@ -16241,395 +16246,395 @@
     </row>
     <row r="6" spans="1:366" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="199">
+      <c r="B6" s="200">
         <v>1</v>
       </c>
-      <c r="C6" s="196"/>
-      <c r="D6" s="196"/>
-      <c r="E6" s="196"/>
-      <c r="F6" s="196"/>
-      <c r="G6" s="196"/>
-      <c r="H6" s="196"/>
-      <c r="I6" s="196"/>
-      <c r="J6" s="196"/>
-      <c r="K6" s="196"/>
-      <c r="L6" s="196"/>
-      <c r="M6" s="196"/>
-      <c r="N6" s="196"/>
-      <c r="O6" s="196"/>
-      <c r="P6" s="196"/>
-      <c r="Q6" s="196"/>
-      <c r="R6" s="196"/>
-      <c r="S6" s="196"/>
-      <c r="T6" s="196"/>
-      <c r="U6" s="196"/>
-      <c r="V6" s="196"/>
-      <c r="W6" s="196"/>
-      <c r="X6" s="196"/>
-      <c r="Y6" s="196"/>
-      <c r="Z6" s="196"/>
-      <c r="AA6" s="196"/>
-      <c r="AB6" s="196"/>
-      <c r="AC6" s="196"/>
-      <c r="AD6" s="196"/>
-      <c r="AE6" s="196"/>
-      <c r="AF6" s="196"/>
-      <c r="AG6" s="199">
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="197"/>
+      <c r="F6" s="197"/>
+      <c r="G6" s="197"/>
+      <c r="H6" s="197"/>
+      <c r="I6" s="197"/>
+      <c r="J6" s="197"/>
+      <c r="K6" s="197"/>
+      <c r="L6" s="197"/>
+      <c r="M6" s="197"/>
+      <c r="N6" s="197"/>
+      <c r="O6" s="197"/>
+      <c r="P6" s="197"/>
+      <c r="Q6" s="197"/>
+      <c r="R6" s="197"/>
+      <c r="S6" s="197"/>
+      <c r="T6" s="197"/>
+      <c r="U6" s="197"/>
+      <c r="V6" s="197"/>
+      <c r="W6" s="197"/>
+      <c r="X6" s="197"/>
+      <c r="Y6" s="197"/>
+      <c r="Z6" s="197"/>
+      <c r="AA6" s="197"/>
+      <c r="AB6" s="197"/>
+      <c r="AC6" s="197"/>
+      <c r="AD6" s="197"/>
+      <c r="AE6" s="197"/>
+      <c r="AF6" s="197"/>
+      <c r="AG6" s="200">
         <v>2</v>
       </c>
-      <c r="AH6" s="196"/>
-      <c r="AI6" s="196"/>
-      <c r="AJ6" s="196"/>
-      <c r="AK6" s="196"/>
-      <c r="AL6" s="196"/>
-      <c r="AM6" s="196"/>
-      <c r="AN6" s="196"/>
-      <c r="AO6" s="196"/>
-      <c r="AP6" s="196"/>
-      <c r="AQ6" s="196"/>
-      <c r="AR6" s="196"/>
-      <c r="AS6" s="196"/>
-      <c r="AT6" s="196"/>
-      <c r="AU6" s="196"/>
-      <c r="AV6" s="196"/>
-      <c r="AW6" s="196"/>
-      <c r="AX6" s="196"/>
-      <c r="AY6" s="196"/>
-      <c r="AZ6" s="196"/>
-      <c r="BA6" s="196"/>
-      <c r="BB6" s="196"/>
-      <c r="BC6" s="196"/>
-      <c r="BD6" s="196"/>
-      <c r="BE6" s="196"/>
-      <c r="BF6" s="196"/>
-      <c r="BG6" s="196"/>
-      <c r="BH6" s="197"/>
-      <c r="BI6" s="196">
+      <c r="AH6" s="197"/>
+      <c r="AI6" s="197"/>
+      <c r="AJ6" s="197"/>
+      <c r="AK6" s="197"/>
+      <c r="AL6" s="197"/>
+      <c r="AM6" s="197"/>
+      <c r="AN6" s="197"/>
+      <c r="AO6" s="197"/>
+      <c r="AP6" s="197"/>
+      <c r="AQ6" s="197"/>
+      <c r="AR6" s="197"/>
+      <c r="AS6" s="197"/>
+      <c r="AT6" s="197"/>
+      <c r="AU6" s="197"/>
+      <c r="AV6" s="197"/>
+      <c r="AW6" s="197"/>
+      <c r="AX6" s="197"/>
+      <c r="AY6" s="197"/>
+      <c r="AZ6" s="197"/>
+      <c r="BA6" s="197"/>
+      <c r="BB6" s="197"/>
+      <c r="BC6" s="197"/>
+      <c r="BD6" s="197"/>
+      <c r="BE6" s="197"/>
+      <c r="BF6" s="197"/>
+      <c r="BG6" s="197"/>
+      <c r="BH6" s="198"/>
+      <c r="BI6" s="197">
         <v>3</v>
       </c>
-      <c r="BJ6" s="196"/>
-      <c r="BK6" s="196"/>
-      <c r="BL6" s="196"/>
-      <c r="BM6" s="196"/>
-      <c r="BN6" s="196"/>
-      <c r="BO6" s="196"/>
-      <c r="BP6" s="196"/>
-      <c r="BQ6" s="196"/>
-      <c r="BR6" s="196"/>
-      <c r="BS6" s="196"/>
-      <c r="BT6" s="196"/>
-      <c r="BU6" s="196"/>
-      <c r="BV6" s="196"/>
-      <c r="BW6" s="196"/>
-      <c r="BX6" s="196"/>
-      <c r="BY6" s="196"/>
-      <c r="BZ6" s="196"/>
-      <c r="CA6" s="196"/>
-      <c r="CB6" s="196"/>
-      <c r="CC6" s="196"/>
-      <c r="CD6" s="196"/>
-      <c r="CE6" s="196"/>
-      <c r="CF6" s="196"/>
-      <c r="CG6" s="196"/>
-      <c r="CH6" s="196"/>
-      <c r="CI6" s="196"/>
-      <c r="CJ6" s="196"/>
-      <c r="CK6" s="196"/>
-      <c r="CL6" s="196"/>
-      <c r="CM6" s="196"/>
-      <c r="CN6" s="200">
+      <c r="BJ6" s="197"/>
+      <c r="BK6" s="197"/>
+      <c r="BL6" s="197"/>
+      <c r="BM6" s="197"/>
+      <c r="BN6" s="197"/>
+      <c r="BO6" s="197"/>
+      <c r="BP6" s="197"/>
+      <c r="BQ6" s="197"/>
+      <c r="BR6" s="197"/>
+      <c r="BS6" s="197"/>
+      <c r="BT6" s="197"/>
+      <c r="BU6" s="197"/>
+      <c r="BV6" s="197"/>
+      <c r="BW6" s="197"/>
+      <c r="BX6" s="197"/>
+      <c r="BY6" s="197"/>
+      <c r="BZ6" s="197"/>
+      <c r="CA6" s="197"/>
+      <c r="CB6" s="197"/>
+      <c r="CC6" s="197"/>
+      <c r="CD6" s="197"/>
+      <c r="CE6" s="197"/>
+      <c r="CF6" s="197"/>
+      <c r="CG6" s="197"/>
+      <c r="CH6" s="197"/>
+      <c r="CI6" s="197"/>
+      <c r="CJ6" s="197"/>
+      <c r="CK6" s="197"/>
+      <c r="CL6" s="197"/>
+      <c r="CM6" s="197"/>
+      <c r="CN6" s="201">
         <v>4</v>
       </c>
-      <c r="CO6" s="201"/>
-      <c r="CP6" s="201"/>
-      <c r="CQ6" s="201"/>
-      <c r="CR6" s="201"/>
-      <c r="CS6" s="201"/>
-      <c r="CT6" s="201"/>
-      <c r="CU6" s="201"/>
-      <c r="CV6" s="201"/>
-      <c r="CW6" s="201"/>
-      <c r="CX6" s="201"/>
-      <c r="CY6" s="201"/>
-      <c r="CZ6" s="201"/>
-      <c r="DA6" s="201"/>
-      <c r="DB6" s="201"/>
-      <c r="DC6" s="201"/>
-      <c r="DD6" s="201"/>
-      <c r="DE6" s="201"/>
-      <c r="DF6" s="201"/>
-      <c r="DG6" s="201"/>
-      <c r="DH6" s="201"/>
-      <c r="DI6" s="201"/>
-      <c r="DJ6" s="201"/>
-      <c r="DK6" s="201"/>
-      <c r="DL6" s="201"/>
-      <c r="DM6" s="201"/>
-      <c r="DN6" s="201"/>
-      <c r="DO6" s="201"/>
-      <c r="DP6" s="201"/>
-      <c r="DQ6" s="202"/>
-      <c r="DR6" s="196">
+      <c r="CO6" s="202"/>
+      <c r="CP6" s="202"/>
+      <c r="CQ6" s="202"/>
+      <c r="CR6" s="202"/>
+      <c r="CS6" s="202"/>
+      <c r="CT6" s="202"/>
+      <c r="CU6" s="202"/>
+      <c r="CV6" s="202"/>
+      <c r="CW6" s="202"/>
+      <c r="CX6" s="202"/>
+      <c r="CY6" s="202"/>
+      <c r="CZ6" s="202"/>
+      <c r="DA6" s="202"/>
+      <c r="DB6" s="202"/>
+      <c r="DC6" s="202"/>
+      <c r="DD6" s="202"/>
+      <c r="DE6" s="202"/>
+      <c r="DF6" s="202"/>
+      <c r="DG6" s="202"/>
+      <c r="DH6" s="202"/>
+      <c r="DI6" s="202"/>
+      <c r="DJ6" s="202"/>
+      <c r="DK6" s="202"/>
+      <c r="DL6" s="202"/>
+      <c r="DM6" s="202"/>
+      <c r="DN6" s="202"/>
+      <c r="DO6" s="202"/>
+      <c r="DP6" s="202"/>
+      <c r="DQ6" s="203"/>
+      <c r="DR6" s="197">
         <v>5</v>
       </c>
-      <c r="DS6" s="196"/>
-      <c r="DT6" s="196"/>
-      <c r="DU6" s="196"/>
-      <c r="DV6" s="196"/>
-      <c r="DW6" s="196"/>
-      <c r="DX6" s="196"/>
-      <c r="DY6" s="196"/>
-      <c r="DZ6" s="196"/>
-      <c r="EA6" s="196"/>
-      <c r="EB6" s="196"/>
-      <c r="EC6" s="196"/>
-      <c r="ED6" s="196"/>
-      <c r="EE6" s="196"/>
-      <c r="EF6" s="196"/>
-      <c r="EG6" s="196"/>
-      <c r="EH6" s="196"/>
-      <c r="EI6" s="196"/>
-      <c r="EJ6" s="196"/>
-      <c r="EK6" s="196"/>
-      <c r="EL6" s="196"/>
-      <c r="EM6" s="196"/>
-      <c r="EN6" s="196"/>
-      <c r="EO6" s="196"/>
-      <c r="EP6" s="196"/>
-      <c r="EQ6" s="196"/>
-      <c r="ER6" s="196"/>
-      <c r="ES6" s="196"/>
-      <c r="ET6" s="196"/>
-      <c r="EU6" s="196"/>
-      <c r="EV6" s="197"/>
-      <c r="EW6" s="200">
+      <c r="DS6" s="197"/>
+      <c r="DT6" s="197"/>
+      <c r="DU6" s="197"/>
+      <c r="DV6" s="197"/>
+      <c r="DW6" s="197"/>
+      <c r="DX6" s="197"/>
+      <c r="DY6" s="197"/>
+      <c r="DZ6" s="197"/>
+      <c r="EA6" s="197"/>
+      <c r="EB6" s="197"/>
+      <c r="EC6" s="197"/>
+      <c r="ED6" s="197"/>
+      <c r="EE6" s="197"/>
+      <c r="EF6" s="197"/>
+      <c r="EG6" s="197"/>
+      <c r="EH6" s="197"/>
+      <c r="EI6" s="197"/>
+      <c r="EJ6" s="197"/>
+      <c r="EK6" s="197"/>
+      <c r="EL6" s="197"/>
+      <c r="EM6" s="197"/>
+      <c r="EN6" s="197"/>
+      <c r="EO6" s="197"/>
+      <c r="EP6" s="197"/>
+      <c r="EQ6" s="197"/>
+      <c r="ER6" s="197"/>
+      <c r="ES6" s="197"/>
+      <c r="ET6" s="197"/>
+      <c r="EU6" s="197"/>
+      <c r="EV6" s="198"/>
+      <c r="EW6" s="201">
         <v>6</v>
       </c>
-      <c r="EX6" s="201"/>
-      <c r="EY6" s="201"/>
-      <c r="EZ6" s="201"/>
-      <c r="FA6" s="201"/>
-      <c r="FB6" s="201"/>
-      <c r="FC6" s="201"/>
-      <c r="FD6" s="201"/>
-      <c r="FE6" s="201"/>
-      <c r="FF6" s="201"/>
-      <c r="FG6" s="201"/>
-      <c r="FH6" s="201"/>
-      <c r="FI6" s="201"/>
-      <c r="FJ6" s="201"/>
-      <c r="FK6" s="201"/>
-      <c r="FL6" s="201"/>
-      <c r="FM6" s="201"/>
-      <c r="FN6" s="201"/>
-      <c r="FO6" s="201"/>
-      <c r="FP6" s="201"/>
-      <c r="FQ6" s="201"/>
-      <c r="FR6" s="201"/>
-      <c r="FS6" s="201"/>
-      <c r="FT6" s="201"/>
-      <c r="FU6" s="201"/>
-      <c r="FV6" s="201"/>
-      <c r="FW6" s="201"/>
-      <c r="FX6" s="201"/>
-      <c r="FY6" s="201"/>
-      <c r="FZ6" s="202"/>
-      <c r="GA6" s="196">
+      <c r="EX6" s="202"/>
+      <c r="EY6" s="202"/>
+      <c r="EZ6" s="202"/>
+      <c r="FA6" s="202"/>
+      <c r="FB6" s="202"/>
+      <c r="FC6" s="202"/>
+      <c r="FD6" s="202"/>
+      <c r="FE6" s="202"/>
+      <c r="FF6" s="202"/>
+      <c r="FG6" s="202"/>
+      <c r="FH6" s="202"/>
+      <c r="FI6" s="202"/>
+      <c r="FJ6" s="202"/>
+      <c r="FK6" s="202"/>
+      <c r="FL6" s="202"/>
+      <c r="FM6" s="202"/>
+      <c r="FN6" s="202"/>
+      <c r="FO6" s="202"/>
+      <c r="FP6" s="202"/>
+      <c r="FQ6" s="202"/>
+      <c r="FR6" s="202"/>
+      <c r="FS6" s="202"/>
+      <c r="FT6" s="202"/>
+      <c r="FU6" s="202"/>
+      <c r="FV6" s="202"/>
+      <c r="FW6" s="202"/>
+      <c r="FX6" s="202"/>
+      <c r="FY6" s="202"/>
+      <c r="FZ6" s="203"/>
+      <c r="GA6" s="197">
         <v>7</v>
       </c>
-      <c r="GB6" s="196"/>
-      <c r="GC6" s="196"/>
-      <c r="GD6" s="196"/>
-      <c r="GE6" s="196"/>
-      <c r="GF6" s="196"/>
-      <c r="GG6" s="196"/>
-      <c r="GH6" s="196"/>
-      <c r="GI6" s="196"/>
-      <c r="GJ6" s="196"/>
-      <c r="GK6" s="196"/>
-      <c r="GL6" s="196"/>
-      <c r="GM6" s="196"/>
-      <c r="GN6" s="196"/>
-      <c r="GO6" s="196"/>
-      <c r="GP6" s="196"/>
-      <c r="GQ6" s="196"/>
-      <c r="GR6" s="196"/>
-      <c r="GS6" s="196"/>
-      <c r="GT6" s="196"/>
-      <c r="GU6" s="196"/>
-      <c r="GV6" s="196"/>
-      <c r="GW6" s="196"/>
-      <c r="GX6" s="196"/>
-      <c r="GY6" s="196"/>
-      <c r="GZ6" s="196"/>
-      <c r="HA6" s="196"/>
-      <c r="HB6" s="196"/>
-      <c r="HC6" s="196"/>
-      <c r="HD6" s="196"/>
-      <c r="HE6" s="197"/>
-      <c r="HF6" s="196">
+      <c r="GB6" s="197"/>
+      <c r="GC6" s="197"/>
+      <c r="GD6" s="197"/>
+      <c r="GE6" s="197"/>
+      <c r="GF6" s="197"/>
+      <c r="GG6" s="197"/>
+      <c r="GH6" s="197"/>
+      <c r="GI6" s="197"/>
+      <c r="GJ6" s="197"/>
+      <c r="GK6" s="197"/>
+      <c r="GL6" s="197"/>
+      <c r="GM6" s="197"/>
+      <c r="GN6" s="197"/>
+      <c r="GO6" s="197"/>
+      <c r="GP6" s="197"/>
+      <c r="GQ6" s="197"/>
+      <c r="GR6" s="197"/>
+      <c r="GS6" s="197"/>
+      <c r="GT6" s="197"/>
+      <c r="GU6" s="197"/>
+      <c r="GV6" s="197"/>
+      <c r="GW6" s="197"/>
+      <c r="GX6" s="197"/>
+      <c r="GY6" s="197"/>
+      <c r="GZ6" s="197"/>
+      <c r="HA6" s="197"/>
+      <c r="HB6" s="197"/>
+      <c r="HC6" s="197"/>
+      <c r="HD6" s="197"/>
+      <c r="HE6" s="198"/>
+      <c r="HF6" s="197">
         <v>8</v>
       </c>
-      <c r="HG6" s="196"/>
-      <c r="HH6" s="196"/>
-      <c r="HI6" s="196"/>
-      <c r="HJ6" s="196"/>
-      <c r="HK6" s="196"/>
-      <c r="HL6" s="196"/>
-      <c r="HM6" s="196"/>
-      <c r="HN6" s="196"/>
-      <c r="HO6" s="196"/>
-      <c r="HP6" s="196"/>
-      <c r="HQ6" s="196"/>
-      <c r="HR6" s="196"/>
-      <c r="HS6" s="196"/>
-      <c r="HT6" s="196"/>
-      <c r="HU6" s="196"/>
-      <c r="HV6" s="196"/>
-      <c r="HW6" s="196"/>
-      <c r="HX6" s="196"/>
-      <c r="HY6" s="196"/>
-      <c r="HZ6" s="196"/>
-      <c r="IA6" s="196"/>
-      <c r="IB6" s="196"/>
-      <c r="IC6" s="196"/>
-      <c r="ID6" s="196"/>
-      <c r="IE6" s="196"/>
-      <c r="IF6" s="196"/>
-      <c r="IG6" s="196"/>
-      <c r="IH6" s="196"/>
-      <c r="II6" s="196"/>
-      <c r="IJ6" s="197"/>
-      <c r="IK6" s="200">
+      <c r="HG6" s="197"/>
+      <c r="HH6" s="197"/>
+      <c r="HI6" s="197"/>
+      <c r="HJ6" s="197"/>
+      <c r="HK6" s="197"/>
+      <c r="HL6" s="197"/>
+      <c r="HM6" s="197"/>
+      <c r="HN6" s="197"/>
+      <c r="HO6" s="197"/>
+      <c r="HP6" s="197"/>
+      <c r="HQ6" s="197"/>
+      <c r="HR6" s="197"/>
+      <c r="HS6" s="197"/>
+      <c r="HT6" s="197"/>
+      <c r="HU6" s="197"/>
+      <c r="HV6" s="197"/>
+      <c r="HW6" s="197"/>
+      <c r="HX6" s="197"/>
+      <c r="HY6" s="197"/>
+      <c r="HZ6" s="197"/>
+      <c r="IA6" s="197"/>
+      <c r="IB6" s="197"/>
+      <c r="IC6" s="197"/>
+      <c r="ID6" s="197"/>
+      <c r="IE6" s="197"/>
+      <c r="IF6" s="197"/>
+      <c r="IG6" s="197"/>
+      <c r="IH6" s="197"/>
+      <c r="II6" s="197"/>
+      <c r="IJ6" s="198"/>
+      <c r="IK6" s="201">
         <v>9</v>
       </c>
-      <c r="IL6" s="201"/>
-      <c r="IM6" s="201"/>
-      <c r="IN6" s="201"/>
-      <c r="IO6" s="201"/>
-      <c r="IP6" s="201"/>
-      <c r="IQ6" s="201"/>
-      <c r="IR6" s="201"/>
-      <c r="IS6" s="201"/>
-      <c r="IT6" s="201"/>
-      <c r="IU6" s="201"/>
-      <c r="IV6" s="201"/>
-      <c r="IW6" s="201"/>
-      <c r="IX6" s="201"/>
-      <c r="IY6" s="201"/>
-      <c r="IZ6" s="201"/>
-      <c r="JA6" s="201"/>
-      <c r="JB6" s="201"/>
-      <c r="JC6" s="201"/>
-      <c r="JD6" s="201"/>
-      <c r="JE6" s="201"/>
-      <c r="JF6" s="201"/>
-      <c r="JG6" s="201"/>
-      <c r="JH6" s="201"/>
-      <c r="JI6" s="201"/>
-      <c r="JJ6" s="201"/>
-      <c r="JK6" s="201"/>
-      <c r="JL6" s="201"/>
-      <c r="JM6" s="201"/>
-      <c r="JN6" s="202"/>
-      <c r="JO6" s="196">
+      <c r="IL6" s="202"/>
+      <c r="IM6" s="202"/>
+      <c r="IN6" s="202"/>
+      <c r="IO6" s="202"/>
+      <c r="IP6" s="202"/>
+      <c r="IQ6" s="202"/>
+      <c r="IR6" s="202"/>
+      <c r="IS6" s="202"/>
+      <c r="IT6" s="202"/>
+      <c r="IU6" s="202"/>
+      <c r="IV6" s="202"/>
+      <c r="IW6" s="202"/>
+      <c r="IX6" s="202"/>
+      <c r="IY6" s="202"/>
+      <c r="IZ6" s="202"/>
+      <c r="JA6" s="202"/>
+      <c r="JB6" s="202"/>
+      <c r="JC6" s="202"/>
+      <c r="JD6" s="202"/>
+      <c r="JE6" s="202"/>
+      <c r="JF6" s="202"/>
+      <c r="JG6" s="202"/>
+      <c r="JH6" s="202"/>
+      <c r="JI6" s="202"/>
+      <c r="JJ6" s="202"/>
+      <c r="JK6" s="202"/>
+      <c r="JL6" s="202"/>
+      <c r="JM6" s="202"/>
+      <c r="JN6" s="203"/>
+      <c r="JO6" s="197">
         <v>10</v>
       </c>
-      <c r="JP6" s="196"/>
-      <c r="JQ6" s="196"/>
-      <c r="JR6" s="196"/>
-      <c r="JS6" s="196"/>
-      <c r="JT6" s="196"/>
-      <c r="JU6" s="196"/>
-      <c r="JV6" s="196"/>
-      <c r="JW6" s="196"/>
-      <c r="JX6" s="196"/>
-      <c r="JY6" s="196"/>
-      <c r="JZ6" s="196"/>
-      <c r="KA6" s="196"/>
-      <c r="KB6" s="196"/>
-      <c r="KC6" s="196"/>
-      <c r="KD6" s="196"/>
-      <c r="KE6" s="196"/>
-      <c r="KF6" s="196"/>
-      <c r="KG6" s="196"/>
-      <c r="KH6" s="196"/>
-      <c r="KI6" s="196"/>
-      <c r="KJ6" s="196"/>
-      <c r="KK6" s="196"/>
-      <c r="KL6" s="196"/>
-      <c r="KM6" s="196"/>
-      <c r="KN6" s="196"/>
-      <c r="KO6" s="196"/>
-      <c r="KP6" s="196"/>
-      <c r="KQ6" s="196"/>
-      <c r="KR6" s="196"/>
-      <c r="KS6" s="197"/>
-      <c r="KT6" s="200">
+      <c r="JP6" s="197"/>
+      <c r="JQ6" s="197"/>
+      <c r="JR6" s="197"/>
+      <c r="JS6" s="197"/>
+      <c r="JT6" s="197"/>
+      <c r="JU6" s="197"/>
+      <c r="JV6" s="197"/>
+      <c r="JW6" s="197"/>
+      <c r="JX6" s="197"/>
+      <c r="JY6" s="197"/>
+      <c r="JZ6" s="197"/>
+      <c r="KA6" s="197"/>
+      <c r="KB6" s="197"/>
+      <c r="KC6" s="197"/>
+      <c r="KD6" s="197"/>
+      <c r="KE6" s="197"/>
+      <c r="KF6" s="197"/>
+      <c r="KG6" s="197"/>
+      <c r="KH6" s="197"/>
+      <c r="KI6" s="197"/>
+      <c r="KJ6" s="197"/>
+      <c r="KK6" s="197"/>
+      <c r="KL6" s="197"/>
+      <c r="KM6" s="197"/>
+      <c r="KN6" s="197"/>
+      <c r="KO6" s="197"/>
+      <c r="KP6" s="197"/>
+      <c r="KQ6" s="197"/>
+      <c r="KR6" s="197"/>
+      <c r="KS6" s="198"/>
+      <c r="KT6" s="201">
         <v>11</v>
       </c>
-      <c r="KU6" s="201"/>
-      <c r="KV6" s="201"/>
-      <c r="KW6" s="201"/>
-      <c r="KX6" s="201"/>
-      <c r="KY6" s="201"/>
-      <c r="KZ6" s="201"/>
-      <c r="LA6" s="201"/>
-      <c r="LB6" s="201"/>
-      <c r="LC6" s="201"/>
-      <c r="LD6" s="201"/>
-      <c r="LE6" s="201"/>
-      <c r="LF6" s="201"/>
-      <c r="LG6" s="201"/>
-      <c r="LH6" s="201"/>
-      <c r="LI6" s="201"/>
-      <c r="LJ6" s="201"/>
-      <c r="LK6" s="201"/>
-      <c r="LL6" s="201"/>
-      <c r="LM6" s="201"/>
-      <c r="LN6" s="201"/>
-      <c r="LO6" s="201"/>
-      <c r="LP6" s="201"/>
-      <c r="LQ6" s="201"/>
-      <c r="LR6" s="201"/>
-      <c r="LS6" s="201"/>
-      <c r="LT6" s="201"/>
-      <c r="LU6" s="201"/>
-      <c r="LV6" s="201"/>
-      <c r="LW6" s="202"/>
-      <c r="LX6" s="196">
+      <c r="KU6" s="202"/>
+      <c r="KV6" s="202"/>
+      <c r="KW6" s="202"/>
+      <c r="KX6" s="202"/>
+      <c r="KY6" s="202"/>
+      <c r="KZ6" s="202"/>
+      <c r="LA6" s="202"/>
+      <c r="LB6" s="202"/>
+      <c r="LC6" s="202"/>
+      <c r="LD6" s="202"/>
+      <c r="LE6" s="202"/>
+      <c r="LF6" s="202"/>
+      <c r="LG6" s="202"/>
+      <c r="LH6" s="202"/>
+      <c r="LI6" s="202"/>
+      <c r="LJ6" s="202"/>
+      <c r="LK6" s="202"/>
+      <c r="LL6" s="202"/>
+      <c r="LM6" s="202"/>
+      <c r="LN6" s="202"/>
+      <c r="LO6" s="202"/>
+      <c r="LP6" s="202"/>
+      <c r="LQ6" s="202"/>
+      <c r="LR6" s="202"/>
+      <c r="LS6" s="202"/>
+      <c r="LT6" s="202"/>
+      <c r="LU6" s="202"/>
+      <c r="LV6" s="202"/>
+      <c r="LW6" s="203"/>
+      <c r="LX6" s="197">
         <v>12</v>
       </c>
-      <c r="LY6" s="196"/>
-      <c r="LZ6" s="196"/>
-      <c r="MA6" s="196"/>
-      <c r="MB6" s="196"/>
-      <c r="MC6" s="196"/>
-      <c r="MD6" s="196"/>
-      <c r="ME6" s="196"/>
-      <c r="MF6" s="196"/>
-      <c r="MG6" s="196"/>
-      <c r="MH6" s="196"/>
-      <c r="MI6" s="196"/>
-      <c r="MJ6" s="196"/>
-      <c r="MK6" s="196"/>
-      <c r="ML6" s="196"/>
-      <c r="MM6" s="196"/>
-      <c r="MN6" s="196"/>
-      <c r="MO6" s="196"/>
-      <c r="MP6" s="196"/>
-      <c r="MQ6" s="196"/>
-      <c r="MR6" s="196"/>
-      <c r="MS6" s="196"/>
-      <c r="MT6" s="196"/>
-      <c r="MU6" s="196"/>
-      <c r="MV6" s="196"/>
-      <c r="MW6" s="196"/>
-      <c r="MX6" s="196"/>
-      <c r="MY6" s="196"/>
-      <c r="MZ6" s="196"/>
-      <c r="NA6" s="196"/>
-      <c r="NB6" s="197"/>
+      <c r="LY6" s="197"/>
+      <c r="LZ6" s="197"/>
+      <c r="MA6" s="197"/>
+      <c r="MB6" s="197"/>
+      <c r="MC6" s="197"/>
+      <c r="MD6" s="197"/>
+      <c r="ME6" s="197"/>
+      <c r="MF6" s="197"/>
+      <c r="MG6" s="197"/>
+      <c r="MH6" s="197"/>
+      <c r="MI6" s="197"/>
+      <c r="MJ6" s="197"/>
+      <c r="MK6" s="197"/>
+      <c r="ML6" s="197"/>
+      <c r="MM6" s="197"/>
+      <c r="MN6" s="197"/>
+      <c r="MO6" s="197"/>
+      <c r="MP6" s="197"/>
+      <c r="MQ6" s="197"/>
+      <c r="MR6" s="197"/>
+      <c r="MS6" s="197"/>
+      <c r="MT6" s="197"/>
+      <c r="MU6" s="197"/>
+      <c r="MV6" s="197"/>
+      <c r="MW6" s="197"/>
+      <c r="MX6" s="197"/>
+      <c r="MY6" s="197"/>
+      <c r="MZ6" s="197"/>
+      <c r="NA6" s="197"/>
+      <c r="NB6" s="198"/>
     </row>
     <row r="7" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -17730,7 +17735,7 @@
       </c>
     </row>
     <row r="8" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="203" t="s">
+      <c r="A8" s="204" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="34"/>
@@ -18118,7 +18123,7 @@
       <c r="NB8" s="141"/>
     </row>
     <row r="9" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="203"/>
+      <c r="A9" s="204"/>
       <c r="B9" s="29"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -18498,7 +18503,7 @@
       <c r="NB9" s="32"/>
     </row>
     <row r="10" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="203"/>
+      <c r="A10" s="204"/>
       <c r="B10" s="29"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
@@ -18878,7 +18883,7 @@
       <c r="NB10" s="32"/>
     </row>
     <row r="11" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="203"/>
+      <c r="A11" s="204"/>
       <c r="B11" s="29"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
@@ -19254,7 +19259,7 @@
       <c r="NB11" s="32"/>
     </row>
     <row r="12" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="203"/>
+      <c r="A12" s="204"/>
       <c r="B12" s="29"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
@@ -19628,7 +19633,7 @@
       <c r="NB12" s="32"/>
     </row>
     <row r="13" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="203"/>
+      <c r="A13" s="204"/>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -19998,7 +20003,7 @@
       <c r="NB13" s="32"/>
     </row>
     <row r="14" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="203"/>
+      <c r="A14" s="204"/>
       <c r="B14" s="50"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51"/>
@@ -20368,7 +20373,7 @@
       <c r="NB14" s="65"/>
     </row>
     <row r="15" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="203" t="s">
+      <c r="A15" s="204" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="42"/>
@@ -20752,7 +20757,7 @@
       <c r="NB15" s="84"/>
     </row>
     <row r="16" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="203"/>
+      <c r="A16" s="204"/>
       <c r="B16" s="24"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -21132,7 +21137,7 @@
       <c r="NB16" s="25"/>
     </row>
     <row r="17" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="203"/>
+      <c r="A17" s="204"/>
       <c r="B17" s="24"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -21508,7 +21513,7 @@
       <c r="NB17" s="25"/>
     </row>
     <row r="18" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="203"/>
+      <c r="A18" s="204"/>
       <c r="B18" s="24"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -21884,7 +21889,7 @@
       <c r="NB18" s="25"/>
     </row>
     <row r="19" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="203"/>
+      <c r="A19" s="204"/>
       <c r="B19" s="26"/>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
@@ -22254,7 +22259,7 @@
       <c r="NB19" s="74"/>
     </row>
     <row r="20" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="203" t="s">
+      <c r="A20" s="204" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="75"/>
@@ -22632,7 +22637,7 @@
       <c r="NB20" s="84"/>
     </row>
     <row r="21" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="203"/>
+      <c r="A21" s="204"/>
       <c r="B21" s="24"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -23006,7 +23011,7 @@
       <c r="NB21" s="25"/>
     </row>
     <row r="22" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="203"/>
+      <c r="A22" s="204"/>
       <c r="B22" s="24"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -23378,7 +23383,7 @@
       <c r="NB22" s="25"/>
     </row>
     <row r="23" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="203"/>
+      <c r="A23" s="204"/>
       <c r="B23" s="24"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -23754,7 +23759,7 @@
       <c r="NB23" s="25"/>
     </row>
     <row r="24" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="203"/>
+      <c r="A24" s="204"/>
       <c r="B24" s="91"/>
       <c r="C24" s="92"/>
       <c r="D24" s="92"/>
@@ -24122,7 +24127,7 @@
       <c r="NB24" s="74"/>
     </row>
     <row r="25" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="204" t="s">
+      <c r="A25" s="205" t="s">
         <v>62</v>
       </c>
       <c r="B25" s="75"/>
@@ -24498,7 +24503,7 @@
       <c r="NB25" s="84"/>
     </row>
     <row r="26" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="203"/>
+      <c r="A26" s="204"/>
       <c r="B26" s="24"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -24870,7 +24875,7 @@
       <c r="NB26" s="25"/>
     </row>
     <row r="27" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="203"/>
+      <c r="A27" s="204"/>
       <c r="B27" s="24"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
@@ -25244,7 +25249,7 @@
       <c r="NB27" s="25"/>
     </row>
     <row r="28" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="203"/>
+      <c r="A28" s="204"/>
       <c r="B28" s="24"/>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
@@ -25616,7 +25621,7 @@
       <c r="NB28" s="25"/>
     </row>
     <row r="29" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="203"/>
+      <c r="A29" s="204"/>
       <c r="B29" s="85"/>
       <c r="C29" s="71"/>
       <c r="D29" s="71"/>
@@ -25986,7 +25991,7 @@
       <c r="NB29" s="74"/>
     </row>
     <row r="30" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="204" t="s">
+      <c r="A30" s="205" t="s">
         <v>63</v>
       </c>
       <c r="B30" s="75"/>
@@ -26358,7 +26363,7 @@
       <c r="NB30" s="84"/>
     </row>
     <row r="31" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="203"/>
+      <c r="A31" s="204"/>
       <c r="B31" s="24"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -26732,7 +26737,7 @@
       <c r="NB31" s="25"/>
     </row>
     <row r="32" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="203"/>
+      <c r="A32" s="204"/>
       <c r="B32" s="24"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
@@ -27106,7 +27111,7 @@
       <c r="NB32" s="25"/>
     </row>
     <row r="33" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="203"/>
+      <c r="A33" s="204"/>
       <c r="B33" s="24"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
@@ -27476,7 +27481,7 @@
       <c r="NB33" s="25"/>
     </row>
     <row r="34" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="203"/>
+      <c r="A34" s="204"/>
       <c r="B34" s="85"/>
       <c r="C34" s="71"/>
       <c r="D34" s="71"/>
@@ -27844,7 +27849,7 @@
       <c r="NB34" s="74"/>
     </row>
     <row r="35" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="203" t="s">
+      <c r="A35" s="204" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="42"/>
@@ -28226,7 +28231,7 @@
       <c r="NB35" s="47"/>
     </row>
     <row r="36" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="203"/>
+      <c r="A36" s="204"/>
       <c r="B36" s="24"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
@@ -28598,7 +28603,7 @@
       <c r="NB36" s="25"/>
     </row>
     <row r="37" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="203"/>
+      <c r="A37" s="204"/>
       <c r="B37" s="24"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -28976,7 +28981,7 @@
       <c r="NB37" s="25"/>
     </row>
     <row r="38" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="203"/>
+      <c r="A38" s="204"/>
       <c r="B38" s="24"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
@@ -29346,7 +29351,7 @@
       <c r="NB38" s="25"/>
     </row>
     <row r="39" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="203"/>
+      <c r="A39" s="204"/>
       <c r="B39" s="85"/>
       <c r="C39" s="71"/>
       <c r="D39" s="71"/>
@@ -29718,7 +29723,7 @@
       <c r="NB39" s="74"/>
     </row>
     <row r="40" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="203" t="s">
+      <c r="A40" s="204" t="s">
         <v>23</v>
       </c>
       <c r="B40" s="75"/>
@@ -30096,7 +30101,7 @@
       <c r="NB40" s="84"/>
     </row>
     <row r="41" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="203"/>
+      <c r="A41" s="204"/>
       <c r="B41" s="24"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
@@ -30470,7 +30475,7 @@
       <c r="NB41" s="25"/>
     </row>
     <row r="42" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="203"/>
+      <c r="A42" s="204"/>
       <c r="B42" s="24"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -30842,7 +30847,7 @@
       <c r="NB42" s="25"/>
     </row>
     <row r="43" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="203"/>
+      <c r="A43" s="204"/>
       <c r="B43" s="24"/>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
@@ -31212,7 +31217,7 @@
       <c r="NB43" s="25"/>
     </row>
     <row r="44" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="203"/>
+      <c r="A44" s="204"/>
       <c r="B44" s="85"/>
       <c r="C44" s="71"/>
       <c r="D44" s="71"/>
@@ -31580,7 +31585,7 @@
       <c r="NB44" s="74"/>
     </row>
     <row r="45" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="203" t="s">
+      <c r="A45" s="204" t="s">
         <v>22</v>
       </c>
       <c r="B45" s="75"/>
@@ -31960,7 +31965,7 @@
       <c r="NB45" s="84"/>
     </row>
     <row r="46" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="203"/>
+      <c r="A46" s="204"/>
       <c r="B46" s="24"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
@@ -32330,7 +32335,7 @@
       <c r="NB46" s="25"/>
     </row>
     <row r="47" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="203"/>
+      <c r="A47" s="204"/>
       <c r="B47" s="24"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
@@ -32706,7 +32711,7 @@
       <c r="NB47" s="25"/>
     </row>
     <row r="48" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="203"/>
+      <c r="A48" s="204"/>
       <c r="B48" s="24"/>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -33076,7 +33081,7 @@
       <c r="NB48" s="25"/>
     </row>
     <row r="49" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="203"/>
+      <c r="A49" s="204"/>
       <c r="B49" s="85"/>
       <c r="C49" s="71"/>
       <c r="D49" s="71"/>
@@ -33450,7 +33455,7 @@
       <c r="NB49" s="74"/>
     </row>
     <row r="50" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="203" t="s">
+      <c r="A50" s="204" t="s">
         <v>24</v>
       </c>
       <c r="B50" s="75"/>
@@ -33832,7 +33837,7 @@
       <c r="NB50" s="84"/>
     </row>
     <row r="51" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="203"/>
+      <c r="A51" s="204"/>
       <c r="B51" s="24"/>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
@@ -34210,7 +34215,7 @@
       <c r="NB51" s="25"/>
     </row>
     <row r="52" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="203"/>
+      <c r="A52" s="204"/>
       <c r="B52" s="24"/>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
@@ -34582,7 +34587,7 @@
       <c r="NB52" s="25"/>
     </row>
     <row r="53" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="203"/>
+      <c r="A53" s="204"/>
       <c r="B53" s="24"/>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
@@ -34952,7 +34957,7 @@
       <c r="NB53" s="25"/>
     </row>
     <row r="54" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="203"/>
+      <c r="A54" s="204"/>
       <c r="B54" s="85"/>
       <c r="C54" s="71"/>
       <c r="D54" s="71"/>
@@ -35372,7 +35377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:NB71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CP1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="EJ39" sqref="EJ39"/>
     </sheetView>
@@ -35411,395 +35416,395 @@
     </row>
     <row r="6" spans="1:366" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="199">
+      <c r="B6" s="200">
         <v>1</v>
       </c>
-      <c r="C6" s="196"/>
-      <c r="D6" s="196"/>
-      <c r="E6" s="196"/>
-      <c r="F6" s="196"/>
-      <c r="G6" s="196"/>
-      <c r="H6" s="196"/>
-      <c r="I6" s="196"/>
-      <c r="J6" s="196"/>
-      <c r="K6" s="196"/>
-      <c r="L6" s="196"/>
-      <c r="M6" s="196"/>
-      <c r="N6" s="196"/>
-      <c r="O6" s="196"/>
-      <c r="P6" s="196"/>
-      <c r="Q6" s="196"/>
-      <c r="R6" s="196"/>
-      <c r="S6" s="196"/>
-      <c r="T6" s="196"/>
-      <c r="U6" s="196"/>
-      <c r="V6" s="196"/>
-      <c r="W6" s="196"/>
-      <c r="X6" s="196"/>
-      <c r="Y6" s="196"/>
-      <c r="Z6" s="196"/>
-      <c r="AA6" s="196"/>
-      <c r="AB6" s="196"/>
-      <c r="AC6" s="196"/>
-      <c r="AD6" s="196"/>
-      <c r="AE6" s="196"/>
-      <c r="AF6" s="196"/>
-      <c r="AG6" s="199">
+      <c r="C6" s="197"/>
+      <c r="D6" s="197"/>
+      <c r="E6" s="197"/>
+      <c r="F6" s="197"/>
+      <c r="G6" s="197"/>
+      <c r="H6" s="197"/>
+      <c r="I6" s="197"/>
+      <c r="J6" s="197"/>
+      <c r="K6" s="197"/>
+      <c r="L6" s="197"/>
+      <c r="M6" s="197"/>
+      <c r="N6" s="197"/>
+      <c r="O6" s="197"/>
+      <c r="P6" s="197"/>
+      <c r="Q6" s="197"/>
+      <c r="R6" s="197"/>
+      <c r="S6" s="197"/>
+      <c r="T6" s="197"/>
+      <c r="U6" s="197"/>
+      <c r="V6" s="197"/>
+      <c r="W6" s="197"/>
+      <c r="X6" s="197"/>
+      <c r="Y6" s="197"/>
+      <c r="Z6" s="197"/>
+      <c r="AA6" s="197"/>
+      <c r="AB6" s="197"/>
+      <c r="AC6" s="197"/>
+      <c r="AD6" s="197"/>
+      <c r="AE6" s="197"/>
+      <c r="AF6" s="197"/>
+      <c r="AG6" s="200">
         <v>2</v>
       </c>
-      <c r="AH6" s="196"/>
-      <c r="AI6" s="196"/>
-      <c r="AJ6" s="196"/>
-      <c r="AK6" s="196"/>
-      <c r="AL6" s="196"/>
-      <c r="AM6" s="196"/>
-      <c r="AN6" s="196"/>
-      <c r="AO6" s="196"/>
-      <c r="AP6" s="196"/>
-      <c r="AQ6" s="196"/>
-      <c r="AR6" s="196"/>
-      <c r="AS6" s="196"/>
-      <c r="AT6" s="196"/>
-      <c r="AU6" s="196"/>
-      <c r="AV6" s="196"/>
-      <c r="AW6" s="196"/>
-      <c r="AX6" s="196"/>
-      <c r="AY6" s="196"/>
-      <c r="AZ6" s="196"/>
-      <c r="BA6" s="196"/>
-      <c r="BB6" s="196"/>
-      <c r="BC6" s="196"/>
-      <c r="BD6" s="196"/>
-      <c r="BE6" s="196"/>
-      <c r="BF6" s="196"/>
-      <c r="BG6" s="196"/>
-      <c r="BH6" s="197"/>
-      <c r="BI6" s="196">
+      <c r="AH6" s="197"/>
+      <c r="AI6" s="197"/>
+      <c r="AJ6" s="197"/>
+      <c r="AK6" s="197"/>
+      <c r="AL6" s="197"/>
+      <c r="AM6" s="197"/>
+      <c r="AN6" s="197"/>
+      <c r="AO6" s="197"/>
+      <c r="AP6" s="197"/>
+      <c r="AQ6" s="197"/>
+      <c r="AR6" s="197"/>
+      <c r="AS6" s="197"/>
+      <c r="AT6" s="197"/>
+      <c r="AU6" s="197"/>
+      <c r="AV6" s="197"/>
+      <c r="AW6" s="197"/>
+      <c r="AX6" s="197"/>
+      <c r="AY6" s="197"/>
+      <c r="AZ6" s="197"/>
+      <c r="BA6" s="197"/>
+      <c r="BB6" s="197"/>
+      <c r="BC6" s="197"/>
+      <c r="BD6" s="197"/>
+      <c r="BE6" s="197"/>
+      <c r="BF6" s="197"/>
+      <c r="BG6" s="197"/>
+      <c r="BH6" s="198"/>
+      <c r="BI6" s="197">
         <v>3</v>
       </c>
-      <c r="BJ6" s="196"/>
-      <c r="BK6" s="196"/>
-      <c r="BL6" s="196"/>
-      <c r="BM6" s="196"/>
-      <c r="BN6" s="196"/>
-      <c r="BO6" s="196"/>
-      <c r="BP6" s="196"/>
-      <c r="BQ6" s="196"/>
-      <c r="BR6" s="196"/>
-      <c r="BS6" s="196"/>
-      <c r="BT6" s="196"/>
-      <c r="BU6" s="196"/>
-      <c r="BV6" s="196"/>
-      <c r="BW6" s="196"/>
-      <c r="BX6" s="196"/>
-      <c r="BY6" s="196"/>
-      <c r="BZ6" s="196"/>
-      <c r="CA6" s="196"/>
-      <c r="CB6" s="196"/>
-      <c r="CC6" s="196"/>
-      <c r="CD6" s="196"/>
-      <c r="CE6" s="196"/>
-      <c r="CF6" s="196"/>
-      <c r="CG6" s="196"/>
-      <c r="CH6" s="196"/>
-      <c r="CI6" s="196"/>
-      <c r="CJ6" s="196"/>
-      <c r="CK6" s="196"/>
-      <c r="CL6" s="196"/>
-      <c r="CM6" s="196"/>
-      <c r="CN6" s="200">
+      <c r="BJ6" s="197"/>
+      <c r="BK6" s="197"/>
+      <c r="BL6" s="197"/>
+      <c r="BM6" s="197"/>
+      <c r="BN6" s="197"/>
+      <c r="BO6" s="197"/>
+      <c r="BP6" s="197"/>
+      <c r="BQ6" s="197"/>
+      <c r="BR6" s="197"/>
+      <c r="BS6" s="197"/>
+      <c r="BT6" s="197"/>
+      <c r="BU6" s="197"/>
+      <c r="BV6" s="197"/>
+      <c r="BW6" s="197"/>
+      <c r="BX6" s="197"/>
+      <c r="BY6" s="197"/>
+      <c r="BZ6" s="197"/>
+      <c r="CA6" s="197"/>
+      <c r="CB6" s="197"/>
+      <c r="CC6" s="197"/>
+      <c r="CD6" s="197"/>
+      <c r="CE6" s="197"/>
+      <c r="CF6" s="197"/>
+      <c r="CG6" s="197"/>
+      <c r="CH6" s="197"/>
+      <c r="CI6" s="197"/>
+      <c r="CJ6" s="197"/>
+      <c r="CK6" s="197"/>
+      <c r="CL6" s="197"/>
+      <c r="CM6" s="197"/>
+      <c r="CN6" s="201">
         <v>4</v>
       </c>
-      <c r="CO6" s="201"/>
-      <c r="CP6" s="201"/>
-      <c r="CQ6" s="201"/>
-      <c r="CR6" s="201"/>
-      <c r="CS6" s="201"/>
-      <c r="CT6" s="201"/>
-      <c r="CU6" s="201"/>
-      <c r="CV6" s="201"/>
-      <c r="CW6" s="201"/>
-      <c r="CX6" s="201"/>
-      <c r="CY6" s="201"/>
-      <c r="CZ6" s="201"/>
-      <c r="DA6" s="201"/>
-      <c r="DB6" s="201"/>
-      <c r="DC6" s="201"/>
-      <c r="DD6" s="201"/>
-      <c r="DE6" s="201"/>
-      <c r="DF6" s="201"/>
-      <c r="DG6" s="201"/>
-      <c r="DH6" s="201"/>
-      <c r="DI6" s="201"/>
-      <c r="DJ6" s="201"/>
-      <c r="DK6" s="201"/>
-      <c r="DL6" s="201"/>
-      <c r="DM6" s="201"/>
-      <c r="DN6" s="201"/>
-      <c r="DO6" s="201"/>
-      <c r="DP6" s="201"/>
-      <c r="DQ6" s="202"/>
-      <c r="DR6" s="196">
+      <c r="CO6" s="202"/>
+      <c r="CP6" s="202"/>
+      <c r="CQ6" s="202"/>
+      <c r="CR6" s="202"/>
+      <c r="CS6" s="202"/>
+      <c r="CT6" s="202"/>
+      <c r="CU6" s="202"/>
+      <c r="CV6" s="202"/>
+      <c r="CW6" s="202"/>
+      <c r="CX6" s="202"/>
+      <c r="CY6" s="202"/>
+      <c r="CZ6" s="202"/>
+      <c r="DA6" s="202"/>
+      <c r="DB6" s="202"/>
+      <c r="DC6" s="202"/>
+      <c r="DD6" s="202"/>
+      <c r="DE6" s="202"/>
+      <c r="DF6" s="202"/>
+      <c r="DG6" s="202"/>
+      <c r="DH6" s="202"/>
+      <c r="DI6" s="202"/>
+      <c r="DJ6" s="202"/>
+      <c r="DK6" s="202"/>
+      <c r="DL6" s="202"/>
+      <c r="DM6" s="202"/>
+      <c r="DN6" s="202"/>
+      <c r="DO6" s="202"/>
+      <c r="DP6" s="202"/>
+      <c r="DQ6" s="203"/>
+      <c r="DR6" s="197">
         <v>5</v>
       </c>
-      <c r="DS6" s="196"/>
-      <c r="DT6" s="196"/>
-      <c r="DU6" s="196"/>
-      <c r="DV6" s="196"/>
-      <c r="DW6" s="196"/>
-      <c r="DX6" s="196"/>
-      <c r="DY6" s="196"/>
-      <c r="DZ6" s="196"/>
-      <c r="EA6" s="196"/>
-      <c r="EB6" s="196"/>
-      <c r="EC6" s="196"/>
-      <c r="ED6" s="196"/>
-      <c r="EE6" s="196"/>
-      <c r="EF6" s="196"/>
-      <c r="EG6" s="196"/>
-      <c r="EH6" s="196"/>
-      <c r="EI6" s="196"/>
-      <c r="EJ6" s="196"/>
-      <c r="EK6" s="196"/>
-      <c r="EL6" s="196"/>
-      <c r="EM6" s="196"/>
-      <c r="EN6" s="196"/>
-      <c r="EO6" s="196"/>
-      <c r="EP6" s="196"/>
-      <c r="EQ6" s="196"/>
-      <c r="ER6" s="196"/>
-      <c r="ES6" s="196"/>
-      <c r="ET6" s="196"/>
-      <c r="EU6" s="196"/>
-      <c r="EV6" s="197"/>
-      <c r="EW6" s="200">
+      <c r="DS6" s="197"/>
+      <c r="DT6" s="197"/>
+      <c r="DU6" s="197"/>
+      <c r="DV6" s="197"/>
+      <c r="DW6" s="197"/>
+      <c r="DX6" s="197"/>
+      <c r="DY6" s="197"/>
+      <c r="DZ6" s="197"/>
+      <c r="EA6" s="197"/>
+      <c r="EB6" s="197"/>
+      <c r="EC6" s="197"/>
+      <c r="ED6" s="197"/>
+      <c r="EE6" s="197"/>
+      <c r="EF6" s="197"/>
+      <c r="EG6" s="197"/>
+      <c r="EH6" s="197"/>
+      <c r="EI6" s="197"/>
+      <c r="EJ6" s="197"/>
+      <c r="EK6" s="197"/>
+      <c r="EL6" s="197"/>
+      <c r="EM6" s="197"/>
+      <c r="EN6" s="197"/>
+      <c r="EO6" s="197"/>
+      <c r="EP6" s="197"/>
+      <c r="EQ6" s="197"/>
+      <c r="ER6" s="197"/>
+      <c r="ES6" s="197"/>
+      <c r="ET6" s="197"/>
+      <c r="EU6" s="197"/>
+      <c r="EV6" s="198"/>
+      <c r="EW6" s="201">
         <v>6</v>
       </c>
-      <c r="EX6" s="201"/>
-      <c r="EY6" s="201"/>
-      <c r="EZ6" s="201"/>
-      <c r="FA6" s="201"/>
-      <c r="FB6" s="201"/>
-      <c r="FC6" s="201"/>
-      <c r="FD6" s="201"/>
-      <c r="FE6" s="201"/>
-      <c r="FF6" s="201"/>
-      <c r="FG6" s="201"/>
-      <c r="FH6" s="201"/>
-      <c r="FI6" s="201"/>
-      <c r="FJ6" s="201"/>
-      <c r="FK6" s="201"/>
-      <c r="FL6" s="201"/>
-      <c r="FM6" s="201"/>
-      <c r="FN6" s="201"/>
-      <c r="FO6" s="201"/>
-      <c r="FP6" s="201"/>
-      <c r="FQ6" s="201"/>
-      <c r="FR6" s="201"/>
-      <c r="FS6" s="201"/>
-      <c r="FT6" s="201"/>
-      <c r="FU6" s="201"/>
-      <c r="FV6" s="201"/>
-      <c r="FW6" s="201"/>
-      <c r="FX6" s="201"/>
-      <c r="FY6" s="201"/>
-      <c r="FZ6" s="202"/>
-      <c r="GA6" s="196">
+      <c r="EX6" s="202"/>
+      <c r="EY6" s="202"/>
+      <c r="EZ6" s="202"/>
+      <c r="FA6" s="202"/>
+      <c r="FB6" s="202"/>
+      <c r="FC6" s="202"/>
+      <c r="FD6" s="202"/>
+      <c r="FE6" s="202"/>
+      <c r="FF6" s="202"/>
+      <c r="FG6" s="202"/>
+      <c r="FH6" s="202"/>
+      <c r="FI6" s="202"/>
+      <c r="FJ6" s="202"/>
+      <c r="FK6" s="202"/>
+      <c r="FL6" s="202"/>
+      <c r="FM6" s="202"/>
+      <c r="FN6" s="202"/>
+      <c r="FO6" s="202"/>
+      <c r="FP6" s="202"/>
+      <c r="FQ6" s="202"/>
+      <c r="FR6" s="202"/>
+      <c r="FS6" s="202"/>
+      <c r="FT6" s="202"/>
+      <c r="FU6" s="202"/>
+      <c r="FV6" s="202"/>
+      <c r="FW6" s="202"/>
+      <c r="FX6" s="202"/>
+      <c r="FY6" s="202"/>
+      <c r="FZ6" s="203"/>
+      <c r="GA6" s="197">
         <v>7</v>
       </c>
-      <c r="GB6" s="196"/>
-      <c r="GC6" s="196"/>
-      <c r="GD6" s="196"/>
-      <c r="GE6" s="196"/>
-      <c r="GF6" s="196"/>
-      <c r="GG6" s="196"/>
-      <c r="GH6" s="196"/>
-      <c r="GI6" s="196"/>
-      <c r="GJ6" s="196"/>
-      <c r="GK6" s="196"/>
-      <c r="GL6" s="196"/>
-      <c r="GM6" s="196"/>
-      <c r="GN6" s="196"/>
-      <c r="GO6" s="196"/>
-      <c r="GP6" s="196"/>
-      <c r="GQ6" s="196"/>
-      <c r="GR6" s="196"/>
-      <c r="GS6" s="196"/>
-      <c r="GT6" s="196"/>
-      <c r="GU6" s="196"/>
-      <c r="GV6" s="196"/>
-      <c r="GW6" s="196"/>
-      <c r="GX6" s="196"/>
-      <c r="GY6" s="196"/>
-      <c r="GZ6" s="196"/>
-      <c r="HA6" s="196"/>
-      <c r="HB6" s="196"/>
-      <c r="HC6" s="196"/>
-      <c r="HD6" s="196"/>
-      <c r="HE6" s="197"/>
-      <c r="HF6" s="196">
+      <c r="GB6" s="197"/>
+      <c r="GC6" s="197"/>
+      <c r="GD6" s="197"/>
+      <c r="GE6" s="197"/>
+      <c r="GF6" s="197"/>
+      <c r="GG6" s="197"/>
+      <c r="GH6" s="197"/>
+      <c r="GI6" s="197"/>
+      <c r="GJ6" s="197"/>
+      <c r="GK6" s="197"/>
+      <c r="GL6" s="197"/>
+      <c r="GM6" s="197"/>
+      <c r="GN6" s="197"/>
+      <c r="GO6" s="197"/>
+      <c r="GP6" s="197"/>
+      <c r="GQ6" s="197"/>
+      <c r="GR6" s="197"/>
+      <c r="GS6" s="197"/>
+      <c r="GT6" s="197"/>
+      <c r="GU6" s="197"/>
+      <c r="GV6" s="197"/>
+      <c r="GW6" s="197"/>
+      <c r="GX6" s="197"/>
+      <c r="GY6" s="197"/>
+      <c r="GZ6" s="197"/>
+      <c r="HA6" s="197"/>
+      <c r="HB6" s="197"/>
+      <c r="HC6" s="197"/>
+      <c r="HD6" s="197"/>
+      <c r="HE6" s="198"/>
+      <c r="HF6" s="197">
         <v>8</v>
       </c>
-      <c r="HG6" s="196"/>
-      <c r="HH6" s="196"/>
-      <c r="HI6" s="196"/>
-      <c r="HJ6" s="196"/>
-      <c r="HK6" s="196"/>
-      <c r="HL6" s="196"/>
-      <c r="HM6" s="196"/>
-      <c r="HN6" s="196"/>
-      <c r="HO6" s="196"/>
-      <c r="HP6" s="196"/>
-      <c r="HQ6" s="196"/>
-      <c r="HR6" s="196"/>
-      <c r="HS6" s="196"/>
-      <c r="HT6" s="196"/>
-      <c r="HU6" s="196"/>
-      <c r="HV6" s="196"/>
-      <c r="HW6" s="196"/>
-      <c r="HX6" s="196"/>
-      <c r="HY6" s="196"/>
-      <c r="HZ6" s="196"/>
-      <c r="IA6" s="196"/>
-      <c r="IB6" s="196"/>
-      <c r="IC6" s="196"/>
-      <c r="ID6" s="196"/>
-      <c r="IE6" s="196"/>
-      <c r="IF6" s="196"/>
-      <c r="IG6" s="196"/>
-      <c r="IH6" s="196"/>
-      <c r="II6" s="196"/>
-      <c r="IJ6" s="197"/>
-      <c r="IK6" s="200">
+      <c r="HG6" s="197"/>
+      <c r="HH6" s="197"/>
+      <c r="HI6" s="197"/>
+      <c r="HJ6" s="197"/>
+      <c r="HK6" s="197"/>
+      <c r="HL6" s="197"/>
+      <c r="HM6" s="197"/>
+      <c r="HN6" s="197"/>
+      <c r="HO6" s="197"/>
+      <c r="HP6" s="197"/>
+      <c r="HQ6" s="197"/>
+      <c r="HR6" s="197"/>
+      <c r="HS6" s="197"/>
+      <c r="HT6" s="197"/>
+      <c r="HU6" s="197"/>
+      <c r="HV6" s="197"/>
+      <c r="HW6" s="197"/>
+      <c r="HX6" s="197"/>
+      <c r="HY6" s="197"/>
+      <c r="HZ6" s="197"/>
+      <c r="IA6" s="197"/>
+      <c r="IB6" s="197"/>
+      <c r="IC6" s="197"/>
+      <c r="ID6" s="197"/>
+      <c r="IE6" s="197"/>
+      <c r="IF6" s="197"/>
+      <c r="IG6" s="197"/>
+      <c r="IH6" s="197"/>
+      <c r="II6" s="197"/>
+      <c r="IJ6" s="198"/>
+      <c r="IK6" s="201">
         <v>9</v>
       </c>
-      <c r="IL6" s="201"/>
-      <c r="IM6" s="201"/>
-      <c r="IN6" s="201"/>
-      <c r="IO6" s="201"/>
-      <c r="IP6" s="201"/>
-      <c r="IQ6" s="201"/>
-      <c r="IR6" s="201"/>
-      <c r="IS6" s="201"/>
-      <c r="IT6" s="201"/>
-      <c r="IU6" s="201"/>
-      <c r="IV6" s="201"/>
-      <c r="IW6" s="201"/>
-      <c r="IX6" s="201"/>
-      <c r="IY6" s="201"/>
-      <c r="IZ6" s="201"/>
-      <c r="JA6" s="201"/>
-      <c r="JB6" s="201"/>
-      <c r="JC6" s="201"/>
-      <c r="JD6" s="201"/>
-      <c r="JE6" s="201"/>
-      <c r="JF6" s="201"/>
-      <c r="JG6" s="201"/>
-      <c r="JH6" s="201"/>
-      <c r="JI6" s="201"/>
-      <c r="JJ6" s="201"/>
-      <c r="JK6" s="201"/>
-      <c r="JL6" s="201"/>
-      <c r="JM6" s="201"/>
-      <c r="JN6" s="202"/>
-      <c r="JO6" s="196">
+      <c r="IL6" s="202"/>
+      <c r="IM6" s="202"/>
+      <c r="IN6" s="202"/>
+      <c r="IO6" s="202"/>
+      <c r="IP6" s="202"/>
+      <c r="IQ6" s="202"/>
+      <c r="IR6" s="202"/>
+      <c r="IS6" s="202"/>
+      <c r="IT6" s="202"/>
+      <c r="IU6" s="202"/>
+      <c r="IV6" s="202"/>
+      <c r="IW6" s="202"/>
+      <c r="IX6" s="202"/>
+      <c r="IY6" s="202"/>
+      <c r="IZ6" s="202"/>
+      <c r="JA6" s="202"/>
+      <c r="JB6" s="202"/>
+      <c r="JC6" s="202"/>
+      <c r="JD6" s="202"/>
+      <c r="JE6" s="202"/>
+      <c r="JF6" s="202"/>
+      <c r="JG6" s="202"/>
+      <c r="JH6" s="202"/>
+      <c r="JI6" s="202"/>
+      <c r="JJ6" s="202"/>
+      <c r="JK6" s="202"/>
+      <c r="JL6" s="202"/>
+      <c r="JM6" s="202"/>
+      <c r="JN6" s="203"/>
+      <c r="JO6" s="197">
         <v>10</v>
       </c>
-      <c r="JP6" s="196"/>
-      <c r="JQ6" s="196"/>
-      <c r="JR6" s="196"/>
-      <c r="JS6" s="196"/>
-      <c r="JT6" s="196"/>
-      <c r="JU6" s="196"/>
-      <c r="JV6" s="196"/>
-      <c r="JW6" s="196"/>
-      <c r="JX6" s="196"/>
-      <c r="JY6" s="196"/>
-      <c r="JZ6" s="196"/>
-      <c r="KA6" s="196"/>
-      <c r="KB6" s="196"/>
-      <c r="KC6" s="196"/>
-      <c r="KD6" s="196"/>
-      <c r="KE6" s="196"/>
-      <c r="KF6" s="196"/>
-      <c r="KG6" s="196"/>
-      <c r="KH6" s="196"/>
-      <c r="KI6" s="196"/>
-      <c r="KJ6" s="196"/>
-      <c r="KK6" s="196"/>
-      <c r="KL6" s="196"/>
-      <c r="KM6" s="196"/>
-      <c r="KN6" s="196"/>
-      <c r="KO6" s="196"/>
-      <c r="KP6" s="196"/>
-      <c r="KQ6" s="196"/>
-      <c r="KR6" s="196"/>
-      <c r="KS6" s="197"/>
-      <c r="KT6" s="200">
+      <c r="JP6" s="197"/>
+      <c r="JQ6" s="197"/>
+      <c r="JR6" s="197"/>
+      <c r="JS6" s="197"/>
+      <c r="JT6" s="197"/>
+      <c r="JU6" s="197"/>
+      <c r="JV6" s="197"/>
+      <c r="JW6" s="197"/>
+      <c r="JX6" s="197"/>
+      <c r="JY6" s="197"/>
+      <c r="JZ6" s="197"/>
+      <c r="KA6" s="197"/>
+      <c r="KB6" s="197"/>
+      <c r="KC6" s="197"/>
+      <c r="KD6" s="197"/>
+      <c r="KE6" s="197"/>
+      <c r="KF6" s="197"/>
+      <c r="KG6" s="197"/>
+      <c r="KH6" s="197"/>
+      <c r="KI6" s="197"/>
+      <c r="KJ6" s="197"/>
+      <c r="KK6" s="197"/>
+      <c r="KL6" s="197"/>
+      <c r="KM6" s="197"/>
+      <c r="KN6" s="197"/>
+      <c r="KO6" s="197"/>
+      <c r="KP6" s="197"/>
+      <c r="KQ6" s="197"/>
+      <c r="KR6" s="197"/>
+      <c r="KS6" s="198"/>
+      <c r="KT6" s="201">
         <v>11</v>
       </c>
-      <c r="KU6" s="201"/>
-      <c r="KV6" s="201"/>
-      <c r="KW6" s="201"/>
-      <c r="KX6" s="201"/>
-      <c r="KY6" s="201"/>
-      <c r="KZ6" s="201"/>
-      <c r="LA6" s="201"/>
-      <c r="LB6" s="201"/>
-      <c r="LC6" s="201"/>
-      <c r="LD6" s="201"/>
-      <c r="LE6" s="201"/>
-      <c r="LF6" s="201"/>
-      <c r="LG6" s="201"/>
-      <c r="LH6" s="201"/>
-      <c r="LI6" s="201"/>
-      <c r="LJ6" s="201"/>
-      <c r="LK6" s="201"/>
-      <c r="LL6" s="201"/>
-      <c r="LM6" s="201"/>
-      <c r="LN6" s="201"/>
-      <c r="LO6" s="201"/>
-      <c r="LP6" s="201"/>
-      <c r="LQ6" s="201"/>
-      <c r="LR6" s="201"/>
-      <c r="LS6" s="201"/>
-      <c r="LT6" s="201"/>
-      <c r="LU6" s="201"/>
-      <c r="LV6" s="201"/>
-      <c r="LW6" s="202"/>
-      <c r="LX6" s="196">
+      <c r="KU6" s="202"/>
+      <c r="KV6" s="202"/>
+      <c r="KW6" s="202"/>
+      <c r="KX6" s="202"/>
+      <c r="KY6" s="202"/>
+      <c r="KZ6" s="202"/>
+      <c r="LA6" s="202"/>
+      <c r="LB6" s="202"/>
+      <c r="LC6" s="202"/>
+      <c r="LD6" s="202"/>
+      <c r="LE6" s="202"/>
+      <c r="LF6" s="202"/>
+      <c r="LG6" s="202"/>
+      <c r="LH6" s="202"/>
+      <c r="LI6" s="202"/>
+      <c r="LJ6" s="202"/>
+      <c r="LK6" s="202"/>
+      <c r="LL6" s="202"/>
+      <c r="LM6" s="202"/>
+      <c r="LN6" s="202"/>
+      <c r="LO6" s="202"/>
+      <c r="LP6" s="202"/>
+      <c r="LQ6" s="202"/>
+      <c r="LR6" s="202"/>
+      <c r="LS6" s="202"/>
+      <c r="LT6" s="202"/>
+      <c r="LU6" s="202"/>
+      <c r="LV6" s="202"/>
+      <c r="LW6" s="203"/>
+      <c r="LX6" s="197">
         <v>12</v>
       </c>
-      <c r="LY6" s="196"/>
-      <c r="LZ6" s="196"/>
-      <c r="MA6" s="196"/>
-      <c r="MB6" s="196"/>
-      <c r="MC6" s="196"/>
-      <c r="MD6" s="196"/>
-      <c r="ME6" s="196"/>
-      <c r="MF6" s="196"/>
-      <c r="MG6" s="196"/>
-      <c r="MH6" s="196"/>
-      <c r="MI6" s="196"/>
-      <c r="MJ6" s="196"/>
-      <c r="MK6" s="196"/>
-      <c r="ML6" s="196"/>
-      <c r="MM6" s="196"/>
-      <c r="MN6" s="196"/>
-      <c r="MO6" s="196"/>
-      <c r="MP6" s="196"/>
-      <c r="MQ6" s="196"/>
-      <c r="MR6" s="196"/>
-      <c r="MS6" s="196"/>
-      <c r="MT6" s="196"/>
-      <c r="MU6" s="196"/>
-      <c r="MV6" s="196"/>
-      <c r="MW6" s="196"/>
-      <c r="MX6" s="196"/>
-      <c r="MY6" s="196"/>
-      <c r="MZ6" s="196"/>
-      <c r="NA6" s="196"/>
-      <c r="NB6" s="197"/>
+      <c r="LY6" s="197"/>
+      <c r="LZ6" s="197"/>
+      <c r="MA6" s="197"/>
+      <c r="MB6" s="197"/>
+      <c r="MC6" s="197"/>
+      <c r="MD6" s="197"/>
+      <c r="ME6" s="197"/>
+      <c r="MF6" s="197"/>
+      <c r="MG6" s="197"/>
+      <c r="MH6" s="197"/>
+      <c r="MI6" s="197"/>
+      <c r="MJ6" s="197"/>
+      <c r="MK6" s="197"/>
+      <c r="ML6" s="197"/>
+      <c r="MM6" s="197"/>
+      <c r="MN6" s="197"/>
+      <c r="MO6" s="197"/>
+      <c r="MP6" s="197"/>
+      <c r="MQ6" s="197"/>
+      <c r="MR6" s="197"/>
+      <c r="MS6" s="197"/>
+      <c r="MT6" s="197"/>
+      <c r="MU6" s="197"/>
+      <c r="MV6" s="197"/>
+      <c r="MW6" s="197"/>
+      <c r="MX6" s="197"/>
+      <c r="MY6" s="197"/>
+      <c r="MZ6" s="197"/>
+      <c r="NA6" s="197"/>
+      <c r="NB6" s="198"/>
     </row>
     <row r="7" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -36900,7 +36905,7 @@
       </c>
     </row>
     <row r="8" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="203" t="s">
+      <c r="A8" s="204" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="34"/>
@@ -37292,7 +37297,7 @@
       <c r="NB8" s="141"/>
     </row>
     <row r="9" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="203"/>
+      <c r="A9" s="204"/>
       <c r="B9" s="29"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -37672,7 +37677,7 @@
       <c r="NB9" s="32"/>
     </row>
     <row r="10" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="203"/>
+      <c r="A10" s="204"/>
       <c r="B10" s="29"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
@@ -38054,7 +38059,7 @@
       <c r="NB10" s="32"/>
     </row>
     <row r="11" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="203"/>
+      <c r="A11" s="204"/>
       <c r="B11" s="29"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
@@ -38430,7 +38435,7 @@
       <c r="NB11" s="32"/>
     </row>
     <row r="12" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="203"/>
+      <c r="A12" s="204"/>
       <c r="B12" s="29"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
@@ -38804,7 +38809,7 @@
       <c r="NB12" s="32"/>
     </row>
     <row r="13" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="203"/>
+      <c r="A13" s="204"/>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -39174,7 +39179,7 @@
       <c r="NB13" s="32"/>
     </row>
     <row r="14" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="203"/>
+      <c r="A14" s="204"/>
       <c r="B14" s="50"/>
       <c r="C14" s="51"/>
       <c r="D14" s="51"/>
@@ -39544,7 +39549,7 @@
       <c r="NB14" s="65"/>
     </row>
     <row r="15" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="204" t="s">
+      <c r="A15" s="205" t="s">
         <v>62</v>
       </c>
       <c r="B15" s="75"/>
@@ -39924,7 +39929,7 @@
       <c r="NB15" s="84"/>
     </row>
     <row r="16" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="203"/>
+      <c r="A16" s="204"/>
       <c r="B16" s="24"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -40296,7 +40301,7 @@
       <c r="NB16" s="25"/>
     </row>
     <row r="17" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="203"/>
+      <c r="A17" s="204"/>
       <c r="B17" s="24"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -40664,7 +40669,7 @@
       <c r="NB17" s="25"/>
     </row>
     <row r="18" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="203"/>
+      <c r="A18" s="204"/>
       <c r="B18" s="24"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -41034,7 +41039,7 @@
       <c r="NB18" s="25"/>
     </row>
     <row r="19" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="203"/>
+      <c r="A19" s="204"/>
       <c r="B19" s="85"/>
       <c r="C19" s="71"/>
       <c r="D19" s="71"/>
@@ -41402,7 +41407,7 @@
       <c r="NB19" s="74"/>
     </row>
     <row r="20" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="203" t="s">
+      <c r="A20" s="204" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="42"/>
@@ -41786,7 +41791,7 @@
       <c r="NB20" s="84"/>
     </row>
     <row r="21" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="203"/>
+      <c r="A21" s="204"/>
       <c r="B21" s="24"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -42163,7 +42168,7 @@
       <c r="NB21" s="25"/>
     </row>
     <row r="22" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="203"/>
+      <c r="A22" s="204"/>
       <c r="B22" s="24"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -42543,7 +42548,7 @@
       <c r="NB22" s="25"/>
     </row>
     <row r="23" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="203"/>
+      <c r="A23" s="204"/>
       <c r="B23" s="24"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
@@ -42919,7 +42924,7 @@
       <c r="NB23" s="25"/>
     </row>
     <row r="24" spans="1:366" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="203"/>
+      <c r="A24" s="204"/>
       <c r="B24" s="26"/>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
@@ -43289,7 +43294,7 @@
       <c r="NB24" s="74"/>
     </row>
     <row r="25" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="203" t="s">
+      <c r="A25" s="204" t="s">
         <v>17</v>
       </c>
       <c r="B25" s="75"/>
@@ -43669,7 +43674,7 @@
       <c r="NB25" s="84"/>
     </row>
     <row r="26" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="203"/>
+      <c r="A26" s="204"/>
       <c r="B26" s="24"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -44045,7 +44050,7 @@
       <c r="NB26" s="25"/>
     </row>
     <row r="27" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="203"/>
+      <c r="A27" s="204"/>
       <c r="B27" s="24"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
@@ -44417,7 +44422,7 @@
       <c r="NB27" s="25"/>
     </row>
     <row r="28" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="203"/>
+      <c r="A28" s="204"/>
       <c r="B28" s="24"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -44790,7 +44795,7 @@
       <c r="NB28" s="25"/>
     </row>
     <row r="29" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="203"/>
+      <c r="A29" s="204"/>
       <c r="B29" s="91"/>
       <c r="C29" s="92"/>
       <c r="D29" s="92"/>
@@ -45160,7 +45165,7 @@
       <c r="NB29" s="74"/>
     </row>
     <row r="30" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="204" t="s">
+      <c r="A30" s="205" t="s">
         <v>63</v>
       </c>
       <c r="B30" s="75"/>
@@ -45532,7 +45537,7 @@
       <c r="NB30" s="84"/>
     </row>
     <row r="31" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="203"/>
+      <c r="A31" s="204"/>
       <c r="B31" s="24"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -45906,7 +45911,7 @@
       <c r="NB31" s="25"/>
     </row>
     <row r="32" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="203"/>
+      <c r="A32" s="204"/>
       <c r="B32" s="24"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
@@ -46280,7 +46285,7 @@
       <c r="NB32" s="25"/>
     </row>
     <row r="33" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="203"/>
+      <c r="A33" s="204"/>
       <c r="B33" s="24"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
@@ -46650,7 +46655,7 @@
       <c r="NB33" s="25"/>
     </row>
     <row r="34" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="203"/>
+      <c r="A34" s="204"/>
       <c r="B34" s="85"/>
       <c r="C34" s="71"/>
       <c r="D34" s="71"/>
@@ -47018,7 +47023,7 @@
       <c r="NB34" s="74"/>
     </row>
     <row r="35" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="203" t="s">
+      <c r="A35" s="204" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="42"/>
@@ -47400,7 +47405,7 @@
       <c r="NB35" s="47"/>
     </row>
     <row r="36" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="203"/>
+      <c r="A36" s="204"/>
       <c r="B36" s="24"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
@@ -47772,7 +47777,7 @@
       <c r="NB36" s="25"/>
     </row>
     <row r="37" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="203"/>
+      <c r="A37" s="204"/>
       <c r="B37" s="24"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -48148,7 +48153,7 @@
       <c r="NB37" s="25"/>
     </row>
     <row r="38" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="203"/>
+      <c r="A38" s="204"/>
       <c r="B38" s="24"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
@@ -48522,7 +48527,7 @@
       <c r="NB38" s="25"/>
     </row>
     <row r="39" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="203"/>
+      <c r="A39" s="204"/>
       <c r="B39" s="85"/>
       <c r="C39" s="71"/>
       <c r="D39" s="71"/>
@@ -48894,7 +48899,7 @@
       <c r="NB39" s="74"/>
     </row>
     <row r="40" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="203" t="s">
+      <c r="A40" s="204" t="s">
         <v>23</v>
       </c>
       <c r="B40" s="75"/>
@@ -49272,7 +49277,7 @@
       <c r="NB40" s="84"/>
     </row>
     <row r="41" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="203"/>
+      <c r="A41" s="204"/>
       <c r="B41" s="24"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
@@ -49648,7 +49653,7 @@
       <c r="NB41" s="25"/>
     </row>
     <row r="42" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="203"/>
+      <c r="A42" s="204"/>
       <c r="B42" s="24"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -50018,7 +50023,7 @@
       <c r="NB42" s="25"/>
     </row>
     <row r="43" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="203"/>
+      <c r="A43" s="204"/>
       <c r="B43" s="24"/>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
@@ -50388,7 +50393,7 @@
       <c r="NB43" s="25"/>
     </row>
     <row r="44" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="203"/>
+      <c r="A44" s="204"/>
       <c r="B44" s="85"/>
       <c r="C44" s="71"/>
       <c r="D44" s="71"/>
@@ -50756,7 +50761,7 @@
       <c r="NB44" s="74"/>
     </row>
     <row r="45" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="203" t="s">
+      <c r="A45" s="204" t="s">
         <v>22</v>
       </c>
       <c r="B45" s="75"/>
@@ -51136,7 +51141,7 @@
       <c r="NB45" s="84"/>
     </row>
     <row r="46" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="203"/>
+      <c r="A46" s="204"/>
       <c r="B46" s="24"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
@@ -51506,7 +51511,7 @@
       <c r="NB46" s="25"/>
     </row>
     <row r="47" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="203"/>
+      <c r="A47" s="204"/>
       <c r="B47" s="24"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
@@ -51882,7 +51887,7 @@
       <c r="NB47" s="25"/>
     </row>
     <row r="48" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="203"/>
+      <c r="A48" s="204"/>
       <c r="B48" s="24"/>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -52252,7 +52257,7 @@
       <c r="NB48" s="25"/>
     </row>
     <row r="49" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="203"/>
+      <c r="A49" s="204"/>
       <c r="B49" s="85"/>
       <c r="C49" s="71"/>
       <c r="D49" s="71"/>
@@ -52626,7 +52631,7 @@
       <c r="NB49" s="74"/>
     </row>
     <row r="50" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="203" t="s">
+      <c r="A50" s="204" t="s">
         <v>24</v>
       </c>
       <c r="B50" s="75"/>
@@ -53008,7 +53013,7 @@
       <c r="NB50" s="84"/>
     </row>
     <row r="51" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="203"/>
+      <c r="A51" s="204"/>
       <c r="B51" s="24"/>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
@@ -53386,7 +53391,7 @@
       <c r="NB51" s="25"/>
     </row>
     <row r="52" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="203"/>
+      <c r="A52" s="204"/>
       <c r="B52" s="24"/>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
@@ -53758,7 +53763,7 @@
       <c r="NB52" s="25"/>
     </row>
     <row r="53" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="203"/>
+      <c r="A53" s="204"/>
       <c r="B53" s="24"/>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
@@ -54128,7 +54133,7 @@
       <c r="NB53" s="25"/>
     </row>
     <row r="54" spans="1:366" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="203"/>
+      <c r="A54" s="204"/>
       <c r="B54" s="85"/>
       <c r="C54" s="71"/>
       <c r="D54" s="71"/>
@@ -54548,10 +54553,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F40"/>
+  <dimension ref="B1:G40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -54565,20 +54570,20 @@
   <sheetData>
     <row r="1" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="205" t="s">
+      <c r="B2" s="206" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="207" t="s">
+      <c r="C2" s="208" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="208"/>
-      <c r="E2" s="209" t="s">
+      <c r="D2" s="209"/>
+      <c r="E2" s="210" t="s">
         <v>127</v>
       </c>
-      <c r="F2" s="208"/>
+      <c r="F2" s="209"/>
     </row>
     <row r="3" spans="2:6" s="167" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="206"/>
+      <c r="B3" s="207"/>
       <c r="C3" s="174" t="s">
         <v>122</v>
       </c>
@@ -54610,7 +54615,7 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="210">
+      <c r="B5" s="211">
         <v>43219</v>
       </c>
       <c r="C5" s="183">
@@ -54627,7 +54632,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="212"/>
+      <c r="B6" s="213"/>
       <c r="C6" s="183"/>
       <c r="D6" s="184"/>
       <c r="E6" s="185">
@@ -54651,7 +54656,7 @@
       <c r="F7" s="184"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="210">
+      <c r="B8" s="211">
         <v>43221</v>
       </c>
       <c r="C8" s="190">
@@ -54668,7 +54673,7 @@
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="211"/>
+      <c r="B9" s="212"/>
       <c r="C9" s="190">
         <v>2</v>
       </c>
@@ -54679,7 +54684,7 @@
       <c r="F9" s="184"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="211"/>
+      <c r="B10" s="212"/>
       <c r="C10" s="190">
         <v>1</v>
       </c>
@@ -54690,7 +54695,7 @@
       <c r="F10" s="184"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="212"/>
+      <c r="B11" s="213"/>
       <c r="C11" s="190">
         <v>1</v>
       </c>
@@ -54777,7 +54782,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="187"/>
       <c r="C17" s="183"/>
       <c r="D17" s="184"/>
@@ -54788,105 +54793,116 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="187"/>
-      <c r="C18" s="183"/>
-      <c r="D18" s="184"/>
-      <c r="E18" s="185"/>
-      <c r="F18" s="184"/>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="187">
+        <v>43228</v>
+      </c>
+      <c r="C18" s="183">
+        <v>1</v>
+      </c>
+      <c r="D18" s="184" t="s">
+        <v>153</v>
+      </c>
+      <c r="E18" s="185">
+        <v>4</v>
+      </c>
+      <c r="F18" s="184" t="s">
+        <v>151</v>
+      </c>
+      <c r="G18" s="192"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="187"/>
       <c r="C19" s="183"/>
       <c r="D19" s="184"/>
       <c r="E19" s="185"/>
       <c r="F19" s="184"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="187"/>
       <c r="C20" s="183"/>
       <c r="D20" s="184"/>
       <c r="E20" s="185"/>
       <c r="F20" s="184"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="187"/>
       <c r="C21" s="183"/>
       <c r="D21" s="184"/>
       <c r="E21" s="185"/>
       <c r="F21" s="184"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="187"/>
       <c r="C22" s="183"/>
       <c r="D22" s="184"/>
       <c r="E22" s="185"/>
       <c r="F22" s="184"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="187"/>
       <c r="C23" s="183"/>
       <c r="D23" s="184"/>
       <c r="E23" s="185"/>
       <c r="F23" s="184"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="187"/>
       <c r="C24" s="183"/>
       <c r="D24" s="184"/>
       <c r="E24" s="185"/>
       <c r="F24" s="184"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="187"/>
       <c r="C25" s="183"/>
       <c r="D25" s="184"/>
       <c r="E25" s="185"/>
       <c r="F25" s="184"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="187"/>
       <c r="C26" s="183"/>
       <c r="D26" s="184"/>
       <c r="E26" s="185"/>
       <c r="F26" s="184"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="187"/>
       <c r="C27" s="183"/>
       <c r="D27" s="184"/>
       <c r="E27" s="185"/>
       <c r="F27" s="184"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" s="187"/>
       <c r="C28" s="183"/>
       <c r="D28" s="184"/>
       <c r="E28" s="185"/>
       <c r="F28" s="184"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B29" s="187"/>
       <c r="C29" s="183"/>
       <c r="D29" s="184"/>
       <c r="E29" s="185"/>
       <c r="F29" s="184"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" s="187"/>
       <c r="C30" s="183"/>
       <c r="D30" s="184"/>
       <c r="E30" s="185"/>
       <c r="F30" s="184"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31" s="187"/>
       <c r="C31" s="175"/>
       <c r="D31" s="169"/>
       <c r="E31" s="177"/>
       <c r="F31" s="169"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B32" s="187"/>
       <c r="C32" s="175"/>
       <c r="D32" s="169"/>

</xml_diff>

<commit_message>
[DOC] Schedule 및 Cost update
</commit_message>
<xml_diff>
--- a/Femto Project schedule V1.0.xlsx
+++ b/Femto Project schedule V1.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="20180207" sheetId="18" r:id="rId1"/>
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="156">
   <si>
     <t>◇PCB설계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -796,11 +796,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Pipette Proto-type F/W 환경 설정
-Source 분석 - Frequency / Battery Temp 조정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>◇ Transformer PCB 2D,BOM,datasheet 전달</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -900,6 +895,19 @@
   </si>
   <si>
     <t>LF Gen Main Simulation - Tr current</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pipette V1.0 Main PCB 제작 - 6ea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pipette Proto-type F/W 환경 설정
+Source 분석 - Frequency / Battery Temp 조정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pipette Proto-type 수리 : 2ea, 1ea 불량처리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -35343,11 +35351,6 @@
     <row r="71" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="GA6:HE6"/>
-    <mergeCell ref="HF6:IJ6"/>
-    <mergeCell ref="IK6:JN6"/>
-    <mergeCell ref="JO6:KS6"/>
-    <mergeCell ref="KT6:LW6"/>
     <mergeCell ref="LX6:NB6"/>
     <mergeCell ref="A50:A54"/>
     <mergeCell ref="A15:A19"/>
@@ -35364,6 +35367,11 @@
     <mergeCell ref="BI6:CM6"/>
     <mergeCell ref="CN6:DQ6"/>
     <mergeCell ref="DR6:EV6"/>
+    <mergeCell ref="GA6:HE6"/>
+    <mergeCell ref="HF6:IJ6"/>
+    <mergeCell ref="IK6:JN6"/>
+    <mergeCell ref="JO6:KS6"/>
+    <mergeCell ref="KT6:LW6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35377,9 +35385,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:NB71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CP1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="EI41" sqref="EI41"/>
+      <selection pane="topRight" activeCell="DZ29" sqref="DZ29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -37807,7 +37815,7 @@
       <c r="DL10" s="30"/>
       <c r="DM10" s="30"/>
       <c r="DN10" s="30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="DO10" s="31"/>
       <c r="DP10" s="31"/>
@@ -39671,7 +39679,7 @@
       <c r="DN15" s="76"/>
       <c r="DO15" s="77"/>
       <c r="DP15" s="80" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="DQ15" s="84"/>
       <c r="DR15" s="82"/>
@@ -40051,7 +40059,7 @@
       <c r="DP16" s="14"/>
       <c r="DQ16" s="25"/>
       <c r="DR16" s="189" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="DS16" s="16"/>
       <c r="DT16" s="16"/>
@@ -40793,7 +40801,7 @@
       <c r="DR18" s="67"/>
       <c r="DS18" s="16"/>
       <c r="DT18" s="56" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="DU18" s="16"/>
       <c r="DV18" s="14"/>
@@ -42303,7 +42311,7 @@
       <c r="DU22" s="16"/>
       <c r="DV22" s="14"/>
       <c r="DW22" s="56" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="DX22" s="14"/>
       <c r="DY22" s="16"/>
@@ -42682,7 +42690,7 @@
       <c r="DZ23" s="16"/>
       <c r="EA23" s="16"/>
       <c r="EB23" s="59" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="EC23" s="59"/>
       <c r="ED23" s="59"/>
@@ -44550,7 +44558,7 @@
       <c r="DR28" s="23"/>
       <c r="DS28" s="13"/>
       <c r="DT28" s="90" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="DU28" s="13"/>
       <c r="DV28" s="14"/>
@@ -44922,7 +44930,7 @@
       <c r="DU29" s="71"/>
       <c r="DV29" s="72"/>
       <c r="DW29" s="191" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="DX29" s="72"/>
       <c r="DY29" s="71"/>
@@ -54521,6 +54529,15 @@
     <row r="71" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="A35:A39"/>
     <mergeCell ref="LX6:NB6"/>
     <mergeCell ref="B6:AF6"/>
     <mergeCell ref="AG6:BH6"/>
@@ -54533,15 +54550,6 @@
     <mergeCell ref="IK6:JN6"/>
     <mergeCell ref="JO6:KS6"/>
     <mergeCell ref="KT6:LW6"/>
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="A45:A49"/>
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A30:A34"/>
-    <mergeCell ref="A35:A39"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -54555,8 +54563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -54605,7 +54613,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="180" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="E4" s="181">
         <v>1</v>
@@ -54622,13 +54630,13 @@
         <v>2</v>
       </c>
       <c r="D5" s="184" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E5" s="185">
         <v>2</v>
       </c>
       <c r="F5" s="188" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
@@ -54639,7 +54647,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="188" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
@@ -54650,7 +54658,7 @@
         <v>3.5</v>
       </c>
       <c r="D7" s="188" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E7" s="185"/>
       <c r="F7" s="184"/>
@@ -54663,13 +54671,13 @@
         <v>2</v>
       </c>
       <c r="D8" s="188" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E8" s="185">
         <v>4</v>
       </c>
       <c r="F8" s="184" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
@@ -54678,7 +54686,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="188" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E9" s="185"/>
       <c r="F9" s="184"/>
@@ -54689,7 +54697,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="188" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E10" s="185"/>
       <c r="F10" s="184"/>
@@ -54700,7 +54708,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="188" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E11" s="185"/>
       <c r="F11" s="184"/>
@@ -54713,13 +54721,13 @@
         <v>1</v>
       </c>
       <c r="D12" s="184" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E12" s="185">
         <v>4</v>
       </c>
       <c r="F12" s="184" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
@@ -54728,13 +54736,13 @@
         <v>0.5</v>
       </c>
       <c r="D13" s="184" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E13" s="185">
         <v>4</v>
       </c>
       <c r="F13" s="188" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
@@ -54745,13 +54753,13 @@
         <v>0.5</v>
       </c>
       <c r="D14" s="184" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E14" s="185">
         <v>8</v>
       </c>
       <c r="F14" s="188" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
@@ -54762,13 +54770,13 @@
         <v>1</v>
       </c>
       <c r="D15" s="184" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E15" s="185">
         <v>3</v>
       </c>
       <c r="F15" s="184" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
@@ -54779,7 +54787,7 @@
         <v>4</v>
       </c>
       <c r="F16" s="188" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
@@ -54790,7 +54798,7 @@
         <v>3</v>
       </c>
       <c r="F17" s="184" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
@@ -54801,13 +54809,13 @@
         <v>1</v>
       </c>
       <c r="D18" s="184" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E18" s="185">
         <v>4</v>
       </c>
       <c r="F18" s="184" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G18" s="192"/>
     </row>
@@ -54817,22 +54825,42 @@
       </c>
       <c r="C19" s="183"/>
       <c r="D19" s="184"/>
-      <c r="E19" s="185"/>
-      <c r="F19" s="184"/>
+      <c r="E19" s="185">
+        <v>4</v>
+      </c>
+      <c r="F19" s="184" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="187"/>
+      <c r="B20" s="187">
+        <v>43230</v>
+      </c>
       <c r="C20" s="183"/>
       <c r="D20" s="184"/>
-      <c r="E20" s="185"/>
-      <c r="F20" s="184"/>
+      <c r="E20" s="185">
+        <v>10</v>
+      </c>
+      <c r="F20" s="184" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="187"/>
-      <c r="C21" s="183"/>
-      <c r="D21" s="184"/>
-      <c r="E21" s="185"/>
-      <c r="F21" s="184"/>
+      <c r="B21" s="187">
+        <v>43232</v>
+      </c>
+      <c r="C21" s="183">
+        <v>8</v>
+      </c>
+      <c r="D21" s="184" t="s">
+        <v>155</v>
+      </c>
+      <c r="E21" s="185">
+        <v>1</v>
+      </c>
+      <c r="F21" s="184" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="187"/>

</xml_diff>